<commit_message>
Fixed Error for "taking inventory" advancement, category was not updated
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BF9042-E5EA-4BC9-96BC-7B7C69FCD78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52132B5-552D-49CF-910D-D6FF3CEEEA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="647">
   <si>
     <t>In-game description</t>
   </si>
@@ -1964,6 +1964,9 @@
   </si>
   <si>
     <t>advHusbandry1</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -2082,7 +2085,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -2246,44 +2263,47 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11298E10-21DD-4EBF-8BF9-EA571BEEC72E}" name="Table1" displayName="Table1" ref="A2:J127" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A2:J127" xr:uid="{11298E10-21DD-4EBF-8BF9-EA571BEEC72E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11298E10-21DD-4EBF-8BF9-EA571BEEC72E}" name="Table1" displayName="Table1" ref="A2:K127" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A2:K127" xr:uid="{11298E10-21DD-4EBF-8BF9-EA571BEEC72E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J127">
     <sortCondition ref="J2:J127"/>
   </sortState>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{324771F9-822A-49B7-893D-1DA308D60F66}" name="Achievment" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{B22A3C33-D5FF-489D-81A0-0CD56EF167F6}" name="In-game description" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{3735BB57-B1D2-421D-9276-41B28AD37626}" name="Actual requirements (if different)" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{36B12DC4-1FAB-47F0-B495-DEEF3597AFFC}" name="Category" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{8DA34B88-F916-4B29-AA18-6228488B3C65}" name="Property Name" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{132DC9C0-CA6E-4B12-886A-9AB9F8BB67DB}" name="Index" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{ED2AFE63-C022-4969-A969-B12DDDC6F848}" name="Achievement (English Title)" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{103D45FE-68CE-4A58-85CD-B46098F4A479}" name="Implement" dataDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{DD3BED5F-4D31-44CA-9FF0-2CAF2DF70419}" name="Player.json" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{F9AD4A86-89AB-4252-BDC8-8698B593B077}" name="Sort Order" dataDxfId="12"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{324771F9-822A-49B7-893D-1DA308D60F66}" name="Achievment" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{B22A3C33-D5FF-489D-81A0-0CD56EF167F6}" name="In-game description" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{3735BB57-B1D2-421D-9276-41B28AD37626}" name="Actual requirements (if different)" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{36B12DC4-1FAB-47F0-B495-DEEF3597AFFC}" name="Category" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{8DA34B88-F916-4B29-AA18-6228488B3C65}" name="Property Name" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{132DC9C0-CA6E-4B12-886A-9AB9F8BB67DB}" name="Index" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{ED2AFE63-C022-4969-A969-B12DDDC6F848}" name="Achievement (English Title)" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{103D45FE-68CE-4A58-85CD-B46098F4A479}" name="Implement" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{DD3BED5F-4D31-44CA-9FF0-2CAF2DF70419}" name="Player.json" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{F9AD4A86-89AB-4252-BDC8-8698B593B077}" name="Sort Order" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{B93282D8-DE87-43DF-B868-238430288F85}" name="Column1" dataDxfId="1">
+      <calculatedColumnFormula>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54FDD79E-9496-444E-BAAB-2BDD7213F39D}" name="Table2" displayName="Table2" ref="A2:J112" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54FDD79E-9496-444E-BAAB-2BDD7213F39D}" name="Table2" displayName="Table2" ref="A2:J112" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A2:J112" xr:uid="{54FDD79E-9496-444E-BAAB-2BDD7213F39D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J112">
     <sortCondition ref="J2:J112"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{28B57E88-78E1-4471-B423-47178E900D39}" name="Advancement" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{3330A286-8064-4F71-8D6D-082AF5351B16}" name="In-game description" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{C6C9DE83-41CB-42D6-BAFA-5804D4D2C45F}" name="Actual requirements (if different)" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{FF11131C-C5A2-4438-95D7-DCC625EAB401}" name="Category" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{82ED0A77-34F2-4BBE-A373-52F72CBA1F8D}" name="Property Name" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{DB75B182-1053-43D2-9CB9-47C7FFF3DEDE}" name="Index" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{81839B7A-887C-4908-8072-601F3ED76542}" name="Advancement (English Title)" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{F3DF0BA5-07D9-46DE-951B-CD21F3246411}" name="Implement" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{6BAF4263-77BF-4F45-A828-572E4E40D09A}" name="Player.json" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{27AB76C4-3016-4553-A87A-9C1F759A0798}" name="Sort Order" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{28B57E88-78E1-4471-B423-47178E900D39}" name="Advancement" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{3330A286-8064-4F71-8D6D-082AF5351B16}" name="In-game description" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{C6C9DE83-41CB-42D6-BAFA-5804D4D2C45F}" name="Actual requirements (if different)" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{FF11131C-C5A2-4438-95D7-DCC625EAB401}" name="Category" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{82ED0A77-34F2-4BBE-A373-52F72CBA1F8D}" name="Property Name" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{DB75B182-1053-43D2-9CB9-47C7FFF3DEDE}" name="Index" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{81839B7A-887C-4908-8072-601F3ED76542}" name="Advancement (English Title)" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{F3DF0BA5-07D9-46DE-951B-CD21F3246411}" name="Implement" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{6BAF4263-77BF-4F45-A828-572E4E40D09A}" name="Player.json" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{27AB76C4-3016-4553-A87A-9C1F759A0798}" name="Sort Order" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2552,10 +2572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J127"/>
+  <dimension ref="A1:K127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C91" workbookViewId="0">
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2572,7 +2592,7 @@
     <col min="11" max="16384" width="50.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>632</v>
       </c>
@@ -2588,7 +2608,7 @@
       <c r="I1" s="10"/>
       <c r="J1" s="8"/>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>631</v>
       </c>
@@ -2619,8 +2639,11 @@
       <c r="J2" s="5" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="2" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>249</v>
       </c>
@@ -2651,8 +2674,12 @@
       <c r="J3" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>102</v>
       </c>
@@ -2683,8 +2710,12 @@
       <c r="J4" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K4" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -2715,8 +2746,12 @@
       <c r="J5" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K5" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>288</v>
       </c>
@@ -2747,8 +2782,12 @@
       <c r="J6" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>109</v>
       </c>
@@ -2779,8 +2818,12 @@
       <c r="J7" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -2811,8 +2854,12 @@
       <c r="J8" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>285</v>
       </c>
@@ -2843,8 +2890,12 @@
       <c r="J9" s="7">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -2875,8 +2926,12 @@
       <c r="J10" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>278</v>
       </c>
@@ -2907,8 +2962,12 @@
       <c r="J11" s="7">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>99</v>
       </c>
@@ -2939,8 +2998,12 @@
       <c r="J12" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
@@ -2971,8 +3034,12 @@
       <c r="J13" s="7">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K13" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>170</v>
       </c>
@@ -3003,8 +3070,12 @@
       <c r="J14" s="7">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>291</v>
       </c>
@@ -3035,8 +3106,12 @@
       <c r="J15" s="7">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K15" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>164</v>
       </c>
@@ -3067,8 +3142,12 @@
       <c r="J16" s="7">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>59</v>
       </c>
@@ -3099,8 +3178,12 @@
       <c r="J17" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K17" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>313</v>
       </c>
@@ -3131,8 +3214,12 @@
       <c r="J18" s="7">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K18" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>228</v>
       </c>
@@ -3163,8 +3250,12 @@
       <c r="J19" s="7">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>68</v>
       </c>
@@ -3195,8 +3286,12 @@
       <c r="J20" s="7">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>125</v>
       </c>
@@ -3227,8 +3322,12 @@
       <c r="J21" s="7">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Nether11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>209</v>
       </c>
@@ -3259,8 +3358,12 @@
       <c r="J22" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Nether12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>122</v>
       </c>
@@ -3291,8 +3394,12 @@
       <c r="J23" s="7">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K23" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Nether13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>149</v>
       </c>
@@ -3323,8 +3430,12 @@
       <c r="J24" s="7">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K24" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Nether14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>268</v>
       </c>
@@ -3355,8 +3466,12 @@
       <c r="J25" s="7">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>The_End11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>265</v>
       </c>
@@ -3387,8 +3502,12 @@
       <c r="J26" s="7">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K26" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>The_End12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>83</v>
       </c>
@@ -3419,8 +3538,12 @@
       <c r="J27" s="7">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K27" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>180</v>
       </c>
@@ -3451,8 +3574,12 @@
       <c r="J28" s="7">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K28" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>144</v>
       </c>
@@ -3483,8 +3610,12 @@
       <c r="J29" s="7">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K29" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -3515,8 +3646,12 @@
       <c r="J30" s="7">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K30" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>257</v>
       </c>
@@ -3547,8 +3682,12 @@
       <c r="J31" s="7">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K31" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Nether15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>260</v>
       </c>
@@ -3579,8 +3718,12 @@
       <c r="J32" s="7">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K32" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Nether16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>254</v>
       </c>
@@ -3611,8 +3754,12 @@
       <c r="J33" s="7">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Nether17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>206</v>
       </c>
@@ -3643,8 +3790,12 @@
       <c r="J34" s="7">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K34" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
@@ -3675,8 +3826,12 @@
       <c r="J35" s="7">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>183</v>
       </c>
@@ -3707,8 +3862,12 @@
       <c r="J36" s="7">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K36" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>161</v>
       </c>
@@ -3739,8 +3898,12 @@
       <c r="J37" s="7">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>73</v>
       </c>
@@ -3771,8 +3934,12 @@
       <c r="J38" s="7">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K38" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>139</v>
       </c>
@@ -3803,8 +3970,12 @@
       <c r="J39" s="7">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>194</v>
       </c>
@@ -3835,8 +4006,12 @@
       <c r="J40" s="7">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K40" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>186</v>
       </c>
@@ -3867,8 +4042,12 @@
       <c r="J41" s="7">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K41" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>273</v>
       </c>
@@ -3899,8 +4078,12 @@
       <c r="J42" s="7">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>196</v>
       </c>
@@ -3931,8 +4114,12 @@
       <c r="J43" s="7">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>135</v>
       </c>
@@ -3963,8 +4150,12 @@
       <c r="J44" s="7">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K44" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>128</v>
       </c>
@@ -3995,8 +4186,12 @@
       <c r="J45" s="7">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>107</v>
       </c>
@@ -4027,8 +4222,12 @@
       <c r="J46" s="7">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K46" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry19</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>200</v>
       </c>
@@ -4059,8 +4258,12 @@
       <c r="J47" s="7">
         <v>45</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>241</v>
       </c>
@@ -4091,8 +4294,12 @@
       <c r="J48" s="7">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K48" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -4123,8 +4330,12 @@
       <c r="J49" s="7">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K49" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story118</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>203</v>
       </c>
@@ -4155,8 +4366,12 @@
       <c r="J50" s="7">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>34</v>
       </c>
@@ -4187,8 +4402,12 @@
       <c r="J51" s="7">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>131</v>
       </c>
@@ -4219,8 +4438,12 @@
       <c r="J52" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K52" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>325</v>
       </c>
@@ -4251,8 +4474,12 @@
       <c r="J53" s="7">
         <v>51</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>147</v>
       </c>
@@ -4283,8 +4510,12 @@
       <c r="J54" s="7">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>14</v>
       </c>
@@ -4315,8 +4546,12 @@
       <c r="J55" s="7">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K55" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>281</v>
       </c>
@@ -4347,8 +4582,12 @@
       <c r="J56" s="7">
         <v>54</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>299</v>
       </c>
@@ -4379,8 +4618,12 @@
       <c r="J57" s="7">
         <v>55</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>41</v>
       </c>
@@ -4411,8 +4654,12 @@
       <c r="J58" s="7">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K58" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure113</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>152</v>
       </c>
@@ -4443,8 +4690,12 @@
       <c r="J59" s="7">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K59" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>94</v>
       </c>
@@ -4475,8 +4726,12 @@
       <c r="J60" s="7">
         <v>58</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K60" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>220</v>
       </c>
@@ -4507,8 +4762,12 @@
       <c r="J61" s="7">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K61" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story124</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>251</v>
       </c>
@@ -4539,8 +4798,12 @@
       <c r="J62" s="7">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K62" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure114</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>120</v>
       </c>
@@ -4571,8 +4834,12 @@
       <c r="J63" s="7">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K63" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>212</v>
       </c>
@@ -4603,8 +4870,12 @@
       <c r="J64" s="7">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K64" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>16</v>
       </c>
@@ -4635,8 +4906,12 @@
       <c r="J65" s="7">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K65" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry115</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>91</v>
       </c>
@@ -4667,8 +4942,12 @@
       <c r="J66" s="7">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K66" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure115</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>198</v>
       </c>
@@ -4699,8 +4978,12 @@
       <c r="J67" s="7">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K67" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>263</v>
       </c>
@@ -4731,8 +5014,12 @@
       <c r="J68" s="7">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K68" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>78</v>
       </c>
@@ -4763,8 +5050,12 @@
       <c r="J69" s="7">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K69" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>245</v>
       </c>
@@ -4795,8 +5086,12 @@
       <c r="J70" s="7">
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K70" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>322</v>
       </c>
@@ -4827,8 +5122,12 @@
       <c r="J71" s="7">
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K71" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>The_End13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>23</v>
       </c>
@@ -4859,8 +5158,12 @@
       <c r="J72" s="7">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K72" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Nether18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>271</v>
       </c>
@@ -4891,8 +5194,12 @@
       <c r="J73" s="7">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K73" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>The_End14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>105</v>
       </c>
@@ -4923,8 +5230,12 @@
       <c r="J74" s="7">
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K74" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>The_End15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>247</v>
       </c>
@@ -4955,8 +5266,12 @@
       <c r="J75" s="7">
         <v>73</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K75" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>The_End16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>301</v>
       </c>
@@ -4987,8 +5302,12 @@
       <c r="J76" s="7">
         <v>74</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K76" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure117</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>178</v>
       </c>
@@ -5019,8 +5338,12 @@
       <c r="J77" s="7">
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K77" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>The_End17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>50</v>
       </c>
@@ -5051,8 +5374,12 @@
       <c r="J78" s="7">
         <v>76</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K78" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>86</v>
       </c>
@@ -5083,8 +5410,12 @@
       <c r="J79" s="7">
         <v>77</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K79" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure119</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>142</v>
       </c>
@@ -5115,8 +5446,12 @@
       <c r="J80" s="7">
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K80" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure120</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>231</v>
       </c>
@@ -5147,8 +5482,12 @@
       <c r="J81" s="7">
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K81" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry117</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>18</v>
       </c>
@@ -5179,8 +5518,12 @@
       <c r="J82" s="7">
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K82" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure121</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>214</v>
       </c>
@@ -5211,8 +5554,12 @@
       <c r="J83" s="7">
         <v>81</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K83" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure122</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>45</v>
       </c>
@@ -5243,8 +5590,12 @@
       <c r="J84" s="7">
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K84" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure123</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>8</v>
       </c>
@@ -5275,8 +5626,12 @@
       <c r="J85" s="7">
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K85" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure124</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>115</v>
       </c>
@@ -5307,8 +5662,12 @@
       <c r="J86" s="7">
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K86" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry118</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>158</v>
       </c>
@@ -5339,8 +5698,12 @@
       <c r="J87" s="7">
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K87" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>217</v>
       </c>
@@ -5371,8 +5734,12 @@
       <c r="J88" s="7">
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K88" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure126</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>11</v>
       </c>
@@ -5403,8 +5770,12 @@
       <c r="J89" s="7">
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K89" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story128</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>75</v>
       </c>
@@ -5435,8 +5806,12 @@
       <c r="J90" s="7">
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K90" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>173</v>
       </c>
@@ -5467,8 +5842,12 @@
       <c r="J91" s="7">
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K91" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story129</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>80</v>
       </c>
@@ -5499,8 +5878,12 @@
       <c r="J92" s="7">
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K92" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure128</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>167</v>
       </c>
@@ -5531,8 +5914,12 @@
       <c r="J93" s="7">
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K93" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story130</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>294</v>
       </c>
@@ -5563,8 +5950,12 @@
       <c r="J94" s="7">
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K94" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story131</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>316</v>
       </c>
@@ -5595,8 +5986,12 @@
       <c r="J95" s="7">
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K95" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry119</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>328</v>
       </c>
@@ -5627,8 +6022,12 @@
       <c r="J96" s="7">
         <v>94</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K96" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry120</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
@@ -5659,8 +6058,12 @@
       <c r="J97" s="7">
         <v>95</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K97" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story132</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>191</v>
       </c>
@@ -5691,8 +6094,12 @@
       <c r="J98" s="7">
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K98" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry121</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>137</v>
       </c>
@@ -5723,8 +6130,12 @@
       <c r="J99" s="7">
         <v>97</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K99" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure129</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>38</v>
       </c>
@@ -5738,7 +6149,7 @@
         <v>621</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>622</v>
+        <v>629</v>
       </c>
       <c r="F100" s="6">
         <v>1</v>
@@ -5755,8 +6166,12 @@
       <c r="J100" s="7">
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K100" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story21</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>71</v>
       </c>
@@ -5787,8 +6202,12 @@
       <c r="J101" s="7">
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K101" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>307</v>
       </c>
@@ -5819,8 +6238,12 @@
       <c r="J102" s="7">
         <v>100</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K102" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure130</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>236</v>
       </c>
@@ -5851,8 +6274,12 @@
       <c r="J103" s="7">
         <v>101</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K103" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>118</v>
       </c>
@@ -5883,8 +6310,12 @@
       <c r="J104" s="7">
         <v>102</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K104" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure131</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>155</v>
       </c>
@@ -5915,8 +6346,12 @@
       <c r="J105" s="7">
         <v>103</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K105" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story24</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>283</v>
       </c>
@@ -5947,8 +6382,12 @@
       <c r="J106" s="7">
         <v>104</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K106" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story25</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>26</v>
       </c>
@@ -5979,8 +6418,12 @@
       <c r="J107" s="7">
         <v>105</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K107" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry122</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>297</v>
       </c>
@@ -6011,8 +6454,12 @@
       <c r="J108" s="7">
         <v>106</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K108" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry123</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>243</v>
       </c>
@@ -6043,8 +6490,12 @@
       <c r="J109" s="7">
         <v>107</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K109" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story26</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>36</v>
       </c>
@@ -6075,8 +6526,12 @@
       <c r="J110" s="7">
         <v>108</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K110" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story27</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>56</v>
       </c>
@@ -6107,8 +6562,12 @@
       <c r="J111" s="7">
         <v>109</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K111" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Nether19</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>175</v>
       </c>
@@ -6139,8 +6598,12 @@
       <c r="J112" s="7">
         <v>110</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K112" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Nether110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>112</v>
       </c>
@@ -6171,8 +6634,12 @@
       <c r="J113" s="7">
         <v>111</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K113" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Nether111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>310</v>
       </c>
@@ -6203,8 +6670,12 @@
       <c r="J114" s="7">
         <v>112</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K114" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Adventure132</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>304</v>
       </c>
@@ -6235,8 +6706,12 @@
       <c r="J115" s="7">
         <v>113</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K115" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story28</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>275</v>
       </c>
@@ -6267,8 +6742,12 @@
       <c r="J116" s="7">
         <v>114</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K116" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry124</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>48</v>
       </c>
@@ -6299,8 +6778,12 @@
       <c r="J117" s="7">
         <v>115</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K117" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story29</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>238</v>
       </c>
@@ -6331,8 +6814,12 @@
       <c r="J118" s="7">
         <v>116</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K118" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story210</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>233</v>
       </c>
@@ -6363,8 +6850,12 @@
       <c r="J119" s="7">
         <v>117</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K119" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story211</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>88</v>
       </c>
@@ -6395,8 +6886,12 @@
       <c r="J120" s="7">
         <v>118</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K120" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Nether112</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>133</v>
       </c>
@@ -6427,8 +6922,12 @@
       <c r="J121" s="7">
         <v>119</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K121" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story212</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>31</v>
       </c>
@@ -6459,8 +6958,12 @@
       <c r="J122" s="7">
         <v>120</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K122" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Husbandry125</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>319</v>
       </c>
@@ -6491,8 +6994,12 @@
       <c r="J123" s="7">
         <v>121</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K123" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Nether113</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>225</v>
       </c>
@@ -6523,8 +7030,12 @@
       <c r="J124" s="7">
         <v>122</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K124" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story213</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>189</v>
       </c>
@@ -6555,8 +7066,12 @@
       <c r="J125" s="7">
         <v>123</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K125" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story214</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>43</v>
       </c>
@@ -6587,8 +7102,12 @@
       <c r="J126" s="7">
         <v>124</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K126" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story215</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>223</v>
       </c>
@@ -6619,9 +7138,16 @@
       <c r="J127" s="7">
         <v>125</v>
       </c>
+      <c r="K127" s="1" t="str">
+        <f>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</f>
+        <v>Story216</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:I127" xr:uid="{D22F8CFF-0A6B-4322-864A-95539535B836}">
       <formula1>"true,false"</formula1>
@@ -6638,8 +7164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771D2FCF-03EA-4C2E-BCB7-15D3321DB186}">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87:E112"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
stated documenting the implemented field in excel
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30783D1-B89A-434B-AD97-39BC1D6BAEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9AD6F8-A57B-46E5-9162-B1E4E038D604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="1" r:id="rId1"/>
@@ -3121,8 +3121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K127"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3718,7 +3718,7 @@
         <v>79</v>
       </c>
       <c r="H17" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>19</v>
@@ -3826,7 +3826,7 @@
         <v>91</v>
       </c>
       <c r="H20" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>19</v>
@@ -3862,7 +3862,7 @@
         <v>97</v>
       </c>
       <c r="H21" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>19</v>
@@ -5662,7 +5662,7 @@
         <v>266</v>
       </c>
       <c r="H71" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I71" s="10" t="s">
         <v>19</v>
@@ -5734,7 +5734,7 @@
         <v>273</v>
       </c>
       <c r="H73" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I73" s="10" t="s">
         <v>19</v>
@@ -6202,7 +6202,7 @@
         <v>316</v>
       </c>
       <c r="H86" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I86" s="10" t="s">
         <v>19</v>
@@ -6562,7 +6562,7 @@
         <v>350</v>
       </c>
       <c r="H96" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I96" s="10" t="s">
         <v>19</v>
@@ -7066,7 +7066,7 @@
         <v>396</v>
       </c>
       <c r="H110" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I110" s="10" t="s">
         <v>19</v>
@@ -7102,7 +7102,7 @@
         <v>401</v>
       </c>
       <c r="H111" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I111" s="10" t="s">
         <v>19</v>
@@ -7711,7 +7711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed achievments and cataloged completed
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9AD6F8-A57B-46E5-9162-B1E4E038D604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4E3109-0AF0-4A2C-8AA0-FD10B05B26E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3121,8 +3121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G127" sqref="G127"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3934,7 +3934,7 @@
         <v>105</v>
       </c>
       <c r="H23" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>19</v>
@@ -4006,7 +4006,7 @@
         <v>115</v>
       </c>
       <c r="H25" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>19</v>
@@ -4042,7 +4042,7 @@
         <v>832</v>
       </c>
       <c r="H26" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>19</v>
@@ -4078,7 +4078,7 @@
         <v>119</v>
       </c>
       <c r="H27" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>19</v>
@@ -4150,7 +4150,7 @@
         <v>125</v>
       </c>
       <c r="H29" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>19</v>
@@ -4222,7 +4222,7 @@
         <v>135</v>
       </c>
       <c r="H31" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>19</v>
@@ -4330,7 +4330,7 @@
         <v>143</v>
       </c>
       <c r="H34" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>19</v>
@@ -4438,7 +4438,7 @@
         <v>156</v>
       </c>
       <c r="H37" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="10" t="s">
         <v>19</v>
@@ -4582,7 +4582,7 @@
         <v>170</v>
       </c>
       <c r="H41" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" s="10" t="s">
         <v>19</v>
@@ -4690,7 +4690,7 @@
         <v>179</v>
       </c>
       <c r="H44" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" s="10" t="s">
         <v>19</v>
@@ -4942,7 +4942,7 @@
         <v>204</v>
       </c>
       <c r="H51" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" s="10" t="s">
         <v>19</v>
@@ -4978,7 +4978,7 @@
         <v>207</v>
       </c>
       <c r="H52" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" s="10" t="s">
         <v>19</v>
@@ -5446,7 +5446,7 @@
         <v>246</v>
       </c>
       <c r="H65" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65" s="10" t="s">
         <v>19</v>
@@ -7606,7 +7606,7 @@
         <v>454</v>
       </c>
       <c r="H125" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I125" s="10" t="s">
         <v>19</v>
@@ -7711,8 +7711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7800,7 +7800,7 @@
         <v>463</v>
       </c>
       <c r="H3" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>19</v>
@@ -7832,7 +7832,7 @@
         <v>470</v>
       </c>
       <c r="H4" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>19</v>
@@ -7864,7 +7864,7 @@
         <v>57</v>
       </c>
       <c r="H5" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>19</v>
@@ -7896,7 +7896,7 @@
         <v>38</v>
       </c>
       <c r="H6" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>19</v>
@@ -7928,7 +7928,7 @@
         <v>478</v>
       </c>
       <c r="H7" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>19</v>
@@ -7960,7 +7960,7 @@
         <v>482</v>
       </c>
       <c r="H8" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>19</v>
@@ -7992,7 +7992,7 @@
         <v>486</v>
       </c>
       <c r="H9" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>19</v>
@@ -8056,7 +8056,7 @@
         <v>494</v>
       </c>
       <c r="H11" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>19</v>
@@ -8088,7 +8088,7 @@
         <v>498</v>
       </c>
       <c r="H12" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>19</v>
@@ -8120,7 +8120,7 @@
         <v>502</v>
       </c>
       <c r="H13" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>19</v>
@@ -8152,7 +8152,7 @@
         <v>506</v>
       </c>
       <c r="H14" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>19</v>
@@ -8280,7 +8280,7 @@
         <v>115</v>
       </c>
       <c r="H18" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>19</v>
@@ -8376,7 +8376,7 @@
         <v>523</v>
       </c>
       <c r="H21" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>19</v>
@@ -8408,7 +8408,7 @@
         <v>527</v>
       </c>
       <c r="H22" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>19</v>
@@ -8440,7 +8440,7 @@
         <v>531</v>
       </c>
       <c r="H23" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>19</v>
@@ -8472,7 +8472,7 @@
         <v>535</v>
       </c>
       <c r="H24" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>19</v>
@@ -8504,7 +8504,7 @@
         <v>539</v>
       </c>
       <c r="H25" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>19</v>
@@ -8600,7 +8600,7 @@
         <v>551</v>
       </c>
       <c r="H28" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>19</v>
@@ -8696,7 +8696,7 @@
         <v>562</v>
       </c>
       <c r="H31" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>19</v>
@@ -8760,7 +8760,7 @@
         <v>105</v>
       </c>
       <c r="H33" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>19</v>
@@ -8888,7 +8888,7 @@
         <v>581</v>
       </c>
       <c r="H37" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="10" t="s">
         <v>19</v>
@@ -8984,7 +8984,7 @@
         <v>591</v>
       </c>
       <c r="H40" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="10" t="s">
         <v>19</v>
@@ -9048,7 +9048,7 @@
         <v>598</v>
       </c>
       <c r="H42" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" s="10" t="s">
         <v>19</v>
@@ -9144,7 +9144,7 @@
         <v>608</v>
       </c>
       <c r="H45" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" s="10" t="s">
         <v>19</v>
@@ -9208,7 +9208,7 @@
         <v>273</v>
       </c>
       <c r="H47" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47" s="10" t="s">
         <v>19</v>
@@ -9237,10 +9237,10 @@
         <v>6</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="H48" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48" s="10" t="s">
         <v>19</v>
@@ -9304,7 +9304,7 @@
         <v>624</v>
       </c>
       <c r="H50" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" s="10" t="s">
         <v>19</v>
@@ -9624,7 +9624,7 @@
         <v>653</v>
       </c>
       <c r="H60" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60" s="10" t="s">
         <v>19</v>
@@ -9720,7 +9720,7 @@
         <v>662</v>
       </c>
       <c r="H63" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I63" s="10" t="s">
         <v>19</v>
@@ -9816,7 +9816,7 @@
         <v>672</v>
       </c>
       <c r="H66" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66" s="10" t="s">
         <v>19</v>
@@ -9880,7 +9880,7 @@
         <v>680</v>
       </c>
       <c r="H68" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68" s="10" t="s">
         <v>19</v>
@@ -9944,7 +9944,7 @@
         <v>688</v>
       </c>
       <c r="H70" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I70" s="10" t="s">
         <v>19</v>
@@ -10040,7 +10040,7 @@
         <v>699</v>
       </c>
       <c r="H73" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I73" s="10" t="s">
         <v>19</v>
@@ -10456,7 +10456,7 @@
         <v>396</v>
       </c>
       <c r="H86" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I86" s="10" t="s">
         <v>19</v>
@@ -10552,7 +10552,7 @@
         <v>749</v>
       </c>
       <c r="H89" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I89" s="10" t="s">
         <v>19</v>
@@ -10680,7 +10680,7 @@
         <v>764</v>
       </c>
       <c r="H93" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I93" s="10" t="s">
         <v>19</v>
@@ -10776,7 +10776,7 @@
         <v>772</v>
       </c>
       <c r="H96" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I96" s="10" t="s">
         <v>19</v>
@@ -10808,7 +10808,7 @@
         <v>776</v>
       </c>
       <c r="H97" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I97" s="10" t="s">
         <v>19</v>
@@ -10840,7 +10840,7 @@
         <v>780</v>
       </c>
       <c r="H98" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I98" s="10" t="s">
         <v>19</v>
@@ -11000,7 +11000,7 @@
         <v>800</v>
       </c>
       <c r="H103" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I103" s="10" t="s">
         <v>19</v>
@@ -11128,7 +11128,7 @@
         <v>816</v>
       </c>
       <c r="H107" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I107" s="10" t="s">
         <v>19</v>
@@ -11192,7 +11192,7 @@
         <v>824</v>
       </c>
       <c r="H109" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I109" s="10" t="s">
         <v>19</v>
@@ -11256,7 +11256,7 @@
         <v>830</v>
       </c>
       <c r="H111" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I111" s="10" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Added 4 eating achievements.
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E4A042-2DD8-4537-8103-52EAB362CE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8E98D6-83AE-42C7-974A-57C88E0C42E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3121,8 +3121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="M2" s="2">
         <f>COUNTIF(Table1[Implement],"=TRUE")</f>
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3232,7 +3232,7 @@
       </c>
       <c r="M3" s="2">
         <f>COUNTIF(Table1[Implement],"=FALSE")</f>
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -4410,7 +4410,7 @@
         <v>150</v>
       </c>
       <c r="H36" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" s="10" t="s">
         <v>19</v>
@@ -4554,7 +4554,7 @@
         <v>166</v>
       </c>
       <c r="H40" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="10" t="s">
         <v>19</v>
@@ -5526,7 +5526,7 @@
         <v>253</v>
       </c>
       <c r="H67" s="10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67" s="10" t="s">
         <v>19</v>
@@ -7854,7 +7854,7 @@
       </c>
       <c r="N4" s="1">
         <f>M4+Achievements!M2</f>
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -7894,7 +7894,7 @@
       </c>
       <c r="N5" s="1">
         <f>M5+Achievements!M3</f>
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed a few achievements, and the database packer, updated database
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8E98D6-83AE-42C7-974A-57C88E0C42E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A5626E-96EC-4592-B827-F1EBB8F1A25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1670" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1481" uniqueCount="834">
   <si>
     <t>Display Only Text</t>
   </si>
@@ -3121,8 +3121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="M2" s="2">
         <f>COUNTIF(Table1[Implement],"=TRUE")</f>
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -3232,7 +3232,7 @@
       </c>
       <c r="M3" s="2">
         <f>COUNTIF(Table1[Implement],"=FALSE")</f>
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -3620,8 +3620,8 @@
       <c r="H14" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>19</v>
+      <c r="I14" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J14" s="11">
         <v>12</v>
@@ -3690,10 +3690,10 @@
         <v>75</v>
       </c>
       <c r="H16" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="I16" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J16" s="11">
         <v>14</v>
@@ -3764,8 +3764,8 @@
       <c r="H18" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="10" t="s">
-        <v>19</v>
+      <c r="I18" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J18" s="11">
         <v>16</v>
@@ -3800,8 +3800,8 @@
       <c r="H19" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I19" s="10" t="s">
-        <v>19</v>
+      <c r="I19" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J19" s="11">
         <v>17</v>
@@ -3908,8 +3908,8 @@
       <c r="H22" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="10" t="s">
-        <v>19</v>
+      <c r="I22" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J22" s="11">
         <v>20</v>
@@ -3980,8 +3980,8 @@
       <c r="H24" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="10" t="s">
-        <v>19</v>
+      <c r="I24" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J24" s="11">
         <v>22</v>
@@ -4124,8 +4124,8 @@
       <c r="H28" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I28" s="10" t="s">
-        <v>19</v>
+      <c r="I28" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J28" s="11">
         <v>26</v>
@@ -4196,8 +4196,8 @@
       <c r="H30" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="10" t="s">
-        <v>19</v>
+      <c r="I30" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J30" s="11">
         <v>28</v>
@@ -4266,10 +4266,10 @@
         <v>833</v>
       </c>
       <c r="H32" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="I32" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J32" s="11">
         <v>30</v>
@@ -4304,8 +4304,8 @@
       <c r="H33" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I33" s="10" t="s">
-        <v>19</v>
+      <c r="I33" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J33" s="11">
         <v>31</v>
@@ -4376,8 +4376,8 @@
       <c r="H35" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I35" s="10" t="s">
-        <v>19</v>
+      <c r="I35" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J35" s="11">
         <v>33</v>
@@ -4484,8 +4484,8 @@
       <c r="H38" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="10" t="s">
-        <v>19</v>
+      <c r="I38" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J38" s="11">
         <v>36</v>
@@ -4520,8 +4520,8 @@
       <c r="H39" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="10" t="s">
-        <v>19</v>
+      <c r="I39" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J39" s="11">
         <v>37</v>
@@ -4628,8 +4628,8 @@
       <c r="H42" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I42" s="10" t="s">
-        <v>19</v>
+      <c r="I42" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J42" s="11">
         <v>40</v>
@@ -4664,8 +4664,8 @@
       <c r="H43" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I43" s="10" t="s">
-        <v>19</v>
+      <c r="I43" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J43" s="11">
         <v>41</v>
@@ -4736,8 +4736,8 @@
       <c r="H45" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I45" s="10" t="s">
-        <v>19</v>
+      <c r="I45" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J45" s="11">
         <v>43</v>
@@ -4772,8 +4772,8 @@
       <c r="H46" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I46" s="10" t="s">
-        <v>19</v>
+      <c r="I46" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J46" s="11">
         <v>44</v>
@@ -4844,8 +4844,8 @@
       <c r="H48" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I48" s="10" t="s">
-        <v>19</v>
+      <c r="I48" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J48" s="11">
         <v>46</v>
@@ -4880,8 +4880,8 @@
       <c r="H49" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I49" s="10" t="s">
-        <v>19</v>
+      <c r="I49" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J49" s="11">
         <v>47</v>
@@ -4916,8 +4916,8 @@
       <c r="H50" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I50" s="10" t="s">
-        <v>19</v>
+      <c r="I50" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J50" s="11">
         <v>48</v>
@@ -5060,8 +5060,8 @@
       <c r="H54" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I54" s="10" t="s">
-        <v>19</v>
+      <c r="I54" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J54" s="11">
         <v>52</v>
@@ -5132,8 +5132,8 @@
       <c r="H56" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I56" s="10" t="s">
-        <v>19</v>
+      <c r="I56" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J56" s="11">
         <v>54</v>
@@ -5168,8 +5168,8 @@
       <c r="H57" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I57" s="10" t="s">
-        <v>19</v>
+      <c r="I57" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J57" s="11">
         <v>55</v>
@@ -5204,8 +5204,8 @@
       <c r="H58" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I58" s="10" t="s">
-        <v>19</v>
+      <c r="I58" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J58" s="11">
         <v>56</v>
@@ -5240,8 +5240,8 @@
       <c r="H59" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I59" s="10" t="s">
-        <v>19</v>
+      <c r="I59" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J59" s="11">
         <v>57</v>
@@ -5276,8 +5276,8 @@
       <c r="H60" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I60" s="10" t="s">
-        <v>19</v>
+      <c r="I60" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J60" s="11">
         <v>58</v>
@@ -5312,8 +5312,8 @@
       <c r="H61" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I61" s="10" t="s">
-        <v>19</v>
+      <c r="I61" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J61" s="11">
         <v>59</v>
@@ -5348,8 +5348,8 @@
       <c r="H62" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I62" s="10" t="s">
-        <v>19</v>
+      <c r="I62" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J62" s="11">
         <v>60</v>
@@ -5384,8 +5384,8 @@
       <c r="H63" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I63" s="10" t="s">
-        <v>19</v>
+      <c r="I63" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J63" s="11">
         <v>61</v>
@@ -5420,8 +5420,8 @@
       <c r="H64" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I64" s="10" t="s">
-        <v>19</v>
+      <c r="I64" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J64" s="11">
         <v>62</v>
@@ -5492,8 +5492,8 @@
       <c r="H66" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I66" s="10" t="s">
-        <v>19</v>
+      <c r="I66" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J66" s="11">
         <v>64</v>
@@ -5600,8 +5600,8 @@
       <c r="H69" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I69" s="10" t="s">
-        <v>19</v>
+      <c r="I69" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J69" s="11">
         <v>67</v>
@@ -5636,8 +5636,8 @@
       <c r="H70" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I70" s="10" t="s">
-        <v>19</v>
+      <c r="I70" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J70" s="11">
         <v>68</v>
@@ -5708,8 +5708,8 @@
       <c r="H72" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I72" s="10" t="s">
-        <v>19</v>
+      <c r="I72" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J72" s="11">
         <v>70</v>
@@ -5780,8 +5780,8 @@
       <c r="H74" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I74" s="10" t="s">
-        <v>19</v>
+      <c r="I74" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J74" s="11">
         <v>72</v>
@@ -5816,8 +5816,8 @@
       <c r="H75" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I75" s="10" t="s">
-        <v>19</v>
+      <c r="I75" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J75" s="11">
         <v>73</v>
@@ -5852,8 +5852,8 @@
       <c r="H76" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I76" s="10" t="s">
-        <v>19</v>
+      <c r="I76" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J76" s="11">
         <v>74</v>
@@ -5924,8 +5924,8 @@
       <c r="H78" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I78" s="10" t="s">
-        <v>19</v>
+      <c r="I78" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J78" s="11">
         <v>76</v>
@@ -5996,8 +5996,8 @@
       <c r="H80" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I80" s="10" t="s">
-        <v>19</v>
+      <c r="I80" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J80" s="11">
         <v>78</v>
@@ -6032,8 +6032,8 @@
       <c r="H81" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I81" s="10" t="s">
-        <v>19</v>
+      <c r="I81" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J81" s="11">
         <v>79</v>
@@ -6068,8 +6068,8 @@
       <c r="H82" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I82" s="10" t="s">
-        <v>19</v>
+      <c r="I82" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J82" s="11">
         <v>80</v>
@@ -6104,8 +6104,8 @@
       <c r="H83" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I83" s="10" t="s">
-        <v>19</v>
+      <c r="I83" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J83" s="11">
         <v>81</v>
@@ -6140,8 +6140,8 @@
       <c r="H84" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I84" s="10" t="s">
-        <v>19</v>
+      <c r="I84" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J84" s="11">
         <v>82</v>
@@ -6176,8 +6176,8 @@
       <c r="H85" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I85" s="10" t="s">
-        <v>19</v>
+      <c r="I85" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J85" s="11">
         <v>83</v>
@@ -6248,8 +6248,8 @@
       <c r="H87" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I87" s="10" t="s">
-        <v>19</v>
+      <c r="I87" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J87" s="11">
         <v>85</v>
@@ -6284,8 +6284,8 @@
       <c r="H88" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I88" s="10" t="s">
-        <v>19</v>
+      <c r="I88" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J88" s="11">
         <v>86</v>
@@ -6320,8 +6320,8 @@
       <c r="H89" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I89" s="10" t="s">
-        <v>19</v>
+      <c r="I89" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J89" s="11">
         <v>87</v>
@@ -6356,8 +6356,8 @@
       <c r="H90" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I90" s="10" t="s">
-        <v>19</v>
+      <c r="I90" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J90" s="11">
         <v>88</v>
@@ -6392,8 +6392,8 @@
       <c r="H91" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I91" s="10" t="s">
-        <v>19</v>
+      <c r="I91" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J91" s="11">
         <v>89</v>
@@ -6428,8 +6428,8 @@
       <c r="H92" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I92" s="10" t="s">
-        <v>19</v>
+      <c r="I92" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J92" s="11">
         <v>90</v>
@@ -6462,10 +6462,10 @@
         <v>339</v>
       </c>
       <c r="H93" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I93" s="10" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="I93" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J93" s="11">
         <v>91</v>
@@ -6500,8 +6500,8 @@
       <c r="H94" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I94" s="10" t="s">
-        <v>19</v>
+      <c r="I94" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J94" s="11">
         <v>92</v>
@@ -6536,8 +6536,8 @@
       <c r="H95" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I95" s="10" t="s">
-        <v>19</v>
+      <c r="I95" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J95" s="11">
         <v>93</v>
@@ -6608,8 +6608,8 @@
       <c r="H97" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I97" s="10" t="s">
-        <v>19</v>
+      <c r="I97" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J97" s="11">
         <v>95</v>
@@ -6644,8 +6644,8 @@
       <c r="H98" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I98" s="10" t="s">
-        <v>19</v>
+      <c r="I98" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J98" s="11">
         <v>96</v>
@@ -6716,8 +6716,8 @@
       <c r="H100" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I100" s="10" t="s">
-        <v>19</v>
+      <c r="I100" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J100" s="11">
         <v>98</v>
@@ -6752,8 +6752,8 @@
       <c r="H101" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I101" s="10" t="s">
-        <v>19</v>
+      <c r="I101" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J101" s="11">
         <v>99</v>
@@ -6788,8 +6788,8 @@
       <c r="H102" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I102" s="10" t="s">
-        <v>19</v>
+      <c r="I102" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J102" s="11">
         <v>100</v>
@@ -6824,8 +6824,8 @@
       <c r="H103" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I103" s="10" t="s">
-        <v>19</v>
+      <c r="I103" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J103" s="11">
         <v>101</v>
@@ -6858,10 +6858,10 @@
         <v>379</v>
       </c>
       <c r="H104" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I104" s="10" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="I104" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J104" s="11">
         <v>102</v>
@@ -6896,8 +6896,8 @@
       <c r="H105" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I105" s="10" t="s">
-        <v>19</v>
+      <c r="I105" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J105" s="11">
         <v>103</v>
@@ -6932,8 +6932,8 @@
       <c r="H106" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I106" s="10" t="s">
-        <v>19</v>
+      <c r="I106" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J106" s="11">
         <v>104</v>
@@ -6968,8 +6968,8 @@
       <c r="H107" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I107" s="10" t="s">
-        <v>19</v>
+      <c r="I107" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J107" s="11">
         <v>105</v>
@@ -7004,8 +7004,8 @@
       <c r="H108" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I108" s="10" t="s">
-        <v>19</v>
+      <c r="I108" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J108" s="11">
         <v>106</v>
@@ -7040,8 +7040,8 @@
       <c r="H109" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I109" s="10" t="s">
-        <v>19</v>
+      <c r="I109" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J109" s="11">
         <v>107</v>
@@ -7148,8 +7148,8 @@
       <c r="H112" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I112" s="10" t="s">
-        <v>19</v>
+      <c r="I112" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J112" s="11">
         <v>110</v>
@@ -7184,8 +7184,8 @@
       <c r="H113" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I113" s="10" t="s">
-        <v>19</v>
+      <c r="I113" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J113" s="11">
         <v>111</v>
@@ -7220,8 +7220,8 @@
       <c r="H114" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I114" s="10" t="s">
-        <v>19</v>
+      <c r="I114" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J114" s="11">
         <v>112</v>
@@ -7256,8 +7256,8 @@
       <c r="H115" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I115" s="10" t="s">
-        <v>19</v>
+      <c r="I115" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J115" s="11">
         <v>113</v>
@@ -7292,8 +7292,8 @@
       <c r="H116" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I116" s="10" t="s">
-        <v>19</v>
+      <c r="I116" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J116" s="11">
         <v>114</v>
@@ -7328,8 +7328,8 @@
       <c r="H117" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I117" s="10" t="s">
-        <v>19</v>
+      <c r="I117" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J117" s="11">
         <v>115</v>
@@ -7364,8 +7364,8 @@
       <c r="H118" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I118" s="10" t="s">
-        <v>19</v>
+      <c r="I118" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J118" s="11">
         <v>116</v>
@@ -7400,8 +7400,8 @@
       <c r="H119" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I119" s="10" t="s">
-        <v>19</v>
+      <c r="I119" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J119" s="11">
         <v>117</v>
@@ -7436,8 +7436,8 @@
       <c r="H120" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I120" s="10" t="s">
-        <v>19</v>
+      <c r="I120" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J120" s="11">
         <v>118</v>
@@ -7472,8 +7472,8 @@
       <c r="H121" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I121" s="10" t="s">
-        <v>19</v>
+      <c r="I121" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J121" s="11">
         <v>119</v>
@@ -7508,8 +7508,8 @@
       <c r="H122" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I122" s="10" t="s">
-        <v>19</v>
+      <c r="I122" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J122" s="11">
         <v>120</v>
@@ -7580,8 +7580,8 @@
       <c r="H124" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I124" s="10" t="s">
-        <v>19</v>
+      <c r="I124" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J124" s="11">
         <v>122</v>
@@ -7652,8 +7652,8 @@
       <c r="H126" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I126" s="10" t="s">
-        <v>19</v>
+      <c r="I126" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J126" s="11">
         <v>124</v>
@@ -7688,8 +7688,8 @@
       <c r="H127" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I127" s="10" t="s">
-        <v>19</v>
+      <c r="I127" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J127" s="11">
         <v>125</v>
@@ -7719,8 +7719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N112"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7810,8 +7810,8 @@
       <c r="H3" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>19</v>
+      <c r="I3" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J3" s="11">
         <v>1</v>
@@ -7842,19 +7842,19 @@
       <c r="H4" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>19</v>
+      <c r="I4" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J4" s="11">
         <v>2</v>
       </c>
       <c r="M4" s="2">
         <f>COUNTIF(Table2[Implement],"=TRUE")</f>
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N4" s="1">
         <f>M4+Achievements!M2</f>
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -7882,19 +7882,19 @@
       <c r="H5" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I5" s="10" t="s">
-        <v>19</v>
+      <c r="I5" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J5" s="11">
         <v>3</v>
       </c>
       <c r="M5" s="2">
         <f>COUNTIF(Table2[Implement],"=FALSE")</f>
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="N5" s="1">
         <f>M5+Achievements!M3</f>
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -7922,8 +7922,8 @@
       <c r="H6" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I6" s="10" t="s">
-        <v>19</v>
+      <c r="I6" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J6" s="11">
         <v>4</v>
@@ -7958,8 +7958,8 @@
       <c r="H7" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I7" s="10" t="s">
-        <v>19</v>
+      <c r="I7" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J7" s="11">
         <v>5</v>
@@ -7990,8 +7990,8 @@
       <c r="H8" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>19</v>
+      <c r="I8" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J8" s="11">
         <v>6</v>
@@ -8022,8 +8022,8 @@
       <c r="H9" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I9" s="10" t="s">
-        <v>19</v>
+      <c r="I9" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J9" s="11">
         <v>7</v>
@@ -8054,8 +8054,8 @@
       <c r="H10" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I10" s="10" t="s">
-        <v>19</v>
+      <c r="I10" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J10" s="11">
         <v>8</v>
@@ -8086,8 +8086,8 @@
       <c r="H11" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>19</v>
+      <c r="I11" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J11" s="11">
         <v>9</v>
@@ -8118,8 +8118,8 @@
       <c r="H12" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>19</v>
+      <c r="I12" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J12" s="11">
         <v>10</v>
@@ -8150,8 +8150,8 @@
       <c r="H13" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I13" s="10" t="s">
-        <v>19</v>
+      <c r="I13" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J13" s="11">
         <v>11</v>
@@ -8182,8 +8182,8 @@
       <c r="H14" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>19</v>
+      <c r="I14" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J14" s="11">
         <v>12</v>
@@ -8214,8 +8214,8 @@
       <c r="H15" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="10" t="s">
-        <v>19</v>
+      <c r="I15" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J15" s="11">
         <v>13</v>
@@ -8244,10 +8244,10 @@
         <v>211</v>
       </c>
       <c r="H16" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="I16" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J16" s="11">
         <v>14</v>
@@ -8278,8 +8278,8 @@
       <c r="H17" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="10" t="s">
-        <v>19</v>
+      <c r="I17" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J17" s="11">
         <v>15</v>
@@ -8310,8 +8310,8 @@
       <c r="H18" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I18" s="10" t="s">
-        <v>19</v>
+      <c r="I18" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J18" s="11">
         <v>16</v>
@@ -8340,10 +8340,10 @@
         <v>95</v>
       </c>
       <c r="H19" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="I19" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J19" s="11">
         <v>17</v>
@@ -8374,8 +8374,8 @@
       <c r="H20" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="10" t="s">
-        <v>19</v>
+      <c r="I20" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J20" s="11">
         <v>18</v>
@@ -8406,8 +8406,8 @@
       <c r="H21" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I21" s="10" t="s">
-        <v>19</v>
+      <c r="I21" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J21" s="11">
         <v>19</v>
@@ -8438,8 +8438,8 @@
       <c r="H22" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I22" s="10" t="s">
-        <v>19</v>
+      <c r="I22" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J22" s="11">
         <v>20</v>
@@ -8470,8 +8470,8 @@
       <c r="H23" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I23" s="10" t="s">
-        <v>19</v>
+      <c r="I23" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J23" s="11">
         <v>21</v>
@@ -8502,8 +8502,8 @@
       <c r="H24" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I24" s="10" t="s">
-        <v>19</v>
+      <c r="I24" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J24" s="11">
         <v>22</v>
@@ -8534,8 +8534,8 @@
       <c r="H25" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I25" s="10" t="s">
-        <v>19</v>
+      <c r="I25" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J25" s="11">
         <v>23</v>
@@ -8566,8 +8566,8 @@
       <c r="H26" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I26" s="10" t="s">
-        <v>19</v>
+      <c r="I26" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J26" s="11">
         <v>24</v>
@@ -8598,8 +8598,8 @@
       <c r="H27" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I27" s="10" t="s">
-        <v>19</v>
+      <c r="I27" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J27" s="11">
         <v>25</v>
@@ -8630,8 +8630,8 @@
       <c r="H28" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I28" s="10" t="s">
-        <v>19</v>
+      <c r="I28" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J28" s="11">
         <v>26</v>
@@ -8662,8 +8662,8 @@
       <c r="H29" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I29" s="10" t="s">
-        <v>19</v>
+      <c r="I29" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J29" s="11">
         <v>27</v>
@@ -8694,8 +8694,8 @@
       <c r="H30" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="10" t="s">
-        <v>19</v>
+      <c r="I30" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J30" s="11">
         <v>28</v>
@@ -8726,8 +8726,8 @@
       <c r="H31" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I31" s="10" t="s">
-        <v>19</v>
+      <c r="I31" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J31" s="11">
         <v>29</v>
@@ -8758,8 +8758,8 @@
       <c r="H32" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I32" s="10" t="s">
-        <v>19</v>
+      <c r="I32" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J32" s="11">
         <v>30</v>
@@ -8790,8 +8790,8 @@
       <c r="H33" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I33" s="10" t="s">
-        <v>19</v>
+      <c r="I33" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J33" s="11">
         <v>31</v>
@@ -8822,8 +8822,8 @@
       <c r="H34" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I34" s="10" t="s">
-        <v>19</v>
+      <c r="I34" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J34" s="11">
         <v>32</v>
@@ -8854,8 +8854,8 @@
       <c r="H35" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I35" s="10" t="s">
-        <v>19</v>
+      <c r="I35" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J35" s="11">
         <v>33</v>
@@ -8886,8 +8886,8 @@
       <c r="H36" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I36" s="10" t="s">
-        <v>19</v>
+      <c r="I36" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J36" s="11">
         <v>34</v>
@@ -8918,8 +8918,8 @@
       <c r="H37" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I37" s="10" t="s">
-        <v>19</v>
+      <c r="I37" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J37" s="11">
         <v>35</v>
@@ -8950,8 +8950,8 @@
       <c r="H38" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="10" t="s">
-        <v>19</v>
+      <c r="I38" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J38" s="11">
         <v>36</v>
@@ -8982,8 +8982,8 @@
       <c r="H39" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="10" t="s">
-        <v>19</v>
+      <c r="I39" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J39" s="11">
         <v>37</v>
@@ -9014,8 +9014,8 @@
       <c r="H40" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I40" s="10" t="s">
-        <v>19</v>
+      <c r="I40" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J40" s="11">
         <v>38</v>
@@ -9046,8 +9046,8 @@
       <c r="H41" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I41" s="10" t="s">
-        <v>19</v>
+      <c r="I41" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J41" s="11">
         <v>39</v>
@@ -9078,8 +9078,8 @@
       <c r="H42" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I42" s="10" t="s">
-        <v>19</v>
+      <c r="I42" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J42" s="11">
         <v>40</v>
@@ -9108,10 +9108,10 @@
         <v>115</v>
       </c>
       <c r="H43" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="I43" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J43" s="11">
         <v>41</v>
@@ -9142,8 +9142,8 @@
       <c r="H44" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I44" s="10" t="s">
-        <v>19</v>
+      <c r="I44" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J44" s="11">
         <v>42</v>
@@ -9174,8 +9174,8 @@
       <c r="H45" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I45" s="10" t="s">
-        <v>19</v>
+      <c r="I45" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J45" s="11">
         <v>43</v>
@@ -9206,8 +9206,8 @@
       <c r="H46" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I46" s="10" t="s">
-        <v>19</v>
+      <c r="I46" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J46" s="11">
         <v>44</v>
@@ -9238,8 +9238,8 @@
       <c r="H47" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I47" s="10" t="s">
-        <v>19</v>
+      <c r="I47" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J47" s="11">
         <v>45</v>
@@ -9270,8 +9270,8 @@
       <c r="H48" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I48" s="10" t="s">
-        <v>19</v>
+      <c r="I48" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J48" s="11">
         <v>46</v>
@@ -9302,8 +9302,8 @@
       <c r="H49" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I49" s="10" t="s">
-        <v>19</v>
+      <c r="I49" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J49" s="11">
         <v>47</v>
@@ -9334,8 +9334,8 @@
       <c r="H50" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I50" s="10" t="s">
-        <v>19</v>
+      <c r="I50" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J50" s="11">
         <v>48</v>
@@ -9366,8 +9366,8 @@
       <c r="H51" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I51" s="10" t="s">
-        <v>19</v>
+      <c r="I51" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J51" s="11">
         <v>49</v>
@@ -9398,8 +9398,8 @@
       <c r="H52" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I52" s="10" t="s">
-        <v>19</v>
+      <c r="I52" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J52" s="11">
         <v>50</v>
@@ -9428,10 +9428,10 @@
         <v>632</v>
       </c>
       <c r="H53" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I53" s="10" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="I53" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J53" s="11">
         <v>51</v>
@@ -9462,8 +9462,8 @@
       <c r="H54" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I54" s="10" t="s">
-        <v>19</v>
+      <c r="I54" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J54" s="11">
         <v>52</v>
@@ -9492,10 +9492,10 @@
         <v>75</v>
       </c>
       <c r="H55" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I55" s="10" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="I55" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J55" s="11">
         <v>53</v>
@@ -9526,8 +9526,8 @@
       <c r="H56" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I56" s="10" t="s">
-        <v>19</v>
+      <c r="I56" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J56" s="11">
         <v>54</v>
@@ -9558,8 +9558,8 @@
       <c r="H57" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I57" s="10" t="s">
-        <v>19</v>
+      <c r="I57" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J57" s="11">
         <v>55</v>
@@ -9590,8 +9590,8 @@
       <c r="H58" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I58" s="10" t="s">
-        <v>19</v>
+      <c r="I58" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J58" s="11">
         <v>56</v>
@@ -9622,8 +9622,8 @@
       <c r="H59" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I59" s="10" t="s">
-        <v>19</v>
+      <c r="I59" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J59" s="11">
         <v>57</v>
@@ -9654,8 +9654,8 @@
       <c r="H60" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I60" s="10" t="s">
-        <v>19</v>
+      <c r="I60" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J60" s="11">
         <v>58</v>
@@ -9686,8 +9686,8 @@
       <c r="H61" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I61" s="10" t="s">
-        <v>19</v>
+      <c r="I61" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J61" s="11">
         <v>59</v>
@@ -9718,8 +9718,8 @@
       <c r="H62" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I62" s="10" t="s">
-        <v>19</v>
+      <c r="I62" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J62" s="11">
         <v>60</v>
@@ -9750,8 +9750,8 @@
       <c r="H63" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I63" s="10" t="s">
-        <v>19</v>
+      <c r="I63" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J63" s="11">
         <v>61</v>
@@ -9782,8 +9782,8 @@
       <c r="H64" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I64" s="10" t="s">
-        <v>19</v>
+      <c r="I64" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J64" s="11">
         <v>62</v>
@@ -9814,8 +9814,8 @@
       <c r="H65" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I65" s="10" t="s">
-        <v>19</v>
+      <c r="I65" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J65" s="11">
         <v>63</v>
@@ -9846,8 +9846,8 @@
       <c r="H66" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I66" s="10" t="s">
-        <v>19</v>
+      <c r="I66" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J66" s="11">
         <v>64</v>
@@ -9878,8 +9878,8 @@
       <c r="H67" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I67" s="10" t="s">
-        <v>19</v>
+      <c r="I67" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J67" s="11">
         <v>65</v>
@@ -9910,8 +9910,8 @@
       <c r="H68" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I68" s="10" t="s">
-        <v>19</v>
+      <c r="I68" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J68" s="11">
         <v>66</v>
@@ -9942,8 +9942,8 @@
       <c r="H69" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I69" s="10" t="s">
-        <v>19</v>
+      <c r="I69" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J69" s="11">
         <v>67</v>
@@ -9974,8 +9974,8 @@
       <c r="H70" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I70" s="10" t="s">
-        <v>19</v>
+      <c r="I70" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J70" s="11">
         <v>68</v>
@@ -10006,8 +10006,8 @@
       <c r="H71" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I71" s="10" t="s">
-        <v>19</v>
+      <c r="I71" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J71" s="11">
         <v>69</v>
@@ -10038,8 +10038,8 @@
       <c r="H72" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I72" s="10" t="s">
-        <v>19</v>
+      <c r="I72" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J72" s="11">
         <v>70</v>
@@ -10070,8 +10070,8 @@
       <c r="H73" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I73" s="10" t="s">
-        <v>19</v>
+      <c r="I73" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J73" s="11">
         <v>71</v>
@@ -10102,8 +10102,8 @@
       <c r="H74" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I74" s="10" t="s">
-        <v>19</v>
+      <c r="I74" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J74" s="11">
         <v>72</v>
@@ -10134,8 +10134,8 @@
       <c r="H75" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I75" s="10" t="s">
-        <v>19</v>
+      <c r="I75" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J75" s="11">
         <v>73</v>
@@ -10166,8 +10166,8 @@
       <c r="H76" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I76" s="10" t="s">
-        <v>19</v>
+      <c r="I76" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J76" s="11">
         <v>74</v>
@@ -10198,8 +10198,8 @@
       <c r="H77" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I77" s="10" t="s">
-        <v>19</v>
+      <c r="I77" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J77" s="11">
         <v>75</v>
@@ -10230,8 +10230,8 @@
       <c r="H78" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I78" s="10" t="s">
-        <v>19</v>
+      <c r="I78" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J78" s="11">
         <v>76</v>
@@ -10262,8 +10262,8 @@
       <c r="H79" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I79" s="10" t="s">
-        <v>19</v>
+      <c r="I79" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J79" s="11">
         <v>77</v>
@@ -10294,8 +10294,8 @@
       <c r="H80" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I80" s="10" t="s">
-        <v>19</v>
+      <c r="I80" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J80" s="11">
         <v>78</v>
@@ -10326,8 +10326,8 @@
       <c r="H81" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I81" s="10" t="s">
-        <v>19</v>
+      <c r="I81" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J81" s="11">
         <v>79</v>
@@ -10358,8 +10358,8 @@
       <c r="H82" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I82" s="10" t="s">
-        <v>19</v>
+      <c r="I82" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J82" s="11">
         <v>80</v>
@@ -10390,8 +10390,8 @@
       <c r="H83" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I83" s="10" t="s">
-        <v>19</v>
+      <c r="I83" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J83" s="11">
         <v>81</v>
@@ -10420,10 +10420,10 @@
         <v>734</v>
       </c>
       <c r="H84" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I84" s="10" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="I84" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J84" s="11">
         <v>82</v>
@@ -10454,8 +10454,8 @@
       <c r="H85" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I85" s="10" t="s">
-        <v>19</v>
+      <c r="I85" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J85" s="11">
         <v>83</v>
@@ -10486,8 +10486,8 @@
       <c r="H86" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I86" s="10" t="s">
-        <v>19</v>
+      <c r="I86" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J86" s="11">
         <v>84</v>
@@ -10518,8 +10518,8 @@
       <c r="H87" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I87" s="10" t="s">
-        <v>19</v>
+      <c r="I87" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J87" s="11">
         <v>85</v>
@@ -10550,8 +10550,8 @@
       <c r="H88" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I88" s="10" t="s">
-        <v>19</v>
+      <c r="I88" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J88" s="11">
         <v>86</v>
@@ -10582,8 +10582,8 @@
       <c r="H89" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I89" s="10" t="s">
-        <v>19</v>
+      <c r="I89" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J89" s="11">
         <v>87</v>
@@ -10614,8 +10614,8 @@
       <c r="H90" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I90" s="10" t="s">
-        <v>19</v>
+      <c r="I90" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J90" s="11">
         <v>88</v>
@@ -10646,8 +10646,8 @@
       <c r="H91" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I91" s="10" t="s">
-        <v>19</v>
+      <c r="I91" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J91" s="11">
         <v>89</v>
@@ -10678,8 +10678,8 @@
       <c r="H92" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I92" s="10" t="s">
-        <v>19</v>
+      <c r="I92" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J92" s="11">
         <v>90</v>
@@ -10710,8 +10710,8 @@
       <c r="H93" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I93" s="10" t="s">
-        <v>19</v>
+      <c r="I93" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J93" s="11">
         <v>91</v>
@@ -10742,8 +10742,8 @@
       <c r="H94" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I94" s="10" t="s">
-        <v>19</v>
+      <c r="I94" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J94" s="11">
         <v>92</v>
@@ -10774,8 +10774,8 @@
       <c r="H95" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I95" s="10" t="s">
-        <v>19</v>
+      <c r="I95" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J95" s="11">
         <v>93</v>
@@ -10806,8 +10806,8 @@
       <c r="H96" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I96" s="10" t="s">
-        <v>19</v>
+      <c r="I96" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J96" s="11">
         <v>94</v>
@@ -10838,8 +10838,8 @@
       <c r="H97" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I97" s="10" t="s">
-        <v>19</v>
+      <c r="I97" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J97" s="11">
         <v>95</v>
@@ -10870,8 +10870,8 @@
       <c r="H98" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I98" s="10" t="s">
-        <v>19</v>
+      <c r="I98" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J98" s="11">
         <v>96</v>
@@ -10902,8 +10902,8 @@
       <c r="H99" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I99" s="10" t="s">
-        <v>19</v>
+      <c r="I99" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J99" s="11">
         <v>97</v>
@@ -10934,8 +10934,8 @@
       <c r="H100" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I100" s="10" t="s">
-        <v>19</v>
+      <c r="I100" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J100" s="11">
         <v>98</v>
@@ -10966,8 +10966,8 @@
       <c r="H101" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I101" s="10" t="s">
-        <v>19</v>
+      <c r="I101" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J101" s="11">
         <v>99</v>
@@ -10998,8 +10998,8 @@
       <c r="H102" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I102" s="10" t="s">
-        <v>19</v>
+      <c r="I102" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J102" s="11">
         <v>100</v>
@@ -11030,8 +11030,8 @@
       <c r="H103" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I103" s="10" t="s">
-        <v>19</v>
+      <c r="I103" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J103" s="11">
         <v>101</v>
@@ -11062,8 +11062,8 @@
       <c r="H104" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I104" s="10" t="s">
-        <v>19</v>
+      <c r="I104" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J104" s="11">
         <v>102</v>
@@ -11094,8 +11094,8 @@
       <c r="H105" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I105" s="10" t="s">
-        <v>19</v>
+      <c r="I105" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J105" s="11">
         <v>103</v>
@@ -11126,8 +11126,8 @@
       <c r="H106" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I106" s="10" t="s">
-        <v>19</v>
+      <c r="I106" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J106" s="11">
         <v>104</v>
@@ -11158,8 +11158,8 @@
       <c r="H107" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I107" s="10" t="s">
-        <v>19</v>
+      <c r="I107" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J107" s="11">
         <v>105</v>
@@ -11190,8 +11190,8 @@
       <c r="H108" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I108" s="10" t="s">
-        <v>19</v>
+      <c r="I108" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J108" s="11">
         <v>106</v>
@@ -11222,8 +11222,8 @@
       <c r="H109" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I109" s="10" t="s">
-        <v>19</v>
+      <c r="I109" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J109" s="11">
         <v>107</v>
@@ -11254,8 +11254,8 @@
       <c r="H110" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I110" s="10" t="s">
-        <v>19</v>
+      <c r="I110" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J110" s="11">
         <v>108</v>
@@ -11286,8 +11286,8 @@
       <c r="H111" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="I111" s="10" t="s">
-        <v>19</v>
+      <c r="I111" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J111" s="11">
         <v>109</v>
@@ -11318,8 +11318,8 @@
       <c r="H112" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="I112" s="10" t="s">
-        <v>19</v>
+      <c r="I112" s="10" t="b">
+        <v>0</v>
       </c>
       <c r="J112" s="11">
         <v>110</v>

</xml_diff>

<commit_message>
Sniper dual and whose the pillager.
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101FEF6C-AE35-4639-B8DC-1AC3E98330DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4578CFDA-5FF8-4E90-A1B3-BE46E489C9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="1" r:id="rId1"/>
     <sheet name="Advancements" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -2610,58 +2610,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -2772,6 +2720,27 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2893,6 +2862,37 @@
       </fill>
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2907,23 +2907,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:K127" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:K127" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A2:K127" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J127">
     <sortCondition ref="J2:J127"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Achievment" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="In-game description" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Actual requirements (if different)" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Category" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Property Name" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Index" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Achievement (English Title)" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Implement" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Player.json" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sort Order" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column1" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Achievment" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="In-game description" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Actual requirements (if different)" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Category" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Property Name" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Index" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Achievement (English Title)" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Implement" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Player.json" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sort Order" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column1" dataDxfId="15">
       <calculatedColumnFormula>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2932,22 +2932,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:J112" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:J112" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A2:J112" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J112">
     <sortCondition ref="J2:J112"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Advancement" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="In-game description" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Actual requirements (if different)" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Category" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Property Name" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Index" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Advancement (English Title)" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Implement" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Player.json" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Sort Order" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Advancement" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="In-game description" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Actual requirements (if different)" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Category" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Property Name" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Index" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Advancement (English Title)" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Implement" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Player.json" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Sort Order" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3218,25 +3218,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G130" sqref="G130"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.59765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.59765625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="50.59765625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="15.59765625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="35.59765625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.59765625" style="3" customWidth="1"/>
-    <col min="9" max="10" width="15.59765625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="35.59765625" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="50.59765625" style="4"/>
+    <col min="1" max="1" width="35.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="3" customWidth="1"/>
+    <col min="9" max="10" width="15.5703125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="35.5703125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="50.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3245,14 +3245,14 @@
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
-      <c r="H1" s="8" t="str">
-        <f>_xlfn.CONCAT("Complete: ",COUNTIF(Table1[Implement],"=TRUE")," / ",ROWS(Table1[]))</f>
-        <v>Complete: 51 / 125</v>
+      <c r="H1" s="8" t="e">
+        <f ca="1">_xlfn.CONCAT("Complete: ",COUNTIF(Table1[Implement],"=TRUE")," / ",ROWS(Table1[]))</f>
+        <v>#NAME?</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3288,10 +3288,10 @@
       </c>
       <c r="M2" s="1">
         <f>COUNTIF(Table1[Implement],"=TRUE")</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -3328,10 +3328,10 @@
       </c>
       <c r="M3" s="1">
         <f>COUNTIF(Table1[Implement],"=FALSE")</f>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>Story12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>Story13</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>Story14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -3475,7 +3475,7 @@
         <v>Story15</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>Story16</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>Husbandry11</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>Husbandry12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>48</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>Husbandry13</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>Story17</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>Husbandry14</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>Adventure11</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>67</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>Story18</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>71</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>Adventure12</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>75</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>Husbandry15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>79</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>Adventure13</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>83</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>86</v>
       </c>
       <c r="H19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="2" t="b">
         <v>0</v>
@@ -3907,7 +3907,7 @@
         <v>Adventure14</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>87</v>
       </c>
@@ -3943,7 +3943,7 @@
         <v>Story19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>91</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>Nether11</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>97</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>Nether12</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>101</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>Nether13</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>105</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>Nether14</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>109</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>The_End11</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>115</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>The_End12</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>118</v>
       </c>
@@ -4195,7 +4195,7 @@
         <v>Story110</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>121</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>Adventure15</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>124</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>Adventure16</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>127</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>Adventure17</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>131</v>
       </c>
@@ -4339,7 +4339,7 @@
         <v>Nether15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>135</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>Nether16</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>138</v>
       </c>
@@ -4411,7 +4411,7 @@
         <v>Nether17</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>142</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>Husbandry17</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>145</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>Story111</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>149</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>Story112</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>152</v>
       </c>
@@ -4555,7 +4555,7 @@
         <v>Story113</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>156</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>Story114</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>159</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>Husbandry16</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>163</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>Husbandry18</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>166</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>Adventure18</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>170</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>Story115</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>173</v>
       </c>
@@ -4771,7 +4771,7 @@
         <v>Story116</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>176</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>Story117</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>179</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>Adventure19</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>183</v>
       </c>
@@ -4879,7 +4879,7 @@
         <v>Husbandry19</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>186</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>Husbandry110</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>190</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>Adventure110</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>193</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>Story118</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>197</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>Story119</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>201</v>
       </c>
@@ -5059,7 +5059,7 @@
         <v>Husbandry111</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>204</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>Story120</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>207</v>
       </c>
@@ -5131,7 +5131,7 @@
         <v>Husbandry112</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>211</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>Husbandry113</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>214</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>Adventure111</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>216</v>
       </c>
@@ -5239,7 +5239,7 @@
         <v>Story121</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>219</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>Adventure112</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>221</v>
       </c>
@@ -5311,7 +5311,7 @@
         <v>Adventure113</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>223</v>
       </c>
@@ -5347,7 +5347,7 @@
         <v>Story122</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>227</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>Story123</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>230</v>
       </c>
@@ -5419,7 +5419,7 @@
         <v>Story124</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>234</v>
       </c>
@@ -5455,7 +5455,7 @@
         <v>Adventure114</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>238</v>
       </c>
@@ -5491,7 +5491,7 @@
         <v>Story125</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>240</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>Husbandry114</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>243</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>Husbandry115</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>246</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>Adventure115</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>250</v>
       </c>
@@ -5635,7 +5635,7 @@
         <v>Husbandry116</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>253</v>
       </c>
@@ -5671,7 +5671,7 @@
         <v>Adventure116</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>256</v>
       </c>
@@ -5707,7 +5707,7 @@
         <v>Story126</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>259</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>Story127</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>262</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>The_End13</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>266</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>Nether18</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>270</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>The_End14</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>273</v>
       </c>
@@ -5887,7 +5887,7 @@
         <v>The_End15</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>276</v>
       </c>
@@ -5923,7 +5923,7 @@
         <v>The_End16</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>279</v>
       </c>
@@ -5959,7 +5959,7 @@
         <v>Adventure117</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>283</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>The_End17</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>286</v>
       </c>
@@ -6031,7 +6031,7 @@
         <v>Adventure118</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>290</v>
       </c>
@@ -6067,7 +6067,7 @@
         <v>Adventure119</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>293</v>
       </c>
@@ -6103,7 +6103,7 @@
         <v>Adventure120</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>296</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>Husbandry117</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>299</v>
       </c>
@@ -6175,7 +6175,7 @@
         <v>Adventure121</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>302</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>Adventure122</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>306</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>Adventure123</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>309</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>Adventure124</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>312</v>
       </c>
@@ -6319,7 +6319,7 @@
         <v>Husbandry118</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>316</v>
       </c>
@@ -6355,7 +6355,7 @@
         <v>Adventure125</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>320</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>Adventure126</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>324</v>
       </c>
@@ -6427,7 +6427,7 @@
         <v>Story128</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>328</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>Adventure127</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>332</v>
       </c>
@@ -6499,7 +6499,7 @@
         <v>Story129</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>335</v>
       </c>
@@ -6535,7 +6535,7 @@
         <v>Adventure128</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>338</v>
       </c>
@@ -6571,7 +6571,7 @@
         <v>Story130</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>341</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>Story131</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>345</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>Husbandry119</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>349</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>Husbandry120</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>351</v>
       </c>
@@ -6715,7 +6715,7 @@
         <v>Story132</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>355</v>
       </c>
@@ -6751,7 +6751,7 @@
         <v>Husbandry121</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>359</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>Adventure129</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>362</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>Story21</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>367</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>Story22</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>369</v>
       </c>
@@ -6895,7 +6895,7 @@
         <v>Adventure130</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>373</v>
       </c>
@@ -6931,7 +6931,7 @@
         <v>Story23</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>376</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>Adventure131</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>379</v>
       </c>
@@ -7003,7 +7003,7 @@
         <v>Story24</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>383</v>
       </c>
@@ -7039,7 +7039,7 @@
         <v>Story25</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>386</v>
       </c>
@@ -7075,7 +7075,7 @@
         <v>Husbandry122</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>389</v>
       </c>
@@ -7111,7 +7111,7 @@
         <v>Husbandry123</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>392</v>
       </c>
@@ -7147,7 +7147,7 @@
         <v>Story26</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>395</v>
       </c>
@@ -7183,7 +7183,7 @@
         <v>Story27</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>397</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>Nether19</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>401</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>Nether110</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>405</v>
       </c>
@@ -7291,7 +7291,7 @@
         <v>Nether111</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>409</v>
       </c>
@@ -7327,7 +7327,7 @@
         <v>Adventure132</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>413</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>Story28</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>417</v>
       </c>
@@ -7399,7 +7399,7 @@
         <v>Husbandry124</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>421</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>Story29</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>424</v>
       </c>
@@ -7471,7 +7471,7 @@
         <v>Story210</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>428</v>
       </c>
@@ -7507,7 +7507,7 @@
         <v>Story211</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>432</v>
       </c>
@@ -7543,7 +7543,7 @@
         <v>Nether112</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>436</v>
       </c>
@@ -7579,7 +7579,7 @@
         <v>Story212</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>439</v>
       </c>
@@ -7615,7 +7615,7 @@
         <v>Husbandry125</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>443</v>
       </c>
@@ -7651,7 +7651,7 @@
         <v>Nether113</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>447</v>
       </c>
@@ -7687,7 +7687,7 @@
         <v>Story213</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>451</v>
       </c>
@@ -7723,7 +7723,7 @@
         <v>Story214</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>454</v>
       </c>
@@ -7759,7 +7759,7 @@
         <v>Story215</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>457</v>
       </c>
@@ -7797,18 +7797,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:K1048576">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="31" priority="3">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="30" priority="4">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="29" priority="5">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I127" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -7826,26 +7826,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.59765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.59765625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="50.59765625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="15.59765625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="35.59765625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.59765625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15.59765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.59765625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="50.59765625" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="50.59765625" style="4"/>
+    <col min="1" max="1" width="35.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="50.5703125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="50.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7857,14 +7857,14 @@
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
-      <c r="H1" s="8" t="str">
-        <f>_xlfn.CONCAT("Complete: ",COUNTIF(Table2[Implement],"=TRUE")," / ",ROWS(Table2[]))</f>
-        <v>Complete: 52 / 110</v>
+      <c r="H1" s="8" t="e">
+        <f ca="1">_xlfn.CONCAT("Complete: ",COUNTIF(Table2[Implement],"=TRUE")," / ",ROWS(Table2[]))</f>
+        <v>#NAME?</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>460</v>
       </c>
@@ -7896,7 +7896,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>462</v>
       </c>
@@ -7928,7 +7928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>466</v>
       </c>
@@ -7961,14 +7961,14 @@
       </c>
       <c r="M4" s="1">
         <f>COUNTIF(Table2[Implement],"=TRUE")</f>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="N4" s="4">
         <f>M4+Achievements!M2</f>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -8001,14 +8001,14 @@
       </c>
       <c r="M5" s="1">
         <f>COUNTIF(Table2[Implement],"=FALSE")</f>
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N5" s="4">
         <f>M5+Achievements!M3</f>
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -8044,7 +8044,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>474</v>
       </c>
@@ -8076,7 +8076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>478</v>
       </c>
@@ -8108,7 +8108,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>482</v>
       </c>
@@ -8140,7 +8140,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>486</v>
       </c>
@@ -8172,7 +8172,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>490</v>
       </c>
@@ -8204,7 +8204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>494</v>
       </c>
@@ -8236,7 +8236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>498</v>
       </c>
@@ -8268,7 +8268,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>502</v>
       </c>
@@ -8300,7 +8300,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>118</v>
       </c>
@@ -8332,7 +8332,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>207</v>
       </c>
@@ -8364,7 +8364,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>510</v>
       </c>
@@ -8396,7 +8396,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>109</v>
       </c>
@@ -8428,7 +8428,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>94</v>
       </c>
@@ -8460,7 +8460,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>97</v>
       </c>
@@ -8492,7 +8492,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>520</v>
       </c>
@@ -8524,7 +8524,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>523</v>
       </c>
@@ -8556,7 +8556,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>527</v>
       </c>
@@ -8588,7 +8588,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>531</v>
       </c>
@@ -8620,7 +8620,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>535</v>
       </c>
@@ -8652,7 +8652,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>539</v>
       </c>
@@ -8684,7 +8684,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>543</v>
       </c>
@@ -8716,7 +8716,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>547</v>
       </c>
@@ -8748,7 +8748,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>551</v>
       </c>
@@ -8780,7 +8780,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>555</v>
       </c>
@@ -8812,7 +8812,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>558</v>
       </c>
@@ -8844,7 +8844,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>562</v>
       </c>
@@ -8876,7 +8876,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>101</v>
       </c>
@@ -8908,7 +8908,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>568</v>
       </c>
@@ -8940,7 +8940,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>432</v>
       </c>
@@ -8972,7 +8972,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>573</v>
       </c>
@@ -9004,7 +9004,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>577</v>
       </c>
@@ -9036,7 +9036,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>105</v>
       </c>
@@ -9068,7 +9068,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>583</v>
       </c>
@@ -9100,7 +9100,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>587</v>
       </c>
@@ -9132,7 +9132,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>591</v>
       </c>
@@ -9164,7 +9164,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>594</v>
       </c>
@@ -9196,7 +9196,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>115</v>
       </c>
@@ -9228,7 +9228,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>600</v>
       </c>
@@ -9260,7 +9260,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>604</v>
       </c>
@@ -9292,7 +9292,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>608</v>
       </c>
@@ -9324,7 +9324,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>270</v>
       </c>
@@ -9356,7 +9356,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>262</v>
       </c>
@@ -9388,7 +9388,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>616</v>
       </c>
@@ -9420,7 +9420,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>620</v>
       </c>
@@ -9452,7 +9452,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>273</v>
       </c>
@@ -9484,7 +9484,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>64</v>
       </c>
@@ -9516,7 +9516,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>628</v>
       </c>
@@ -9548,7 +9548,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>632</v>
       </c>
@@ -9580,7 +9580,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>71</v>
       </c>
@@ -9612,7 +9612,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>637</v>
       </c>
@@ -9644,7 +9644,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>641</v>
       </c>
@@ -9676,7 +9676,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>645</v>
       </c>
@@ -9708,7 +9708,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>392</v>
       </c>
@@ -9740,7 +9740,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>650</v>
       </c>
@@ -9772,7 +9772,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>653</v>
       </c>
@@ -9804,7 +9804,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>421</v>
       </c>
@@ -9836,7 +9836,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>659</v>
       </c>
@@ -9868,7 +9868,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>447</v>
       </c>
@@ -9900,7 +9900,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>664</v>
       </c>
@@ -9932,7 +9932,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>668</v>
       </c>
@@ -9964,7 +9964,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>672</v>
       </c>
@@ -9996,7 +9996,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>676</v>
       </c>
@@ -10028,7 +10028,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>680</v>
       </c>
@@ -10060,7 +10060,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>684</v>
       </c>
@@ -10092,7 +10092,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>688</v>
       </c>
@@ -10124,7 +10124,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>692</v>
       </c>
@@ -10156,7 +10156,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>695</v>
       </c>
@@ -10188,7 +10188,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>699</v>
       </c>
@@ -10220,7 +10220,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>703</v>
       </c>
@@ -10252,7 +10252,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>705</v>
       </c>
@@ -10284,7 +10284,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>709</v>
       </c>
@@ -10307,7 +10307,7 @@
         <v>712</v>
       </c>
       <c r="H77" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I77" s="2" t="b">
         <v>0</v>
@@ -10316,7 +10316,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>713</v>
       </c>
@@ -10348,7 +10348,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>716</v>
       </c>
@@ -10380,7 +10380,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="285" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:10" ht="285" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>127</v>
       </c>
@@ -10412,7 +10412,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>428</v>
       </c>
@@ -10444,7 +10444,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>722</v>
       </c>
@@ -10476,7 +10476,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>726</v>
       </c>
@@ -10508,7 +10508,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>729</v>
       </c>
@@ -10540,7 +10540,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
@@ -10563,7 +10563,7 @@
         <v>86</v>
       </c>
       <c r="H85" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I85" s="2" t="b">
         <v>0</v>
@@ -10572,7 +10572,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>395</v>
       </c>
@@ -10604,7 +10604,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>41</v>
       </c>
@@ -10636,7 +10636,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>741</v>
       </c>
@@ -10668,7 +10668,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>745</v>
       </c>
@@ -10700,7 +10700,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>749</v>
       </c>
@@ -10732,7 +10732,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>753</v>
       </c>
@@ -10764,7 +10764,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>756</v>
       </c>
@@ -10796,7 +10796,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>760</v>
       </c>
@@ -10828,7 +10828,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>764</v>
       </c>
@@ -10860,7 +10860,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>389</v>
       </c>
@@ -10892,7 +10892,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>769</v>
       </c>
@@ -10924,7 +10924,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>772</v>
       </c>
@@ -10956,7 +10956,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>776</v>
       </c>
@@ -10988,7 +10988,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>780</v>
       </c>
@@ -11020,7 +11020,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>784</v>
       </c>
@@ -11052,7 +11052,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>788</v>
       </c>
@@ -11084,7 +11084,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>792</v>
       </c>
@@ -11116,7 +11116,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>796</v>
       </c>
@@ -11148,7 +11148,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>800</v>
       </c>
@@ -11180,7 +11180,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>804</v>
       </c>
@@ -11212,7 +11212,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="195" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:10" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>808</v>
       </c>
@@ -11244,7 +11244,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>812</v>
       </c>
@@ -11276,7 +11276,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>816</v>
       </c>
@@ -11308,7 +11308,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>820</v>
       </c>
@@ -11340,7 +11340,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>824</v>
       </c>
@@ -11372,7 +11372,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>828</v>
       </c>
@@ -11404,7 +11404,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>417</v>
       </c>
@@ -11438,13 +11438,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:J1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added use on block method and added copper advancements.
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9D0E91-57BF-42EA-9261-424F45BFB198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859CF76C-0E01-42C4-9B2B-AD916CD58695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="1" r:id="rId1"/>
@@ -2943,7 +2943,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:K127" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A2:K127" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <autoFilter ref="A2:K127" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J127">
     <sortCondition ref="J2:J127"/>
   </sortState>
@@ -3253,8 +3259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M127"/>
   <sheetViews>
-    <sheetView topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="H115" sqref="H115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3282,7 +3288,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="8" t="str">
         <f>CONCATENATE("Complete: ",COUNTIF(Table1[Implement],"=TRUE"),"/",ROWS(Table1[Implement]))</f>
-        <v>Complete: 60/125</v>
+        <v>Complete: 62/125</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -3323,10 +3329,10 @@
       </c>
       <c r="M2" s="1">
         <f>COUNTIF(Table1[Implement],"=TRUE")</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -3363,10 +3369,10 @@
       </c>
       <c r="M3" s="1">
         <f>COUNTIF(Table1[Implement],"=FALSE")</f>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -3402,7 +3408,7 @@
         <v>Story12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -3438,7 +3444,7 @@
         <v>Story13</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -3474,7 +3480,7 @@
         <v>Story14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -3510,7 +3516,7 @@
         <v>Story15</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -3546,7 +3552,7 @@
         <v>Story16</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -3582,7 +3588,7 @@
         <v>Husbandry11</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -3618,7 +3624,7 @@
         <v>Husbandry12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>48</v>
       </c>
@@ -3654,7 +3660,7 @@
         <v>Husbandry13</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
@@ -3690,7 +3696,7 @@
         <v>Story17</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
@@ -3726,7 +3732,7 @@
         <v>Husbandry14</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
@@ -3762,7 +3768,7 @@
         <v>Adventure11</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
@@ -3798,7 +3804,7 @@
         <v>Story18</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>70</v>
       </c>
@@ -3834,7 +3840,7 @@
         <v>Adventure12</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>74</v>
       </c>
@@ -3906,7 +3912,7 @@
         <v>Adventure13</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
@@ -3942,7 +3948,7 @@
         <v>Adventure14</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>86</v>
       </c>
@@ -3978,7 +3984,7 @@
         <v>Story19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>90</v>
       </c>
@@ -4014,7 +4020,7 @@
         <v>Nether11</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>96</v>
       </c>
@@ -4050,7 +4056,7 @@
         <v>Nether12</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>100</v>
       </c>
@@ -4122,7 +4128,7 @@
         <v>Nether14</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>108</v>
       </c>
@@ -4158,7 +4164,7 @@
         <v>The_End11</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>114</v>
       </c>
@@ -4194,7 +4200,7 @@
         <v>The_End12</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>117</v>
       </c>
@@ -4230,7 +4236,7 @@
         <v>Story110</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>120</v>
       </c>
@@ -4266,7 +4272,7 @@
         <v>Adventure15</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>123</v>
       </c>
@@ -4338,7 +4344,7 @@
         <v>Adventure17</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>130</v>
       </c>
@@ -4374,7 +4380,7 @@
         <v>Nether15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>134</v>
       </c>
@@ -4446,7 +4452,7 @@
         <v>Nether17</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>141</v>
       </c>
@@ -4518,7 +4524,7 @@
         <v>Story111</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>148</v>
       </c>
@@ -4554,7 +4560,7 @@
         <v>Story112</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>151</v>
       </c>
@@ -4626,7 +4632,7 @@
         <v>Story114</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>158</v>
       </c>
@@ -4662,7 +4668,7 @@
         <v>Husbandry16</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>162</v>
       </c>
@@ -4698,7 +4704,7 @@
         <v>Husbandry18</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>165</v>
       </c>
@@ -4770,7 +4776,7 @@
         <v>Story115</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>172</v>
       </c>
@@ -4806,7 +4812,7 @@
         <v>Story116</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>175</v>
       </c>
@@ -4914,7 +4920,7 @@
         <v>Husbandry19</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>185</v>
       </c>
@@ -5058,7 +5064,7 @@
         <v>Story119</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>200</v>
       </c>
@@ -5094,7 +5100,7 @@
         <v>Husbandry111</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>203</v>
       </c>
@@ -5130,7 +5136,7 @@
         <v>Story120</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>206</v>
       </c>
@@ -5166,7 +5172,7 @@
         <v>Husbandry112</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>210</v>
       </c>
@@ -5202,7 +5208,7 @@
         <v>Husbandry113</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>213</v>
       </c>
@@ -5526,7 +5532,7 @@
         <v>Story125</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>239</v>
       </c>
@@ -5562,7 +5568,7 @@
         <v>Husbandry114</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>242</v>
       </c>
@@ -5634,7 +5640,7 @@
         <v>Adventure115</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>249</v>
       </c>
@@ -5670,7 +5676,7 @@
         <v>Husbandry116</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>252</v>
       </c>
@@ -5778,7 +5784,7 @@
         <v>Story127</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>261</v>
       </c>
@@ -5814,7 +5820,7 @@
         <v>The_End13</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>265</v>
       </c>
@@ -5850,7 +5856,7 @@
         <v>Nether18</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>269</v>
       </c>
@@ -5994,7 +6000,7 @@
         <v>Adventure117</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>282</v>
       </c>
@@ -6030,7 +6036,7 @@
         <v>The_End17</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>285</v>
       </c>
@@ -6066,7 +6072,7 @@
         <v>Adventure118</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>289</v>
       </c>
@@ -6318,7 +6324,7 @@
         <v>Adventure124</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>311</v>
       </c>
@@ -6570,7 +6576,7 @@
         <v>Adventure128</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>337</v>
       </c>
@@ -6678,7 +6684,7 @@
         <v>Husbandry119</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>348</v>
       </c>
@@ -6773,7 +6779,7 @@
         <v>357</v>
       </c>
       <c r="H98" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I98" s="2" t="b">
         <v>0</v>
@@ -6786,7 +6792,7 @@
         <v>Husbandry121</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>358</v>
       </c>
@@ -6966,7 +6972,7 @@
         <v>Story23</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>375</v>
       </c>
@@ -7182,7 +7188,7 @@
         <v>Story26</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>394</v>
       </c>
@@ -7218,7 +7224,7 @@
         <v>Story27</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>396</v>
       </c>
@@ -7385,7 +7391,7 @@
         <v>415</v>
       </c>
       <c r="H115" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I115" s="2" t="b">
         <v>0</v>
@@ -7650,7 +7656,7 @@
         <v>Husbandry125</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>442</v>
       </c>
@@ -7722,7 +7728,7 @@
         <v>Story213</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>450</v>
       </c>
@@ -7845,7 +7851,7 @@
   <conditionalFormatting sqref="K1:K1048576">
     <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I127" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
@@ -7861,8 +7867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7894,7 +7900,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="8" t="str">
         <f>CONCATENATE("Complete: ",COUNTIF(Table2[Implement],"=TRUE"),"/",ROWS(Table2[Implement]))</f>
-        <v>Complete: 59/110</v>
+        <v>Complete: 61/110</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -11029,7 +11035,7 @@
         <v>782</v>
       </c>
       <c r="H99" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I99" s="2" t="b">
         <v>0</v>
@@ -11317,7 +11323,7 @@
         <v>818</v>
       </c>
       <c r="H108" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I108" s="2" t="b">
         <v>0</v>
@@ -11466,7 +11472,7 @@
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I112" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
@@ -11482,13 +11488,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03723C66-8E0B-48F3-9CF4-1B0F8B736B8C}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -11516,7 +11522,7 @@
       </c>
       <c r="B2">
         <f>COUNTIF(Table1[Implement],"=TRUE")</f>
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C2">
         <f>COUNTIF(Table1[Player.json],"=TRUE")</f>
@@ -11524,15 +11530,15 @@
       </c>
       <c r="D2">
         <f>COUNTIF(Table1[Implement],"=FALSE")</f>
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E2">
-        <f>ROWS(Table2[Implement])</f>
-        <v>110</v>
+        <f>ROWS(Table1[Implement])</f>
+        <v>125</v>
       </c>
       <c r="F2" s="9">
         <f>B2/E2</f>
-        <v>0.54545454545454541</v>
+        <v>0.496</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -11541,7 +11547,7 @@
       </c>
       <c r="B3">
         <f>COUNTIF(Table2[Implement],"=TRUE")</f>
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C3">
         <f>COUNTIF(Table2[Player.json],"=TRUE")</f>
@@ -11549,15 +11555,15 @@
       </c>
       <c r="D3">
         <f>COUNTIF(Table2[Implement],"=FALSE")</f>
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3">
-        <f>ROWS(Table1[Implement])</f>
-        <v>125</v>
+        <f>ROWS(Table2[Implement])</f>
+        <v>110</v>
       </c>
       <c r="F3" s="9">
         <f t="shared" ref="F3:F4" si="0">B3/E3</f>
-        <v>0.47199999999999998</v>
+        <v>0.55454545454545456</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -11566,7 +11572,7 @@
       </c>
       <c r="B4">
         <f>B3+B2</f>
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:E4" si="1">C3+C2</f>
@@ -11574,7 +11580,7 @@
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
@@ -11582,7 +11588,7 @@
       </c>
       <c r="F4" s="9">
         <f t="shared" si="0"/>
-        <v>0.50638297872340421</v>
+        <v>0.52340425531914891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to enable zombie doctor and very very frightning
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859CF76C-0E01-42C4-9B2B-AD916CD58695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A19DE8-E94D-47D9-99A8-A8E5B340FD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2974,7 +2974,13 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:J112" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="A2:J112" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <autoFilter ref="A2:J112" xr:uid="{00000000-0009-0000-0100-000002000000}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="FALSE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J112">
     <sortCondition ref="J2:J112"/>
   </sortState>
@@ -6756,7 +6762,7 @@
         <v>Story132</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>354</v>
       </c>
@@ -7368,7 +7374,7 @@
         <v>Adventure132</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>412</v>
       </c>
@@ -7867,8 +7873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7900,7 +7906,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="8" t="str">
         <f>CONCATENATE("Complete: ",COUNTIF(Table2[Implement],"=TRUE"),"/",ROWS(Table2[Implement]))</f>
-        <v>Complete: 61/110</v>
+        <v>Complete: 62/110</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -7940,7 +7946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>461</v>
       </c>
@@ -7972,7 +7978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>465</v>
       </c>
@@ -8004,7 +8010,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -8036,7 +8042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -8068,7 +8074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>473</v>
       </c>
@@ -8100,7 +8106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>477</v>
       </c>
@@ -8132,7 +8138,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>481</v>
       </c>
@@ -8196,7 +8202,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>489</v>
       </c>
@@ -8228,7 +8234,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>493</v>
       </c>
@@ -8260,7 +8266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>497</v>
       </c>
@@ -8292,7 +8298,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>501</v>
       </c>
@@ -8356,7 +8362,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>206</v>
       </c>
@@ -8420,7 +8426,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>108</v>
       </c>
@@ -8452,7 +8458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>93</v>
       </c>
@@ -8484,7 +8490,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>96</v>
       </c>
@@ -8516,7 +8522,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>519</v>
       </c>
@@ -8548,7 +8554,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>522</v>
       </c>
@@ -8580,7 +8586,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>526</v>
       </c>
@@ -8612,7 +8618,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>530</v>
       </c>
@@ -8644,7 +8650,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>534</v>
       </c>
@@ -8740,7 +8746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>546</v>
       </c>
@@ -8836,7 +8842,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>557</v>
       </c>
@@ -8900,7 +8906,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>100</v>
       </c>
@@ -9028,7 +9034,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>576</v>
       </c>
@@ -9124,7 +9130,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="120" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>586</v>
       </c>
@@ -9188,7 +9194,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="225" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>593</v>
       </c>
@@ -9220,7 +9226,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>114</v>
       </c>
@@ -9252,7 +9258,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>599</v>
       </c>
@@ -9284,7 +9290,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>603</v>
       </c>
@@ -9348,7 +9354,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>269</v>
       </c>
@@ -9380,7 +9386,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>261</v>
       </c>
@@ -9444,7 +9450,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>619</v>
       </c>
@@ -9508,7 +9514,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>64</v>
       </c>
@@ -9540,7 +9546,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>627</v>
       </c>
@@ -9604,7 +9610,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="165" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>70</v>
       </c>
@@ -9764,7 +9770,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>649</v>
       </c>
@@ -9860,7 +9866,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>658</v>
       </c>
@@ -9956,7 +9962,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="135" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>667</v>
       </c>
@@ -10020,7 +10026,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>675</v>
       </c>
@@ -10084,7 +10090,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>683</v>
       </c>
@@ -10148,7 +10154,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>691</v>
       </c>
@@ -10180,7 +10186,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>694</v>
       </c>
@@ -10308,7 +10314,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>708</v>
       </c>
@@ -10532,7 +10538,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>728</v>
       </c>
@@ -10564,7 +10570,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>82</v>
       </c>
@@ -10596,7 +10602,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>394</v>
       </c>
@@ -10628,7 +10634,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>41</v>
       </c>
@@ -10692,7 +10698,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="120" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>744</v>
       </c>
@@ -10788,7 +10794,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>755</v>
       </c>
@@ -10820,7 +10826,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>759</v>
       </c>
@@ -10875,7 +10881,7 @@
         <v>766</v>
       </c>
       <c r="H94" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I94" s="2" t="b">
         <v>0</v>
@@ -10916,7 +10922,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>768</v>
       </c>
@@ -10948,7 +10954,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>771</v>
       </c>
@@ -10980,7 +10986,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>775</v>
       </c>
@@ -11012,7 +11018,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>779</v>
       </c>
@@ -11108,7 +11114,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>791</v>
       </c>
@@ -11140,7 +11146,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>795</v>
       </c>
@@ -11268,7 +11274,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>811</v>
       </c>
@@ -11300,7 +11306,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>815</v>
       </c>
@@ -11332,7 +11338,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>819</v>
       </c>
@@ -11364,7 +11370,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>823</v>
       </c>
@@ -11396,7 +11402,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>827</v>
       </c>
@@ -11489,7 +11495,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11547,7 +11553,7 @@
       </c>
       <c r="B3">
         <f>COUNTIF(Table2[Implement],"=TRUE")</f>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C3">
         <f>COUNTIF(Table2[Player.json],"=TRUE")</f>
@@ -11555,7 +11561,7 @@
       </c>
       <c r="D3">
         <f>COUNTIF(Table2[Implement],"=FALSE")</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3">
         <f>ROWS(Table2[Implement])</f>
@@ -11563,7 +11569,7 @@
       </c>
       <c r="F3" s="9">
         <f t="shared" ref="F3:F4" si="0">B3/E3</f>
-        <v>0.55454545454545456</v>
+        <v>0.5636363636363636</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -11572,7 +11578,7 @@
       </c>
       <c r="B4">
         <f>B3+B2</f>
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:E4" si="1">C3+C2</f>
@@ -11580,7 +11586,7 @@
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
@@ -11588,7 +11594,7 @@
       </c>
       <c r="F4" s="9">
         <f t="shared" si="0"/>
-        <v>0.52340425531914891</v>
+        <v>0.52765957446808509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding some "Slackville" challenges.
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549FAAA4-F8E9-452A-AA59-3054B305C9F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832BBFC8-A2C8-4D76-8F69-D0C14CC53C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="1" r:id="rId1"/>
     <sheet name="Advancements" sheetId="2" r:id="rId2"/>
-    <sheet name="Statistics" sheetId="3" r:id="rId3"/>
+    <sheet name="Challenges" sheetId="4" r:id="rId3"/>
+    <sheet name="Statistics" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="898">
   <si>
     <t>Display Only Text</t>
   </si>
@@ -2545,6 +2546,177 @@
   </si>
   <si>
     <t>Both</t>
+  </si>
+  <si>
+    <t>Kill a mob with a pork chop</t>
+  </si>
+  <si>
+    <t>Slackville</t>
+  </si>
+  <si>
+    <t>slackvill1</t>
+  </si>
+  <si>
+    <t>Beef Slap</t>
+  </si>
+  <si>
+    <t>Kill a mob with a cooked beef</t>
+  </si>
+  <si>
+    <t>BeefSlap</t>
+  </si>
+  <si>
+    <t>Hatter Vaction Home</t>
+  </si>
+  <si>
+    <t>Die in the end in the viod</t>
+  </si>
+  <si>
+    <t>HattersVacationHome</t>
+  </si>
+  <si>
+    <t>Why Gypsy</t>
+  </si>
+  <si>
+    <t>Kill a Tamed Horse</t>
+  </si>
+  <si>
+    <t>WhyGypsy</t>
+  </si>
+  <si>
+    <t>You Too Radar?</t>
+  </si>
+  <si>
+    <t>Kill A named Horse</t>
+  </si>
+  <si>
+    <t>YouTooRadar</t>
+  </si>
+  <si>
+    <t>At Least it wasn’t Skyblock</t>
+  </si>
+  <si>
+    <t>Be Killed By a Dolphin.</t>
+  </si>
+  <si>
+    <t>AtLeastItWasntSkyblock</t>
+  </si>
+  <si>
+    <t>Its Color not Colour</t>
+  </si>
+  <si>
+    <t>Get all 16 Dyes</t>
+  </si>
+  <si>
+    <t>ItsColorNotColour</t>
+  </si>
+  <si>
+    <t>Obtain a Wither Rose</t>
+  </si>
+  <si>
+    <t>Place Slime at Build Height</t>
+  </si>
+  <si>
+    <t>No More Traders</t>
+  </si>
+  <si>
+    <t>Tman's Black Dye</t>
+  </si>
+  <si>
+    <t>TmansBlackDye</t>
+  </si>
+  <si>
+    <t>No Really How did we get here</t>
+  </si>
+  <si>
+    <t>Have 20 vindicators within 16 blocks of the player</t>
+  </si>
+  <si>
+    <t>NoReallyHowDidWeGetHere</t>
+  </si>
+  <si>
+    <t>Now That, That is a gold farm</t>
+  </si>
+  <si>
+    <t>Place 42,000 magma blocks</t>
+  </si>
+  <si>
+    <t>NowThatThatIsAGoldFarm</t>
+  </si>
+  <si>
+    <t>Just Getting Started</t>
+  </si>
+  <si>
+    <t>Break 1,000,000 Blocks</t>
+  </si>
+  <si>
+    <t>Tman Armor</t>
+  </si>
+  <si>
+    <t>swim in lava for 5 minutes Without dying (fire protection on everything)</t>
+  </si>
+  <si>
+    <t>TmanArmor</t>
+  </si>
+  <si>
+    <t>Red Sheep</t>
+  </si>
+  <si>
+    <t>Dye a sheep red</t>
+  </si>
+  <si>
+    <t>RedSheep</t>
+  </si>
+  <si>
+    <t>Debts to be settled</t>
+  </si>
+  <si>
+    <t>Did you loose a bet tman?</t>
+  </si>
+  <si>
+    <t>Debtstobesettled</t>
+  </si>
+  <si>
+    <t>Run Slack Run</t>
+  </si>
+  <si>
+    <t>Summon a Wither</t>
+  </si>
+  <si>
+    <t>RunSlackRun</t>
+  </si>
+  <si>
+    <t>Plick is that you</t>
+  </si>
+  <si>
+    <t>Place 1,000,000 gravel</t>
+  </si>
+  <si>
+    <t>PlickIsThatYou</t>
+  </si>
+  <si>
+    <t>Day one Guardian Farm</t>
+  </si>
+  <si>
+    <t>Kill a guardian with no diamond gear</t>
+  </si>
+  <si>
+    <t>DayOneGuardianFarm</t>
+  </si>
+  <si>
+    <t>Structura</t>
+  </si>
+  <si>
+    <t>Name tag an armorstand</t>
+  </si>
+  <si>
+    <t>Day one Wither</t>
+  </si>
+  <si>
+    <t>Kill a wither with no beacon effects and no diamond gear</t>
+  </si>
+  <si>
+    <t>DayOneWither</t>
   </si>
 </sst>
 </file>
@@ -2554,7 +2726,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2592,16 +2764,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2609,12 +2805,70 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF9BC2E6"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF9BC2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF9BC2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2639,12 +2893,295 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="74">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2942,23 +3479,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:K127" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:K127" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
   <autoFilter ref="A2:K127" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J127">
     <sortCondition ref="J2:J127"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Achievment" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="In-game description" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Actual requirements (if different)" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Category" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Property Name" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Index" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Achievement (English Title)" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Implement" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Player.json" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sort Order" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column1" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Achievment" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="In-game description" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Actual requirements (if different)" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Category" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Property Name" dataDxfId="67"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Index" dataDxfId="66"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Achievement (English Title)" dataDxfId="65"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Implement" dataDxfId="64"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Player.json" dataDxfId="63"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sort Order" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column1" dataDxfId="61">
       <calculatedColumnFormula>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2967,22 +3504,43 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:J112" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:J112" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="A2:J112" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J112">
     <sortCondition ref="J2:J112"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Advancement" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="In-game description" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Actual requirements (if different)" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Category" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Property Name" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Index" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Advancement (English Title)" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Implement" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Player.json" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Sort Order" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Advancement" dataDxfId="58"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="In-game description" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Actual requirements (if different)" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Category" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Property Name" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Index" dataDxfId="53"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Advancement (English Title)" dataDxfId="52"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Implement" dataDxfId="51"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Player.json" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Sort Order" dataDxfId="49"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE12FC0E-4709-4C73-B5B1-A169ACDBA6CE}" name="Table3" displayName="Table3" ref="A2:J22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:J22" xr:uid="{DE12FC0E-4709-4C73-B5B1-A169ACDBA6CE}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{8A34E490-4B28-46A5-A4B0-AA9721A0B999}" name="Advancement" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{240DE560-2643-41B9-93AE-AD1D0B88670F}" name="In-game description" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{C9EBD348-EFEF-45E4-B948-8938B27250F0}" name="Actual requirements (if different)" dataDxfId="8">
+      <calculatedColumnFormula>Table3[[#This Row],[In-game description]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{9DFAE2BC-F7A2-4E66-90D3-F7DEEBB0B980}" name="Category" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{C0BC5EC9-9291-4522-9534-16D631CD7152}" name="Property Name" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{7DDCB0E6-93DB-429A-AB2F-32609D87D9F6}" name="Index" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{771A1498-3C80-4E7A-8546-D022BD7155E4}" name="Advancement (English Title)" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{FAE293DB-7B8C-4B07-A5E0-F90A7FFAEF84}" name="Implement" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{F2787C17-E8A3-485F-9265-F0C2BFC9FAB1}" name="Player.json" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{785A3721-274D-4362-BD30-E3B0A3260CA8}" name="Sort Order" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3254,24 +3812,24 @@
   <dimension ref="A1:M127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.59765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.59765625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="50.59765625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="15.59765625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="35.59765625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.59765625" style="3" customWidth="1"/>
-    <col min="9" max="10" width="15.59765625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="35.59765625" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="50.59765625" style="4"/>
+    <col min="1" max="1" width="35.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="3" customWidth="1"/>
+    <col min="9" max="10" width="15.5703125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="35.5703125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="50.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3287,7 +3845,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3326,7 +3884,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -3366,7 +3924,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -3402,7 +3960,7 @@
         <v>Story12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -3438,7 +3996,7 @@
         <v>Story13</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -3474,7 +4032,7 @@
         <v>Story14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -3510,7 +4068,7 @@
         <v>Story15</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -3546,7 +4104,7 @@
         <v>Story16</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -3582,7 +4140,7 @@
         <v>Husbandry11</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -3618,7 +4176,7 @@
         <v>Husbandry12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>48</v>
       </c>
@@ -3654,7 +4212,7 @@
         <v>Husbandry13</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
@@ -3690,7 +4248,7 @@
         <v>Story17</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
@@ -3726,7 +4284,7 @@
         <v>Husbandry14</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
@@ -3762,7 +4320,7 @@
         <v>Adventure11</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
@@ -3798,7 +4356,7 @@
         <v>Story18</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>70</v>
       </c>
@@ -3834,7 +4392,7 @@
         <v>Adventure12</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>74</v>
       </c>
@@ -3870,7 +4428,7 @@
         <v>Husbandry15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>78</v>
       </c>
@@ -3906,7 +4464,7 @@
         <v>Adventure13</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
@@ -3942,7 +4500,7 @@
         <v>Adventure14</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>86</v>
       </c>
@@ -3978,7 +4536,7 @@
         <v>Story19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>90</v>
       </c>
@@ -4014,7 +4572,7 @@
         <v>Nether11</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>96</v>
       </c>
@@ -4050,7 +4608,7 @@
         <v>Nether12</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>100</v>
       </c>
@@ -4086,7 +4644,7 @@
         <v>Nether13</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>104</v>
       </c>
@@ -4122,7 +4680,7 @@
         <v>Nether14</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>108</v>
       </c>
@@ -4158,7 +4716,7 @@
         <v>The_End11</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>114</v>
       </c>
@@ -4194,7 +4752,7 @@
         <v>The_End12</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>117</v>
       </c>
@@ -4230,7 +4788,7 @@
         <v>Story110</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>120</v>
       </c>
@@ -4266,7 +4824,7 @@
         <v>Adventure15</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>123</v>
       </c>
@@ -4302,7 +4860,7 @@
         <v>Adventure16</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>126</v>
       </c>
@@ -4338,7 +4896,7 @@
         <v>Adventure17</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>130</v>
       </c>
@@ -4374,7 +4932,7 @@
         <v>Nether15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>134</v>
       </c>
@@ -4410,7 +4968,7 @@
         <v>Nether16</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>137</v>
       </c>
@@ -4446,7 +5004,7 @@
         <v>Nether17</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>141</v>
       </c>
@@ -4482,7 +5040,7 @@
         <v>Husbandry17</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>144</v>
       </c>
@@ -4518,7 +5076,7 @@
         <v>Story111</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>148</v>
       </c>
@@ -4554,7 +5112,7 @@
         <v>Story112</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>151</v>
       </c>
@@ -4590,7 +5148,7 @@
         <v>Story113</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>155</v>
       </c>
@@ -4626,7 +5184,7 @@
         <v>Story114</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>158</v>
       </c>
@@ -4662,7 +5220,7 @@
         <v>Husbandry16</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>162</v>
       </c>
@@ -4698,7 +5256,7 @@
         <v>Husbandry18</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>165</v>
       </c>
@@ -4734,7 +5292,7 @@
         <v>Adventure18</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>169</v>
       </c>
@@ -4770,7 +5328,7 @@
         <v>Story115</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>172</v>
       </c>
@@ -4806,7 +5364,7 @@
         <v>Story116</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>175</v>
       </c>
@@ -4842,7 +5400,7 @@
         <v>Story117</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>178</v>
       </c>
@@ -4878,7 +5436,7 @@
         <v>Adventure19</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>182</v>
       </c>
@@ -4914,7 +5472,7 @@
         <v>Husbandry19</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>185</v>
       </c>
@@ -4950,7 +5508,7 @@
         <v>Husbandry110</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>189</v>
       </c>
@@ -4986,7 +5544,7 @@
         <v>Adventure110</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>192</v>
       </c>
@@ -5022,7 +5580,7 @@
         <v>Story118</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>196</v>
       </c>
@@ -5058,7 +5616,7 @@
         <v>Story119</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>200</v>
       </c>
@@ -5094,7 +5652,7 @@
         <v>Husbandry111</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>203</v>
       </c>
@@ -5130,7 +5688,7 @@
         <v>Story120</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>206</v>
       </c>
@@ -5166,7 +5724,7 @@
         <v>Husbandry112</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>210</v>
       </c>
@@ -5202,7 +5760,7 @@
         <v>Husbandry113</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>213</v>
       </c>
@@ -5238,7 +5796,7 @@
         <v>Adventure111</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>215</v>
       </c>
@@ -5274,7 +5832,7 @@
         <v>Story121</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>218</v>
       </c>
@@ -5310,7 +5868,7 @@
         <v>Adventure112</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>220</v>
       </c>
@@ -5346,7 +5904,7 @@
         <v>Adventure113</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>222</v>
       </c>
@@ -5382,7 +5940,7 @@
         <v>Story122</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>226</v>
       </c>
@@ -5418,7 +5976,7 @@
         <v>Story123</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>229</v>
       </c>
@@ -5454,7 +6012,7 @@
         <v>Story124</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>233</v>
       </c>
@@ -5490,7 +6048,7 @@
         <v>Adventure114</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>237</v>
       </c>
@@ -5526,7 +6084,7 @@
         <v>Story125</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>239</v>
       </c>
@@ -5562,7 +6120,7 @@
         <v>Husbandry114</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>242</v>
       </c>
@@ -5598,7 +6156,7 @@
         <v>Husbandry115</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>245</v>
       </c>
@@ -5634,7 +6192,7 @@
         <v>Adventure115</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>249</v>
       </c>
@@ -5670,7 +6228,7 @@
         <v>Husbandry116</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>252</v>
       </c>
@@ -5706,7 +6264,7 @@
         <v>Adventure116</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>255</v>
       </c>
@@ -5742,7 +6300,7 @@
         <v>Story126</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>258</v>
       </c>
@@ -5778,7 +6336,7 @@
         <v>Story127</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>261</v>
       </c>
@@ -5814,7 +6372,7 @@
         <v>The_End13</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>265</v>
       </c>
@@ -5850,7 +6408,7 @@
         <v>Nether18</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>269</v>
       </c>
@@ -5886,7 +6444,7 @@
         <v>The_End14</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>272</v>
       </c>
@@ -5922,7 +6480,7 @@
         <v>The_End15</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>275</v>
       </c>
@@ -5958,7 +6516,7 @@
         <v>The_End16</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>278</v>
       </c>
@@ -5994,7 +6552,7 @@
         <v>Adventure117</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>282</v>
       </c>
@@ -6030,7 +6588,7 @@
         <v>The_End17</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>285</v>
       </c>
@@ -6066,7 +6624,7 @@
         <v>Adventure118</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>289</v>
       </c>
@@ -6102,7 +6660,7 @@
         <v>Adventure119</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>292</v>
       </c>
@@ -6138,7 +6696,7 @@
         <v>Adventure120</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>295</v>
       </c>
@@ -6174,7 +6732,7 @@
         <v>Husbandry117</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>298</v>
       </c>
@@ -6210,7 +6768,7 @@
         <v>Adventure121</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>301</v>
       </c>
@@ -6246,7 +6804,7 @@
         <v>Adventure122</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>305</v>
       </c>
@@ -6282,7 +6840,7 @@
         <v>Adventure123</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>308</v>
       </c>
@@ -6318,7 +6876,7 @@
         <v>Adventure124</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>311</v>
       </c>
@@ -6354,7 +6912,7 @@
         <v>Husbandry118</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>315</v>
       </c>
@@ -6390,7 +6948,7 @@
         <v>Adventure125</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>319</v>
       </c>
@@ -6426,7 +6984,7 @@
         <v>Adventure126</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>323</v>
       </c>
@@ -6462,7 +7020,7 @@
         <v>Story128</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>327</v>
       </c>
@@ -6498,7 +7056,7 @@
         <v>Adventure127</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>331</v>
       </c>
@@ -6534,7 +7092,7 @@
         <v>Story129</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>334</v>
       </c>
@@ -6570,7 +7128,7 @@
         <v>Adventure128</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>337</v>
       </c>
@@ -6606,7 +7164,7 @@
         <v>Story130</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>340</v>
       </c>
@@ -6642,7 +7200,7 @@
         <v>Story131</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>344</v>
       </c>
@@ -6678,7 +7236,7 @@
         <v>Husbandry119</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>348</v>
       </c>
@@ -6714,7 +7272,7 @@
         <v>Husbandry120</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>350</v>
       </c>
@@ -6750,7 +7308,7 @@
         <v>Story132</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>354</v>
       </c>
@@ -6786,7 +7344,7 @@
         <v>Husbandry121</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>358</v>
       </c>
@@ -6822,7 +7380,7 @@
         <v>Adventure129</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>361</v>
       </c>
@@ -6858,7 +7416,7 @@
         <v>Story21</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>366</v>
       </c>
@@ -6894,7 +7452,7 @@
         <v>Story22</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>368</v>
       </c>
@@ -6930,7 +7488,7 @@
         <v>Adventure130</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>372</v>
       </c>
@@ -6966,7 +7524,7 @@
         <v>Story23</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>375</v>
       </c>
@@ -7002,7 +7560,7 @@
         <v>Adventure131</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>378</v>
       </c>
@@ -7038,7 +7596,7 @@
         <v>Story24</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>382</v>
       </c>
@@ -7074,7 +7632,7 @@
         <v>Story25</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>385</v>
       </c>
@@ -7110,7 +7668,7 @@
         <v>Husbandry122</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>388</v>
       </c>
@@ -7146,7 +7704,7 @@
         <v>Husbandry123</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>391</v>
       </c>
@@ -7182,7 +7740,7 @@
         <v>Story26</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>394</v>
       </c>
@@ -7218,7 +7776,7 @@
         <v>Story27</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>396</v>
       </c>
@@ -7254,7 +7812,7 @@
         <v>Nether19</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>400</v>
       </c>
@@ -7290,7 +7848,7 @@
         <v>Nether110</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>404</v>
       </c>
@@ -7326,7 +7884,7 @@
         <v>Nether111</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>408</v>
       </c>
@@ -7362,7 +7920,7 @@
         <v>Adventure132</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>412</v>
       </c>
@@ -7398,7 +7956,7 @@
         <v>Story28</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>416</v>
       </c>
@@ -7434,7 +7992,7 @@
         <v>Husbandry124</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>420</v>
       </c>
@@ -7470,7 +8028,7 @@
         <v>Story29</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>423</v>
       </c>
@@ -7506,7 +8064,7 @@
         <v>Story210</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>427</v>
       </c>
@@ -7542,7 +8100,7 @@
         <v>Story211</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>431</v>
       </c>
@@ -7578,7 +8136,7 @@
         <v>Nether112</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>435</v>
       </c>
@@ -7614,7 +8172,7 @@
         <v>Story212</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>438</v>
       </c>
@@ -7650,7 +8208,7 @@
         <v>Husbandry125</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>442</v>
       </c>
@@ -7686,7 +8244,7 @@
         <v>Nether113</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>446</v>
       </c>
@@ -7722,7 +8280,7 @@
         <v>Story213</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>450</v>
       </c>
@@ -7758,7 +8316,7 @@
         <v>Story214</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>453</v>
       </c>
@@ -7794,7 +8352,7 @@
         <v>Story215</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>456</v>
       </c>
@@ -7832,18 +8390,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:K1048576">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="48" priority="3">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="47" priority="4">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="46" priority="5">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I127" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -7861,26 +8419,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.59765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.59765625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="50.59765625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="15.59765625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.59765625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="35.59765625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.59765625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15.59765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.59765625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="50.59765625" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="50.59765625" style="4"/>
+    <col min="1" max="1" width="35.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.5703125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="50.5703125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="50.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -7902,7 +8460,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>459</v>
       </c>
@@ -7934,7 +8492,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>461</v>
       </c>
@@ -7966,7 +8524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>465</v>
       </c>
@@ -7998,7 +8556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -8030,7 +8588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -8062,7 +8620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>473</v>
       </c>
@@ -8094,7 +8652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>477</v>
       </c>
@@ -8126,7 +8684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>481</v>
       </c>
@@ -8158,7 +8716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>485</v>
       </c>
@@ -8190,7 +8748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>489</v>
       </c>
@@ -8222,7 +8780,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>493</v>
       </c>
@@ -8254,7 +8812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>497</v>
       </c>
@@ -8286,7 +8844,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>501</v>
       </c>
@@ -8318,7 +8876,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>117</v>
       </c>
@@ -8350,7 +8908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>206</v>
       </c>
@@ -8382,7 +8940,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>509</v>
       </c>
@@ -8414,7 +8972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>108</v>
       </c>
@@ -8446,7 +9004,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>93</v>
       </c>
@@ -8478,7 +9036,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>96</v>
       </c>
@@ -8510,7 +9068,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>519</v>
       </c>
@@ -8542,7 +9100,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>522</v>
       </c>
@@ -8574,7 +9132,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>526</v>
       </c>
@@ -8606,7 +9164,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>530</v>
       </c>
@@ -8638,7 +9196,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>534</v>
       </c>
@@ -8670,7 +9228,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>538</v>
       </c>
@@ -8702,7 +9260,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>542</v>
       </c>
@@ -8734,7 +9292,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>546</v>
       </c>
@@ -8766,7 +9324,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>550</v>
       </c>
@@ -8798,7 +9356,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>554</v>
       </c>
@@ -8830,7 +9388,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>557</v>
       </c>
@@ -8862,7 +9420,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>561</v>
       </c>
@@ -8894,7 +9452,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>100</v>
       </c>
@@ -8926,7 +9484,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>567</v>
       </c>
@@ -8958,7 +9516,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>431</v>
       </c>
@@ -8990,7 +9548,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>572</v>
       </c>
@@ -9022,7 +9580,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>576</v>
       </c>
@@ -9054,7 +9612,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>104</v>
       </c>
@@ -9086,7 +9644,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>582</v>
       </c>
@@ -9118,7 +9676,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>586</v>
       </c>
@@ -9150,7 +9708,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>590</v>
       </c>
@@ -9182,7 +9740,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>593</v>
       </c>
@@ -9214,7 +9772,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>114</v>
       </c>
@@ -9246,7 +9804,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>599</v>
       </c>
@@ -9278,7 +9836,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>603</v>
       </c>
@@ -9310,7 +9868,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>607</v>
       </c>
@@ -9342,7 +9900,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>269</v>
       </c>
@@ -9374,7 +9932,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>261</v>
       </c>
@@ -9406,7 +9964,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>615</v>
       </c>
@@ -9438,7 +9996,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>619</v>
       </c>
@@ -9470,7 +10028,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>272</v>
       </c>
@@ -9502,7 +10060,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>64</v>
       </c>
@@ -9534,7 +10092,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>627</v>
       </c>
@@ -9566,7 +10124,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>631</v>
       </c>
@@ -9598,7 +10156,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>70</v>
       </c>
@@ -9630,7 +10188,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>636</v>
       </c>
@@ -9662,7 +10220,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>640</v>
       </c>
@@ -9694,7 +10252,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>644</v>
       </c>
@@ -9726,7 +10284,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>391</v>
       </c>
@@ -9758,7 +10316,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>649</v>
       </c>
@@ -9790,7 +10348,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>652</v>
       </c>
@@ -9822,7 +10380,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>420</v>
       </c>
@@ -9854,7 +10412,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>658</v>
       </c>
@@ -9886,7 +10444,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>446</v>
       </c>
@@ -9918,7 +10476,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>663</v>
       </c>
@@ -9950,7 +10508,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>667</v>
       </c>
@@ -9982,7 +10540,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>671</v>
       </c>
@@ -10014,7 +10572,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>675</v>
       </c>
@@ -10046,7 +10604,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>679</v>
       </c>
@@ -10078,7 +10636,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>683</v>
       </c>
@@ -10110,7 +10668,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>687</v>
       </c>
@@ -10142,7 +10700,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>691</v>
       </c>
@@ -10174,7 +10732,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>694</v>
       </c>
@@ -10206,7 +10764,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>698</v>
       </c>
@@ -10238,7 +10796,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>702</v>
       </c>
@@ -10270,7 +10828,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>704</v>
       </c>
@@ -10302,7 +10860,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>708</v>
       </c>
@@ -10334,7 +10892,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>712</v>
       </c>
@@ -10366,7 +10924,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>715</v>
       </c>
@@ -10398,7 +10956,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="285" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:10" ht="285" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>126</v>
       </c>
@@ -10430,7 +10988,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>427</v>
       </c>
@@ -10462,7 +11020,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>721</v>
       </c>
@@ -10494,7 +11052,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>725</v>
       </c>
@@ -10526,7 +11084,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>728</v>
       </c>
@@ -10558,7 +11116,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>82</v>
       </c>
@@ -10590,7 +11148,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>394</v>
       </c>
@@ -10622,7 +11180,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>41</v>
       </c>
@@ -10654,7 +11212,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>740</v>
       </c>
@@ -10686,7 +11244,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>744</v>
       </c>
@@ -10718,7 +11276,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>748</v>
       </c>
@@ -10750,7 +11308,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>752</v>
       </c>
@@ -10782,7 +11340,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>755</v>
       </c>
@@ -10814,7 +11372,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>759</v>
       </c>
@@ -10846,7 +11404,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>763</v>
       </c>
@@ -10878,7 +11436,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>388</v>
       </c>
@@ -10910,7 +11468,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>768</v>
       </c>
@@ -10942,7 +11500,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>771</v>
       </c>
@@ -10974,7 +11532,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>775</v>
       </c>
@@ -11006,7 +11564,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>779</v>
       </c>
@@ -11038,7 +11596,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>783</v>
       </c>
@@ -11070,7 +11628,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>787</v>
       </c>
@@ -11102,7 +11660,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>791</v>
       </c>
@@ -11134,7 +11692,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>795</v>
       </c>
@@ -11166,7 +11724,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>799</v>
       </c>
@@ -11198,7 +11756,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>803</v>
       </c>
@@ -11230,7 +11788,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="195" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:10" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>807</v>
       </c>
@@ -11262,7 +11820,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>811</v>
       </c>
@@ -11294,7 +11852,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>815</v>
       </c>
@@ -11326,7 +11884,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>819</v>
       </c>
@@ -11358,7 +11916,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>823</v>
       </c>
@@ -11390,7 +11948,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>827</v>
       </c>
@@ -11422,7 +11980,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>416</v>
       </c>
@@ -11456,13 +12014,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:J1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="44" priority="1">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="43" priority="2">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="42" priority="3">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11479,21 +12037,1303 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A114CABE-4723-471F-81B1-1F98BAE7D3E1}">
+  <dimension ref="A1:N127"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" style="22" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" style="3" customWidth="1"/>
+    <col min="9" max="10" width="15.5703125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="8" t="str">
+        <f>CONCATENATE("Complete: ",COUNTIF(Table3[Implement],"=TRUE"),"/",ROWS(Table3[Implement]))</f>
+        <v>Complete: 0/20</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Kill a mob with a pork chop</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Kill a mob with a cooked beef</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="H4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>848</v>
+      </c>
+      <c r="C5" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Die in the end in the viod</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="H5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>851</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Kill a Tamed Horse</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="H6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>854</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Kill A named Horse</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="H7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>857</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Be Killed By a Dolphin.</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F8" s="2">
+        <v>6</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="H8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="C9" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Get all 16 Dyes</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F9" s="2">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="H9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>862</v>
+      </c>
+      <c r="C10" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Obtain a Wither Rose</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F10" s="2">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="H10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>863</v>
+      </c>
+      <c r="C11" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Place Slime at Build Height</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F11" s="2">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="H11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="C12" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Have 20 vindicators within 16 blocks of the player</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F12" s="2">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="H12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>870</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>871</v>
+      </c>
+      <c r="C13" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Place 42,000 magma blocks</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F13" s="2">
+        <v>11</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="H13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>874</v>
+      </c>
+      <c r="C14" s="4" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Break 1,000,000 Blocks</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F14" s="2">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="H14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>875</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>876</v>
+      </c>
+      <c r="C15" s="15" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>swim in lava for 5 minutes Without dying (fire protection on everything)</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>842</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>843</v>
+      </c>
+      <c r="F15" s="16">
+        <v>13</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>877</v>
+      </c>
+      <c r="H15" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>878</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>879</v>
+      </c>
+      <c r="C16" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Dye a sheep red</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F16" s="2">
+        <v>14</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="H16" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>881</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>882</v>
+      </c>
+      <c r="C17" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Did you loose a bet tman?</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F17" s="2">
+        <v>15</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>883</v>
+      </c>
+      <c r="H17" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>884</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>885</v>
+      </c>
+      <c r="C18" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Summon a Wither</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F18" s="2">
+        <v>16</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>886</v>
+      </c>
+      <c r="H18" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13" t="s">
+        <v>887</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>888</v>
+      </c>
+      <c r="C19" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Place 1,000,000 gravel</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F19" s="2">
+        <v>17</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>889</v>
+      </c>
+      <c r="H19" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>890</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>891</v>
+      </c>
+      <c r="C20" s="15" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Kill a guardian with no diamond gear</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>842</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>843</v>
+      </c>
+      <c r="F20" s="16">
+        <v>18</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>892</v>
+      </c>
+      <c r="H20" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>893</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>894</v>
+      </c>
+      <c r="C21" s="15" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Name tag an armorstand</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>842</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>843</v>
+      </c>
+      <c r="F21" s="16">
+        <v>19</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>893</v>
+      </c>
+      <c r="H21" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" s="17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="15"/>
+      <c r="B22" s="24" t="s">
+        <v>895</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>896</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>842</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>843</v>
+      </c>
+      <c r="F22" s="16">
+        <v>20</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>897</v>
+      </c>
+      <c r="H22" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="3"/>
+    </row>
+    <row r="45" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="3"/>
+    </row>
+    <row r="46" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="3"/>
+    </row>
+    <row r="47" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="3"/>
+    </row>
+    <row r="48" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="3"/>
+    </row>
+    <row r="49" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="3"/>
+    </row>
+    <row r="50" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="3"/>
+    </row>
+    <row r="52" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="3"/>
+    </row>
+    <row r="54" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="3"/>
+    </row>
+    <row r="55" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="3"/>
+    </row>
+    <row r="56" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="3"/>
+    </row>
+    <row r="57" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="3"/>
+    </row>
+    <row r="58" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="3"/>
+    </row>
+    <row r="59" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="3"/>
+    </row>
+    <row r="60" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="3"/>
+    </row>
+    <row r="62" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="3"/>
+    </row>
+    <row r="63" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="3"/>
+    </row>
+    <row r="64" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="3"/>
+    </row>
+    <row r="65" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="3"/>
+    </row>
+    <row r="66" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="3"/>
+    </row>
+    <row r="67" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="3"/>
+    </row>
+    <row r="68" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="3"/>
+    </row>
+    <row r="69" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H69" s="2"/>
+      <c r="I69" s="2"/>
+      <c r="J69" s="3"/>
+    </row>
+    <row r="70" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="3"/>
+    </row>
+    <row r="71" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="3"/>
+    </row>
+    <row r="72" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H72" s="2"/>
+      <c r="I72" s="2"/>
+      <c r="J72" s="3"/>
+    </row>
+    <row r="73" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="3"/>
+    </row>
+    <row r="74" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="3"/>
+    </row>
+    <row r="75" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="3"/>
+    </row>
+    <row r="76" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="3"/>
+    </row>
+    <row r="77" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="3"/>
+    </row>
+    <row r="78" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="3"/>
+    </row>
+    <row r="79" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+      <c r="J79" s="3"/>
+    </row>
+    <row r="80" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="3"/>
+    </row>
+    <row r="81" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="3"/>
+    </row>
+    <row r="82" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="3"/>
+    </row>
+    <row r="83" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="3"/>
+    </row>
+    <row r="84" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="3"/>
+    </row>
+    <row r="85" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="3"/>
+    </row>
+    <row r="86" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H86" s="2"/>
+      <c r="I86" s="2"/>
+      <c r="J86" s="3"/>
+    </row>
+    <row r="87" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H87" s="2"/>
+      <c r="I87" s="2"/>
+      <c r="J87" s="3"/>
+    </row>
+    <row r="88" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+      <c r="J88" s="3"/>
+    </row>
+    <row r="89" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H89" s="2"/>
+      <c r="I89" s="2"/>
+      <c r="J89" s="3"/>
+    </row>
+    <row r="90" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H90" s="2"/>
+      <c r="I90" s="2"/>
+      <c r="J90" s="3"/>
+    </row>
+    <row r="91" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="3"/>
+    </row>
+    <row r="92" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H92" s="2"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="3"/>
+    </row>
+    <row r="93" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H93" s="2"/>
+      <c r="I93" s="2"/>
+      <c r="J93" s="3"/>
+    </row>
+    <row r="94" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H94" s="2"/>
+      <c r="I94" s="2"/>
+      <c r="J94" s="3"/>
+    </row>
+    <row r="95" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H95" s="2"/>
+      <c r="I95" s="2"/>
+      <c r="J95" s="3"/>
+    </row>
+    <row r="96" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H96" s="2"/>
+      <c r="I96" s="2"/>
+      <c r="J96" s="3"/>
+    </row>
+    <row r="97" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H97" s="2"/>
+      <c r="I97" s="2"/>
+      <c r="J97" s="3"/>
+    </row>
+    <row r="98" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+      <c r="J98" s="3"/>
+    </row>
+    <row r="99" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H99" s="2"/>
+      <c r="I99" s="2"/>
+      <c r="J99" s="3"/>
+    </row>
+    <row r="100" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H100" s="2"/>
+      <c r="I100" s="2"/>
+      <c r="J100" s="3"/>
+    </row>
+    <row r="101" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H101" s="2"/>
+      <c r="I101" s="2"/>
+      <c r="J101" s="3"/>
+    </row>
+    <row r="102" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="3"/>
+    </row>
+    <row r="103" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H103" s="2"/>
+      <c r="I103" s="2"/>
+      <c r="J103" s="3"/>
+    </row>
+    <row r="104" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H104" s="2"/>
+      <c r="I104" s="2"/>
+      <c r="J104" s="3"/>
+    </row>
+    <row r="105" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H105" s="2"/>
+      <c r="I105" s="2"/>
+      <c r="J105" s="3"/>
+    </row>
+    <row r="106" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H106" s="2"/>
+      <c r="I106" s="2"/>
+      <c r="J106" s="3"/>
+    </row>
+    <row r="107" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H107" s="2"/>
+      <c r="I107" s="2"/>
+      <c r="J107" s="3"/>
+    </row>
+    <row r="108" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H108" s="2"/>
+      <c r="I108" s="2"/>
+      <c r="J108" s="3"/>
+    </row>
+    <row r="109" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H109" s="2"/>
+      <c r="I109" s="2"/>
+      <c r="J109" s="3"/>
+    </row>
+    <row r="110" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H110" s="2"/>
+      <c r="I110" s="2"/>
+      <c r="J110" s="3"/>
+    </row>
+    <row r="111" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H111" s="2"/>
+      <c r="I111" s="2"/>
+      <c r="J111" s="3"/>
+    </row>
+    <row r="112" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="3"/>
+    </row>
+    <row r="113" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="J113" s="3"/>
+    </row>
+    <row r="114" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="3"/>
+    </row>
+    <row r="115" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="3"/>
+    </row>
+    <row r="116" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="3"/>
+    </row>
+    <row r="117" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="3"/>
+    </row>
+    <row r="118" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+      <c r="J118" s="3"/>
+    </row>
+    <row r="119" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
+      <c r="J119" s="3"/>
+    </row>
+    <row r="120" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+      <c r="J120" s="3"/>
+    </row>
+    <row r="121" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+      <c r="J121" s="3"/>
+    </row>
+    <row r="122" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
+      <c r="J122" s="3"/>
+    </row>
+    <row r="123" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+      <c r="J123" s="3"/>
+    </row>
+    <row r="124" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+      <c r="J124" s="3"/>
+    </row>
+    <row r="125" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+      <c r="J125" s="3"/>
+    </row>
+    <row r="126" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H126" s="2"/>
+      <c r="I126" s="2"/>
+      <c r="J126" s="3"/>
+    </row>
+    <row r="127" spans="8:10" x14ac:dyDescent="0.25">
+      <c r="H127" s="2"/>
+      <c r="I127" s="2"/>
+      <c r="J127" s="3"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:J15 E17:F20 E16:G16 H16:J20 E21:J21 E23:J1048576 E22:F22 H22:J22">
+    <cfRule type="expression" dxfId="14" priority="1">
+      <formula>ROW()=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="2">
+      <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="3">
+      <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I22" xr:uid="{889EB968-2309-4054-9531-83439D0DAB8B}">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03723C66-8E0B-48F3-9CF4-1B0F8B736B8C}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>834</v>
       </c>
@@ -11510,7 +13350,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>833</v>
       </c>
@@ -11535,7 +13375,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>838</v>
       </c>
@@ -11560,7 +13400,7 @@
         <v>0.59090909090909094</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>840</v>
       </c>

</xml_diff>

<commit_message>
Added Slackville category challenges.
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832BBFC8-A2C8-4D76-8F69-D0C14CC53C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55046D6-4889-4513-AB00-814DDC8C1450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="898">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="960">
   <si>
     <t>Display Only Text</t>
   </si>
@@ -2717,6 +2717,192 @@
   </si>
   <si>
     <t>DayOneWither</t>
+  </si>
+  <si>
+    <t>Where is Hatter</t>
+  </si>
+  <si>
+    <t>Be killed by friendly fire while you have the wither effect</t>
+  </si>
+  <si>
+    <t>More Dangerous than the wither</t>
+  </si>
+  <si>
+    <t>Kill a player when that player has the wither effect</t>
+  </si>
+  <si>
+    <t>WhereIsHatter</t>
+  </si>
+  <si>
+    <t>MoreDangerousThanTheWither</t>
+  </si>
+  <si>
+    <t>See you in Court</t>
+  </si>
+  <si>
+    <t>Killed by a player when you have no gear on</t>
+  </si>
+  <si>
+    <t>SeeYouInCort</t>
+  </si>
+  <si>
+    <t>charcoal seeds</t>
+  </si>
+  <si>
+    <t>have dark oak log, dark oak saplings and a furnace in your inventory</t>
+  </si>
+  <si>
+    <t>fastest unloader</t>
+  </si>
+  <si>
+    <t>destroy a shulker with fire</t>
+  </si>
+  <si>
+    <t>heafty garbage bag</t>
+  </si>
+  <si>
+    <t>have a shulker that is dyed black</t>
+  </si>
+  <si>
+    <t>Mr-Cheese-less No More</t>
+  </si>
+  <si>
+    <t>Obtain a gold ingot</t>
+  </si>
+  <si>
+    <t>May the cheese be ever in your flavor!</t>
+  </si>
+  <si>
+    <t>Obtain 164 gold blocks</t>
+  </si>
+  <si>
+    <t>Tell them MrFearless Sent You</t>
+  </si>
+  <si>
+    <t>Send a dolphin to the nether</t>
+  </si>
+  <si>
+    <t>It doesn't work like that</t>
+  </si>
+  <si>
+    <t>Water does not belong here.</t>
+  </si>
+  <si>
+    <t>Place water in the nether</t>
+  </si>
+  <si>
+    <t>Spicy Orange Juice</t>
+  </si>
+  <si>
+    <t>Die in lava</t>
+  </si>
+  <si>
+    <t>Die to starvation</t>
+  </si>
+  <si>
+    <t>Ask Jen first</t>
+  </si>
+  <si>
+    <t>Tman Ladder</t>
+  </si>
+  <si>
+    <t>Craft 64 crafting tables</t>
+  </si>
+  <si>
+    <t>Charcoal Cheddar</t>
+  </si>
+  <si>
+    <t>Burn 64 dark oak logs</t>
+  </si>
+  <si>
+    <t>Story Time</t>
+  </si>
+  <si>
+    <t>Jump for 5 minutes or jump 1,000,000 times, whichever can be programmed</t>
+  </si>
+  <si>
+    <t>That Was Easy</t>
+  </si>
+  <si>
+    <t>Have 164 netherite blocks and a beacon in your inventory</t>
+  </si>
+  <si>
+    <t>The BestVille</t>
+  </si>
+  <si>
+    <t>Play for 1 in-game year</t>
+  </si>
+  <si>
+    <t>365 in-game days pass</t>
+  </si>
+  <si>
+    <t>SuperCow Returns</t>
+  </si>
+  <si>
+    <t>Name a cow SuperCow or just name a cow, whichever can be programmed</t>
+  </si>
+  <si>
+    <t>Death of SuperCow</t>
+  </si>
+  <si>
+    <t>Kill a named cow with a bow</t>
+  </si>
+  <si>
+    <t>Punch a Piggy</t>
+  </si>
+  <si>
+    <t>Punch a zombie piglin or a piglin</t>
+  </si>
+  <si>
+    <t>slackvill2</t>
+  </si>
+  <si>
+    <t>CharcoalSeeds</t>
+  </si>
+  <si>
+    <t>FastestUnloader</t>
+  </si>
+  <si>
+    <t>HeaftyGarbageBag</t>
+  </si>
+  <si>
+    <t>MrCheeseLessNoMore</t>
+  </si>
+  <si>
+    <t>MayTheCheeseBeEverInYourFlavor</t>
+  </si>
+  <si>
+    <t>TellThemMrfearlessSentYou</t>
+  </si>
+  <si>
+    <t>ItDoesn'tWorkLikeThat</t>
+  </si>
+  <si>
+    <t>SpicyOrangeJuice</t>
+  </si>
+  <si>
+    <t>TmanLadder</t>
+  </si>
+  <si>
+    <t>CharcoalCheddar</t>
+  </si>
+  <si>
+    <t>StoryTime</t>
+  </si>
+  <si>
+    <t>ThatWasEasy</t>
+  </si>
+  <si>
+    <t>TheBestville</t>
+  </si>
+  <si>
+    <t>SupercowReturns</t>
+  </si>
+  <si>
+    <t>DeathOfSupercow</t>
+  </si>
+  <si>
+    <t>PunchAPiggy</t>
   </si>
 </sst>
 </file>
@@ -2726,7 +2912,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2776,8 +2962,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2793,6 +2991,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2868,7 +3072,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2893,7 +3097,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2906,15 +3109,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2924,20 +3118,48 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="74">
+  <dxfs count="56">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2962,6 +3184,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3011,205 +3236,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3346,6 +3372,27 @@
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -3465,6 +3512,37 @@
       </fill>
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3479,23 +3557,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:K127" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:K127" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="A2:K127" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J127">
     <sortCondition ref="J2:J127"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Achievment" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="In-game description" dataDxfId="70"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Actual requirements (if different)" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Category" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Property Name" dataDxfId="67"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Index" dataDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Achievement (English Title)" dataDxfId="65"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Implement" dataDxfId="64"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Player.json" dataDxfId="63"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sort Order" dataDxfId="62"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column1" dataDxfId="61">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Achievment" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="In-game description" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Actual requirements (if different)" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Category" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Property Name" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Index" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Achievement (English Title)" dataDxfId="43"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Implement" dataDxfId="42"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Player.json" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sort Order" dataDxfId="40"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column1" dataDxfId="39">
       <calculatedColumnFormula>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3504,43 +3582,43 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:J112" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:J112" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A2:J112" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J112">
     <sortCondition ref="J2:J112"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Advancement" dataDxfId="58"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="In-game description" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Actual requirements (if different)" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Category" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Property Name" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Index" dataDxfId="53"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Advancement (English Title)" dataDxfId="52"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Implement" dataDxfId="51"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Player.json" dataDxfId="50"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Sort Order" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Advancement" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="In-game description" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Actual requirements (if different)" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Category" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Property Name" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Index" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Advancement (English Title)" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Implement" dataDxfId="26"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Player.json" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Sort Order" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE12FC0E-4709-4C73-B5B1-A169ACDBA6CE}" name="Table3" displayName="Table3" ref="A2:J22" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A2:J22" xr:uid="{DE12FC0E-4709-4C73-B5B1-A169ACDBA6CE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE12FC0E-4709-4C73-B5B1-A169ACDBA6CE}" name="Table3" displayName="Table3" ref="A2:J42" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A2:J42" xr:uid="{DE12FC0E-4709-4C73-B5B1-A169ACDBA6CE}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8A34E490-4B28-46A5-A4B0-AA9721A0B999}" name="Advancement" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{240DE560-2643-41B9-93AE-AD1D0B88670F}" name="In-game description" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{C9EBD348-EFEF-45E4-B948-8938B27250F0}" name="Actual requirements (if different)" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{8A34E490-4B28-46A5-A4B0-AA9721A0B999}" name="Advancement" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{240DE560-2643-41B9-93AE-AD1D0B88670F}" name="In-game description" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{C9EBD348-EFEF-45E4-B948-8938B27250F0}" name="Actual requirements (if different)" dataDxfId="10">
       <calculatedColumnFormula>Table3[[#This Row],[In-game description]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9DFAE2BC-F7A2-4E66-90D3-F7DEEBB0B980}" name="Category" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{C0BC5EC9-9291-4522-9534-16D631CD7152}" name="Property Name" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{7DDCB0E6-93DB-429A-AB2F-32609D87D9F6}" name="Index" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{771A1498-3C80-4E7A-8546-D022BD7155E4}" name="Advancement (English Title)" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{FAE293DB-7B8C-4B07-A5E0-F90A7FFAEF84}" name="Implement" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{F2787C17-E8A3-485F-9265-F0C2BFC9FAB1}" name="Player.json" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{785A3721-274D-4362-BD30-E3B0A3260CA8}" name="Sort Order" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{9DFAE2BC-F7A2-4E66-90D3-F7DEEBB0B980}" name="Category" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{C0BC5EC9-9291-4522-9534-16D631CD7152}" name="Property Name" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{7DDCB0E6-93DB-429A-AB2F-32609D87D9F6}" name="Index" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{771A1498-3C80-4E7A-8546-D022BD7155E4}" name="Advancement (English Title)" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{FAE293DB-7B8C-4B07-A5E0-F90A7FFAEF84}" name="Implement" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{F2787C17-E8A3-485F-9265-F0C2BFC9FAB1}" name="Player.json" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{785A3721-274D-4362-BD30-E3B0A3260CA8}" name="Sort Order" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8390,18 +8468,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:K1048576">
-    <cfRule type="expression" dxfId="48" priority="3">
+    <cfRule type="expression" dxfId="55" priority="3">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="4">
+    <cfRule type="expression" dxfId="54" priority="4">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="5">
+    <cfRule type="expression" dxfId="53" priority="5">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="duplicateValues" dxfId="45" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I127" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -8419,7 +8497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N112"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -12014,13 +12092,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:J1048576">
-    <cfRule type="expression" dxfId="44" priority="1">
+    <cfRule type="expression" dxfId="38" priority="1">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="2">
+    <cfRule type="expression" dxfId="37" priority="2">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="3">
+    <cfRule type="expression" dxfId="36" priority="3">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12040,14 +12118,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A114CABE-4723-471F-81B1-1F98BAE7D3E1}">
   <dimension ref="A1:N127"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.85546875" customWidth="1"/>
-    <col min="2" max="2" width="49.7109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="49.7109375" customWidth="1"/>
     <col min="3" max="3" width="63.42578125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" style="2" customWidth="1"/>
@@ -12061,7 +12139,6 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="5" t="s">
@@ -12071,7 +12148,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="8" t="str">
         <f>CONCATENATE("Complete: ",COUNTIF(Table3[Implement],"=TRUE"),"/",ROWS(Table3[Implement]))</f>
-        <v>Complete: 0/20</v>
+        <v>Complete: 0/40</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -12442,10 +12519,10 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>870</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="17" t="s">
         <v>871</v>
       </c>
       <c r="C13" s="1" t="str">
@@ -12508,43 +12585,43 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="18" t="s">
         <v>876</v>
       </c>
-      <c r="C15" s="15" t="str">
+      <c r="C15" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>swim in lava for 5 minutes Without dying (fire protection on everything)</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="2" t="s">
         <v>842</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="2" t="s">
         <v>843</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="2">
         <v>13</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="2" t="s">
         <v>877</v>
       </c>
-      <c r="H15" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="17">
+      <c r="H15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>878</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>879</v>
       </c>
       <c r="C16" s="1" t="str">
@@ -12563,10 +12640,10 @@
       <c r="G16" s="2" t="s">
         <v>880</v>
       </c>
-      <c r="H16" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="16" t="b">
+      <c r="H16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J16" s="3">
@@ -12574,10 +12651,10 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>881</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>882</v>
       </c>
       <c r="C17" s="1" t="str">
@@ -12593,13 +12670,13 @@
       <c r="F17" s="2">
         <v>15</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="16" t="s">
         <v>883</v>
       </c>
-      <c r="H17" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="16" t="b">
+      <c r="H17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J17" s="3">
@@ -12607,10 +12684,10 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>884</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>885</v>
       </c>
       <c r="C18" s="1" t="str">
@@ -12626,13 +12703,13 @@
       <c r="F18" s="2">
         <v>16</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="15" t="s">
         <v>886</v>
       </c>
-      <c r="H18" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="16" t="b">
+      <c r="H18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J18" s="3">
@@ -12640,10 +12717,10 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>887</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>888</v>
       </c>
       <c r="C19" s="1" t="str">
@@ -12659,13 +12736,13 @@
       <c r="F19" s="2">
         <v>17</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="14" t="s">
         <v>889</v>
       </c>
-      <c r="H19" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="16" t="b">
+      <c r="H19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J19" s="3">
@@ -12673,32 +12750,32 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>890</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>891</v>
       </c>
-      <c r="C20" s="15" t="str">
+      <c r="C20" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Kill a guardian with no diamond gear</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="2" t="s">
         <v>842</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="2" t="s">
         <v>843</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="2">
         <v>18</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="15" t="s">
         <v>892</v>
       </c>
-      <c r="H20" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="16" t="b">
+      <c r="H20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J20" s="3">
@@ -12706,194 +12783,636 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>893</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="18" t="s">
         <v>894</v>
       </c>
-      <c r="C21" s="15" t="str">
+      <c r="C21" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Name tag an armorstand</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="2" t="s">
         <v>842</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="2" t="s">
         <v>843</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="2">
         <v>19</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="2" t="s">
         <v>893</v>
       </c>
-      <c r="H21" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" s="17">
+      <c r="H21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="24" t="s">
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
         <v>895</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>896</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="C22" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Kill a wither with no beacon effects and no diamond gear</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>842</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="2" t="s">
         <v>843</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="2">
         <v>20</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="15" t="s">
         <v>897</v>
       </c>
-      <c r="H22" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" s="17">
+      <c r="H22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11" t="s">
+        <v>898</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>899</v>
+      </c>
+      <c r="C23" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Be killed by friendly fire while you have the wither effect</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F23" s="2">
+        <v>21</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="H23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>900</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>901</v>
+      </c>
+      <c r="C24" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Kill a player when that player has the wither effect</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F24" s="2">
+        <v>22</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>903</v>
+      </c>
+      <c r="H24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>905</v>
+      </c>
+      <c r="C25" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Killed by a player when you have no gear on</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F25" s="2">
+        <v>23</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="H25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
+        <v>907</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>908</v>
+      </c>
+      <c r="C26" s="12" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>have dark oak log, dark oak saplings and a furnace in your inventory</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F26" s="2">
+        <v>24</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>944</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
+        <v>909</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>910</v>
+      </c>
+      <c r="C27" s="12" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>destroy a shulker with fire</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F27" s="2">
+        <v>25</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>945</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
+        <v>911</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>912</v>
+      </c>
+      <c r="C28" s="12" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>have a shulker that is dyed black</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F28" s="2">
+        <v>26</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>946</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>913</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>914</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>914</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F29" s="2">
+        <v>27</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>947</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
+        <v>915</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>916</v>
+      </c>
+      <c r="C30" s="12" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Obtain 164 gold blocks</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F30" s="2">
+        <v>28</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>948</v>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
+        <v>917</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>918</v>
+      </c>
+      <c r="C31" s="12" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Send a dolphin to the nether</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F31" s="2">
+        <v>29</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>949</v>
+      </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="12" t="s">
+        <v>919</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>920</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>921</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F32" s="2">
+        <v>30</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>950</v>
+      </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
+        <v>922</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>923</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>923</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F33" s="2">
+        <v>31</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>951</v>
+      </c>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="11" t="s">
+        <v>924</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>925</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="F34" s="2">
+        <v>32</v>
+      </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="12" t="s">
+        <v>926</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>927</v>
+      </c>
+      <c r="C35" s="12" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Craft 64 crafting tables</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>952</v>
+      </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
+        <v>928</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>929</v>
+      </c>
+      <c r="C36" s="12" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Burn 64 dark oak logs</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="F36" s="2">
+        <v>2</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>953</v>
+      </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="12" t="s">
+        <v>930</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="12" t="s">
+        <v>931</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="F37" s="2">
+        <v>3</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>954</v>
+      </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="12" t="s">
+        <v>932</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>933</v>
+      </c>
+      <c r="C38" s="12" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Have 164 netherite blocks and a beacon in your inventory</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="F38" s="2">
+        <v>4</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>955</v>
+      </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="12" t="s">
+        <v>934</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>935</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>936</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="F39" s="2">
+        <v>5</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>956</v>
+      </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
+        <v>937</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="12" t="s">
+        <v>938</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="F40" s="2">
+        <v>6</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>957</v>
+      </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
+        <v>939</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="12" t="s">
+        <v>940</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="F41" s="2">
+        <v>7</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>958</v>
+      </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="3"/>
-    </row>
-    <row r="43" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
+        <v>941</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>942</v>
+      </c>
+      <c r="C42" s="13" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Punch a zombie piglin or a piglin</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>943</v>
+      </c>
+      <c r="F42" s="21">
+        <v>8</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>959</v>
+      </c>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="22"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="3"/>
@@ -13294,19 +13813,53 @@
       <c r="J127" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:J15 E17:F20 E16:G16 H16:J20 E21:J21 E23:J1048576 E22:F22 H22:J22">
-    <cfRule type="expression" dxfId="14" priority="1">
+  <phoneticPr fontId="7" type="noConversion"/>
+  <conditionalFormatting sqref="E1:J15 E16:G16 H16:J20 E21:J21 E43:J1048576 E17:F20 F40:J42 G26:J39">
+    <cfRule type="expression" dxfId="23" priority="10">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="22" priority="11">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="21" priority="12">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H24:J24 E25:J25 E24:F24 F27:F28 F30:F31 F33:F34 F36:F37 F39 E26:E42">
+    <cfRule type="expression" dxfId="2" priority="7">
+      <formula>ROW()=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="8">
+      <formula>AND($A24&lt;&gt;"",MOD(ROW(),2)=1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>AND($A24&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22:J22 E22:F22">
+    <cfRule type="expression" dxfId="20" priority="4">
+      <formula>ROW()=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="5">
+      <formula>AND($A22&lt;&gt;"",MOD(ROW(),2)=1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="6">
+      <formula>AND($A22&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23:J23 F26 F29 F32 F35 F38">
+    <cfRule type="expression" dxfId="17" priority="1">
+      <formula>ROW()=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="2">
+      <formula>AND($A23&lt;&gt;"",MOD(ROW(),2)=1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="3">
+      <formula>AND($A23&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I22" xr:uid="{889EB968-2309-4054-9531-83439D0DAB8B}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I42" xr:uid="{889EB968-2309-4054-9531-83439D0DAB8B}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13322,7 +13875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03723C66-8E0B-48F3-9CF4-1B0F8B736B8C}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added bud category challenges
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7772E86C-4D10-4DF8-B654-C679881E79F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3BD364-8D60-4334-9E83-0C68D0F63487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Challenges" sheetId="4" r:id="rId3"/>
     <sheet name="Statistics" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="1023">
   <si>
     <t>Display Only Text</t>
   </si>
@@ -2903,6 +2903,195 @@
   </si>
   <si>
     <t>Name a cow super cow.</t>
+  </si>
+  <si>
+    <t>I Need Mo' Allowance</t>
+  </si>
+  <si>
+    <t>Hero in a Half Shell</t>
+  </si>
+  <si>
+    <t>HeroInAHalfShell</t>
+  </si>
+  <si>
+    <t>Hanami</t>
+  </si>
+  <si>
+    <t>Visit a cherry grove during Sakura Season (day 74 to 105, annually)</t>
+  </si>
+  <si>
+    <t>Eat a beetroot</t>
+  </si>
+  <si>
+    <t>Look at an Enderman</t>
+  </si>
+  <si>
+    <t>The Slender Man</t>
+  </si>
+  <si>
+    <t>TheSlenderMan</t>
+  </si>
+  <si>
+    <t>Return of Pumpkinhead</t>
+  </si>
+  <si>
+    <t>Wear a Jack o'Lantern on your head</t>
+  </si>
+  <si>
+    <t>Wear a Turtle Shell</t>
+  </si>
+  <si>
+    <t>Wear a leather helmet</t>
+  </si>
+  <si>
+    <t>Eat glow berries</t>
+  </si>
+  <si>
+    <t>bud</t>
+  </si>
+  <si>
+    <t>bud1</t>
+  </si>
+  <si>
+    <t>Gummiberry Juice</t>
+  </si>
+  <si>
+    <t>GummiberryJuice</t>
+  </si>
+  <si>
+    <t>Drink a Potion of Healing</t>
+  </si>
+  <si>
+    <t>You’re Gonna Need A Bigger Boat</t>
+  </si>
+  <si>
+    <t>Game Over, Man! Game Over!</t>
+  </si>
+  <si>
+    <t>Get killed by a Silverfish</t>
+  </si>
+  <si>
+    <t>Get killed by a Dolphin</t>
+  </si>
+  <si>
+    <t>Hello Clarice…</t>
+  </si>
+  <si>
+    <t>Kill a baby sheep</t>
+  </si>
+  <si>
+    <t>HelloClarice</t>
+  </si>
+  <si>
+    <t>Something Went Wrong</t>
+  </si>
+  <si>
+    <t>Teleport to the Nether with another entity</t>
+  </si>
+  <si>
+    <t>Get killed by a Drowned</t>
+  </si>
+  <si>
+    <t>YoullFloatToo</t>
+  </si>
+  <si>
+    <t>This... Is My Boomstick!</t>
+  </si>
+  <si>
+    <t>Kill a skeleton</t>
+  </si>
+  <si>
+    <t>ThisIsMyBoomstick</t>
+  </si>
+  <si>
+    <t>Kill a Stray</t>
+  </si>
+  <si>
+    <t>The Night Is Dark and Full Of Terrors</t>
+  </si>
+  <si>
+    <t>For the Dead Travel Fast</t>
+  </si>
+  <si>
+    <t>You’ll Float, Too</t>
+  </si>
+  <si>
+    <t>Never Feed Him After Midnight</t>
+  </si>
+  <si>
+    <t>Breed mobs between 00:00 and 01:00 (day tick 18,000 to 19,000)</t>
+  </si>
+  <si>
+    <t>Everyone's Entitled To One Good Scare</t>
+  </si>
+  <si>
+    <t>Get killed by a Creeper</t>
+  </si>
+  <si>
+    <t>OneGoodScare</t>
+  </si>
+  <si>
+    <t>TheNightIsDark</t>
+  </si>
+  <si>
+    <t>AfterMidnight</t>
+  </si>
+  <si>
+    <t>WentWrong</t>
+  </si>
+  <si>
+    <t>GameOverMan</t>
+  </si>
+  <si>
+    <t>ABiggerBoat</t>
+  </si>
+  <si>
+    <t>DeadTravelFast</t>
+  </si>
+  <si>
+    <t>Pumpkinhead</t>
+  </si>
+  <si>
+    <t>FootballHead</t>
+  </si>
+  <si>
+    <t>MoAllowance</t>
+  </si>
+  <si>
+    <t>Move it, Football Head!</t>
+  </si>
+  <si>
+    <t>Place a crimson door</t>
+  </si>
+  <si>
+    <t>PaintItBlack</t>
+  </si>
+  <si>
+    <t>Look Mommy, The Rhino's Getting Too Close To the Car</t>
+  </si>
+  <si>
+    <t>Get hit by a Ravager</t>
+  </si>
+  <si>
+    <t>CloseToTheCar</t>
+  </si>
+  <si>
+    <t>Enter Sandman</t>
+  </si>
+  <si>
+    <t>Suffocate in sand</t>
+  </si>
+  <si>
+    <t>EnterSandman</t>
+  </si>
+  <si>
+    <t>I Want It Painted Black</t>
+  </si>
+  <si>
+    <t>Deathbat</t>
+  </si>
+  <si>
+    <t>Get killed by a Phantom</t>
   </si>
 </sst>
 </file>
@@ -3072,7 +3261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3128,39 +3317,12 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="56">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -3236,6 +3398,79 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3372,27 +3607,6 @@
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -3512,37 +3726,6 @@
       </fill>
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3557,23 +3740,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:K127" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:K127" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <autoFilter ref="A2:K127" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J127">
     <sortCondition ref="J2:J127"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Achievment" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="In-game description" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Actual requirements (if different)" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Category" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Property Name" dataDxfId="45"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Index" dataDxfId="44"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Achievement (English Title)" dataDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Implement" dataDxfId="42"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Player.json" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sort Order" dataDxfId="40"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column1" dataDxfId="39">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Achievment" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="In-game description" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Actual requirements (if different)" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Category" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Property Name" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Index" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Achievement (English Title)" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Implement" dataDxfId="46"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Player.json" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sort Order" dataDxfId="44"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column1" dataDxfId="43">
       <calculatedColumnFormula>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3582,43 +3765,43 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:J112" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:J112" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A2:J112" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J112">
     <sortCondition ref="J2:J112"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Advancement" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="In-game description" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Actual requirements (if different)" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Category" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Property Name" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Index" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Advancement (English Title)" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Implement" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Player.json" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Sort Order" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Advancement" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="In-game description" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Actual requirements (if different)" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Category" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Property Name" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Index" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Advancement (English Title)" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Implement" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Player.json" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Sort Order" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE12FC0E-4709-4C73-B5B1-A169ACDBA6CE}" name="Table3" displayName="Table3" ref="A2:J42" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A2:J42" xr:uid="{DE12FC0E-4709-4C73-B5B1-A169ACDBA6CE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE12FC0E-4709-4C73-B5B1-A169ACDBA6CE}" name="Table3" displayName="Table3" ref="A2:J63" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A2:J63" xr:uid="{DE12FC0E-4709-4C73-B5B1-A169ACDBA6CE}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8A34E490-4B28-46A5-A4B0-AA9721A0B999}" name="Advancement" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{240DE560-2643-41B9-93AE-AD1D0B88670F}" name="In-game description" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{C9EBD348-EFEF-45E4-B948-8938B27250F0}" name="Actual requirements (if different)" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{8A34E490-4B28-46A5-A4B0-AA9721A0B999}" name="Advancement" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{240DE560-2643-41B9-93AE-AD1D0B88670F}" name="In-game description" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{C9EBD348-EFEF-45E4-B948-8938B27250F0}" name="Actual requirements (if different)" dataDxfId="7">
       <calculatedColumnFormula>Table3[[#This Row],[In-game description]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9DFAE2BC-F7A2-4E66-90D3-F7DEEBB0B980}" name="Category" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{C0BC5EC9-9291-4522-9534-16D631CD7152}" name="Property Name" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{7DDCB0E6-93DB-429A-AB2F-32609D87D9F6}" name="Index" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{771A1498-3C80-4E7A-8546-D022BD7155E4}" name="Advancement (English Title)" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{FAE293DB-7B8C-4B07-A5E0-F90A7FFAEF84}" name="Implement" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{F2787C17-E8A3-485F-9265-F0C2BFC9FAB1}" name="Player.json" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{785A3721-274D-4362-BD30-E3B0A3260CA8}" name="Sort Order" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{9DFAE2BC-F7A2-4E66-90D3-F7DEEBB0B980}" name="Category" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{C0BC5EC9-9291-4522-9534-16D631CD7152}" name="Property Name" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{7DDCB0E6-93DB-429A-AB2F-32609D87D9F6}" name="Index" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{771A1498-3C80-4E7A-8546-D022BD7155E4}" name="Advancement (English Title)" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{FAE293DB-7B8C-4B07-A5E0-F90A7FFAEF84}" name="Implement" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{F2787C17-E8A3-485F-9265-F0C2BFC9FAB1}" name="Player.json" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{785A3721-274D-4362-BD30-E3B0A3260CA8}" name="Sort Order" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3893,21 +4076,21 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="50.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="15.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" style="3" customWidth="1"/>
-    <col min="9" max="10" width="15.5703125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="35.5703125" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="50.5703125" style="4"/>
+    <col min="1" max="1" width="35.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.59765625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.59765625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15.59765625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="35.59765625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.59765625" style="3" customWidth="1"/>
+    <col min="9" max="10" width="15.59765625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="35.59765625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="50.59765625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3923,7 +4106,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3962,7 +4145,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -4002,7 +4185,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -4038,7 +4221,7 @@
         <v>Story12</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -4074,7 +4257,7 @@
         <v>Story13</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -4110,7 +4293,7 @@
         <v>Story14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -4146,7 +4329,7 @@
         <v>Story15</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -4182,7 +4365,7 @@
         <v>Story16</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -4218,7 +4401,7 @@
         <v>Husbandry11</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -4254,7 +4437,7 @@
         <v>Husbandry12</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>48</v>
       </c>
@@ -4290,7 +4473,7 @@
         <v>Husbandry13</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
@@ -4326,7 +4509,7 @@
         <v>Story17</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
@@ -4362,7 +4545,7 @@
         <v>Husbandry14</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
@@ -4398,7 +4581,7 @@
         <v>Adventure11</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
@@ -4434,7 +4617,7 @@
         <v>Story18</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>70</v>
       </c>
@@ -4470,7 +4653,7 @@
         <v>Adventure12</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>74</v>
       </c>
@@ -4506,7 +4689,7 @@
         <v>Husbandry15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>78</v>
       </c>
@@ -4542,7 +4725,7 @@
         <v>Adventure13</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
@@ -4578,7 +4761,7 @@
         <v>Adventure14</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>86</v>
       </c>
@@ -4614,7 +4797,7 @@
         <v>Story19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>90</v>
       </c>
@@ -4650,7 +4833,7 @@
         <v>Nether11</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>96</v>
       </c>
@@ -4686,7 +4869,7 @@
         <v>Nether12</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>100</v>
       </c>
@@ -4722,7 +4905,7 @@
         <v>Nether13</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>104</v>
       </c>
@@ -4758,7 +4941,7 @@
         <v>Nether14</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>108</v>
       </c>
@@ -4794,7 +4977,7 @@
         <v>The_End11</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>114</v>
       </c>
@@ -4830,7 +5013,7 @@
         <v>The_End12</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>117</v>
       </c>
@@ -4866,7 +5049,7 @@
         <v>Story110</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>120</v>
       </c>
@@ -4902,7 +5085,7 @@
         <v>Adventure15</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>123</v>
       </c>
@@ -4938,7 +5121,7 @@
         <v>Adventure16</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>126</v>
       </c>
@@ -4974,7 +5157,7 @@
         <v>Adventure17</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>130</v>
       </c>
@@ -5010,7 +5193,7 @@
         <v>Nether15</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>134</v>
       </c>
@@ -5046,7 +5229,7 @@
         <v>Nether16</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>137</v>
       </c>
@@ -5082,7 +5265,7 @@
         <v>Nether17</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>141</v>
       </c>
@@ -5118,7 +5301,7 @@
         <v>Husbandry17</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>144</v>
       </c>
@@ -5154,7 +5337,7 @@
         <v>Story111</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>148</v>
       </c>
@@ -5190,7 +5373,7 @@
         <v>Story112</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>151</v>
       </c>
@@ -5226,7 +5409,7 @@
         <v>Story113</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>155</v>
       </c>
@@ -5262,7 +5445,7 @@
         <v>Story114</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>158</v>
       </c>
@@ -5298,7 +5481,7 @@
         <v>Husbandry16</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>162</v>
       </c>
@@ -5334,7 +5517,7 @@
         <v>Husbandry18</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>165</v>
       </c>
@@ -5370,7 +5553,7 @@
         <v>Adventure18</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>169</v>
       </c>
@@ -5406,7 +5589,7 @@
         <v>Story115</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>172</v>
       </c>
@@ -5442,7 +5625,7 @@
         <v>Story116</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>175</v>
       </c>
@@ -5478,7 +5661,7 @@
         <v>Story117</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>178</v>
       </c>
@@ -5514,7 +5697,7 @@
         <v>Adventure19</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>182</v>
       </c>
@@ -5550,7 +5733,7 @@
         <v>Husbandry19</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>185</v>
       </c>
@@ -5586,7 +5769,7 @@
         <v>Husbandry110</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>189</v>
       </c>
@@ -5622,7 +5805,7 @@
         <v>Adventure110</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>192</v>
       </c>
@@ -5658,7 +5841,7 @@
         <v>Story118</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>196</v>
       </c>
@@ -5694,7 +5877,7 @@
         <v>Story119</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>200</v>
       </c>
@@ -5730,7 +5913,7 @@
         <v>Husbandry111</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>203</v>
       </c>
@@ -5766,7 +5949,7 @@
         <v>Story120</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>206</v>
       </c>
@@ -5802,7 +5985,7 @@
         <v>Husbandry112</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>210</v>
       </c>
@@ -5838,7 +6021,7 @@
         <v>Husbandry113</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>213</v>
       </c>
@@ -5874,7 +6057,7 @@
         <v>Adventure111</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>215</v>
       </c>
@@ -5910,7 +6093,7 @@
         <v>Story121</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>218</v>
       </c>
@@ -5946,7 +6129,7 @@
         <v>Adventure112</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>220</v>
       </c>
@@ -5982,7 +6165,7 @@
         <v>Adventure113</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>222</v>
       </c>
@@ -6018,7 +6201,7 @@
         <v>Story122</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>226</v>
       </c>
@@ -6054,7 +6237,7 @@
         <v>Story123</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>229</v>
       </c>
@@ -6090,7 +6273,7 @@
         <v>Story124</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>233</v>
       </c>
@@ -6126,7 +6309,7 @@
         <v>Adventure114</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>237</v>
       </c>
@@ -6162,7 +6345,7 @@
         <v>Story125</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>239</v>
       </c>
@@ -6198,7 +6381,7 @@
         <v>Husbandry114</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>242</v>
       </c>
@@ -6234,7 +6417,7 @@
         <v>Husbandry115</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>245</v>
       </c>
@@ -6270,7 +6453,7 @@
         <v>Adventure115</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>249</v>
       </c>
@@ -6306,7 +6489,7 @@
         <v>Husbandry116</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
         <v>252</v>
       </c>
@@ -6342,7 +6525,7 @@
         <v>Adventure116</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>255</v>
       </c>
@@ -6378,7 +6561,7 @@
         <v>Story126</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>258</v>
       </c>
@@ -6414,7 +6597,7 @@
         <v>Story127</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>261</v>
       </c>
@@ -6450,7 +6633,7 @@
         <v>The_End13</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
         <v>265</v>
       </c>
@@ -6486,7 +6669,7 @@
         <v>Nether18</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>269</v>
       </c>
@@ -6522,7 +6705,7 @@
         <v>The_End14</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
         <v>272</v>
       </c>
@@ -6558,7 +6741,7 @@
         <v>The_End15</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
         <v>275</v>
       </c>
@@ -6594,7 +6777,7 @@
         <v>The_End16</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
         <v>278</v>
       </c>
@@ -6630,7 +6813,7 @@
         <v>Adventure117</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
         <v>282</v>
       </c>
@@ -6666,7 +6849,7 @@
         <v>The_End17</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
         <v>285</v>
       </c>
@@ -6702,7 +6885,7 @@
         <v>Adventure118</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
         <v>289</v>
       </c>
@@ -6738,7 +6921,7 @@
         <v>Adventure119</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
         <v>292</v>
       </c>
@@ -6774,7 +6957,7 @@
         <v>Adventure120</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
         <v>295</v>
       </c>
@@ -6810,7 +6993,7 @@
         <v>Husbandry117</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
         <v>298</v>
       </c>
@@ -6846,7 +7029,7 @@
         <v>Adventure121</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
         <v>301</v>
       </c>
@@ -6882,7 +7065,7 @@
         <v>Adventure122</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
         <v>305</v>
       </c>
@@ -6918,7 +7101,7 @@
         <v>Adventure123</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
         <v>308</v>
       </c>
@@ -6954,7 +7137,7 @@
         <v>Adventure124</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
         <v>311</v>
       </c>
@@ -6990,7 +7173,7 @@
         <v>Husbandry118</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
         <v>315</v>
       </c>
@@ -7026,7 +7209,7 @@
         <v>Adventure125</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
         <v>319</v>
       </c>
@@ -7062,7 +7245,7 @@
         <v>Adventure126</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
         <v>323</v>
       </c>
@@ -7098,7 +7281,7 @@
         <v>Story128</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
         <v>327</v>
       </c>
@@ -7134,7 +7317,7 @@
         <v>Adventure127</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
         <v>331</v>
       </c>
@@ -7170,7 +7353,7 @@
         <v>Story129</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
         <v>334</v>
       </c>
@@ -7206,7 +7389,7 @@
         <v>Adventure128</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
         <v>337</v>
       </c>
@@ -7242,7 +7425,7 @@
         <v>Story130</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
         <v>340</v>
       </c>
@@ -7278,7 +7461,7 @@
         <v>Story131</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
         <v>344</v>
       </c>
@@ -7314,7 +7497,7 @@
         <v>Husbandry119</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
         <v>348</v>
       </c>
@@ -7350,7 +7533,7 @@
         <v>Husbandry120</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
         <v>350</v>
       </c>
@@ -7386,7 +7569,7 @@
         <v>Story132</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
         <v>354</v>
       </c>
@@ -7422,7 +7605,7 @@
         <v>Husbandry121</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A99" s="1" t="s">
         <v>358</v>
       </c>
@@ -7458,7 +7641,7 @@
         <v>Adventure129</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
         <v>361</v>
       </c>
@@ -7494,7 +7677,7 @@
         <v>Story21</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
         <v>366</v>
       </c>
@@ -7530,7 +7713,7 @@
         <v>Story22</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="s">
         <v>368</v>
       </c>
@@ -7566,7 +7749,7 @@
         <v>Adventure130</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="s">
         <v>372</v>
       </c>
@@ -7602,7 +7785,7 @@
         <v>Story23</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
         <v>375</v>
       </c>
@@ -7638,7 +7821,7 @@
         <v>Adventure131</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
         <v>378</v>
       </c>
@@ -7674,7 +7857,7 @@
         <v>Story24</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
         <v>382</v>
       </c>
@@ -7710,7 +7893,7 @@
         <v>Story25</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
         <v>385</v>
       </c>
@@ -7746,7 +7929,7 @@
         <v>Husbandry122</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A108" s="1" t="s">
         <v>388</v>
       </c>
@@ -7782,7 +7965,7 @@
         <v>Husbandry123</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A109" s="1" t="s">
         <v>391</v>
       </c>
@@ -7818,7 +8001,7 @@
         <v>Story26</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A110" s="1" t="s">
         <v>394</v>
       </c>
@@ -7854,7 +8037,7 @@
         <v>Story27</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A111" s="1" t="s">
         <v>396</v>
       </c>
@@ -7890,7 +8073,7 @@
         <v>Nether19</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112" s="1" t="s">
         <v>400</v>
       </c>
@@ -7926,7 +8109,7 @@
         <v>Nether110</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A113" s="1" t="s">
         <v>404</v>
       </c>
@@ -7962,7 +8145,7 @@
         <v>Nether111</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A114" s="1" t="s">
         <v>408</v>
       </c>
@@ -7998,7 +8181,7 @@
         <v>Adventure132</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A115" s="1" t="s">
         <v>412</v>
       </c>
@@ -8034,7 +8217,7 @@
         <v>Story28</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A116" s="1" t="s">
         <v>416</v>
       </c>
@@ -8070,7 +8253,7 @@
         <v>Husbandry124</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A117" s="1" t="s">
         <v>420</v>
       </c>
@@ -8106,7 +8289,7 @@
         <v>Story29</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A118" s="1" t="s">
         <v>423</v>
       </c>
@@ -8142,7 +8325,7 @@
         <v>Story210</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A119" s="1" t="s">
         <v>427</v>
       </c>
@@ -8178,7 +8361,7 @@
         <v>Story211</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A120" s="1" t="s">
         <v>431</v>
       </c>
@@ -8214,7 +8397,7 @@
         <v>Nether112</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A121" s="1" t="s">
         <v>435</v>
       </c>
@@ -8250,7 +8433,7 @@
         <v>Story212</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A122" s="1" t="s">
         <v>438</v>
       </c>
@@ -8286,7 +8469,7 @@
         <v>Husbandry125</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A123" s="1" t="s">
         <v>442</v>
       </c>
@@ -8322,7 +8505,7 @@
         <v>Nether113</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A124" s="1" t="s">
         <v>446</v>
       </c>
@@ -8358,7 +8541,7 @@
         <v>Story213</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A125" s="1" t="s">
         <v>450</v>
       </c>
@@ -8394,7 +8577,7 @@
         <v>Story214</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A126" s="1" t="s">
         <v>453</v>
       </c>
@@ -8430,7 +8613,7 @@
         <v>Story215</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A127" s="1" t="s">
         <v>456</v>
       </c>
@@ -8468,18 +8651,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:K1048576">
-    <cfRule type="expression" dxfId="55" priority="3">
+    <cfRule type="expression" dxfId="30" priority="3">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="4">
+    <cfRule type="expression" dxfId="29" priority="4">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="5">
+    <cfRule type="expression" dxfId="28" priority="5">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="duplicateValues" dxfId="52" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I127" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -8501,22 +8684,22 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="50.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="15.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="50.5703125" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="50.5703125" style="4"/>
+    <col min="1" max="1" width="35.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.59765625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="50.59765625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="15.59765625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="35.59765625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.59765625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.59765625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.59765625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="50.59765625" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="50.59765625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -8538,7 +8721,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>459</v>
       </c>
@@ -8570,7 +8753,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>461</v>
       </c>
@@ -8602,7 +8785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>465</v>
       </c>
@@ -8634,7 +8817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -8666,7 +8849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -8698,7 +8881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>473</v>
       </c>
@@ -8730,7 +8913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>477</v>
       </c>
@@ -8762,7 +8945,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>481</v>
       </c>
@@ -8794,7 +8977,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>485</v>
       </c>
@@ -8826,7 +9009,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>489</v>
       </c>
@@ -8858,7 +9041,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>493</v>
       </c>
@@ -8890,7 +9073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>497</v>
       </c>
@@ -8922,7 +9105,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>501</v>
       </c>
@@ -8954,7 +9137,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>117</v>
       </c>
@@ -8986,7 +9169,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>206</v>
       </c>
@@ -9018,7 +9201,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>509</v>
       </c>
@@ -9050,7 +9233,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>108</v>
       </c>
@@ -9082,7 +9265,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>93</v>
       </c>
@@ -9114,7 +9297,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>96</v>
       </c>
@@ -9146,7 +9329,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>519</v>
       </c>
@@ -9178,7 +9361,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>522</v>
       </c>
@@ -9210,7 +9393,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>526</v>
       </c>
@@ -9242,7 +9425,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>530</v>
       </c>
@@ -9274,7 +9457,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>534</v>
       </c>
@@ -9306,7 +9489,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>538</v>
       </c>
@@ -9338,7 +9521,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>542</v>
       </c>
@@ -9370,7 +9553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>546</v>
       </c>
@@ -9402,7 +9585,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>550</v>
       </c>
@@ -9434,7 +9617,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>554</v>
       </c>
@@ -9466,7 +9649,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>557</v>
       </c>
@@ -9498,7 +9681,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>561</v>
       </c>
@@ -9530,7 +9713,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>100</v>
       </c>
@@ -9562,7 +9745,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>567</v>
       </c>
@@ -9594,7 +9777,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>431</v>
       </c>
@@ -9626,7 +9809,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>572</v>
       </c>
@@ -9658,7 +9841,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>576</v>
       </c>
@@ -9690,7 +9873,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>104</v>
       </c>
@@ -9722,7 +9905,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>582</v>
       </c>
@@ -9754,7 +9937,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>586</v>
       </c>
@@ -9786,7 +9969,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>590</v>
       </c>
@@ -9818,7 +10001,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>593</v>
       </c>
@@ -9850,7 +10033,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>114</v>
       </c>
@@ -9882,7 +10065,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>599</v>
       </c>
@@ -9914,7 +10097,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>603</v>
       </c>
@@ -9946,7 +10129,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>607</v>
       </c>
@@ -9978,7 +10161,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>269</v>
       </c>
@@ -10010,7 +10193,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>261</v>
       </c>
@@ -10042,7 +10225,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>615</v>
       </c>
@@ -10074,7 +10257,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>619</v>
       </c>
@@ -10106,7 +10289,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>272</v>
       </c>
@@ -10138,7 +10321,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>64</v>
       </c>
@@ -10170,7 +10353,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>627</v>
       </c>
@@ -10202,7 +10385,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>631</v>
       </c>
@@ -10234,7 +10417,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>70</v>
       </c>
@@ -10266,7 +10449,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>636</v>
       </c>
@@ -10298,7 +10481,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>640</v>
       </c>
@@ -10330,7 +10513,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>644</v>
       </c>
@@ -10362,7 +10545,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>391</v>
       </c>
@@ -10394,7 +10577,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>649</v>
       </c>
@@ -10426,7 +10609,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>652</v>
       </c>
@@ -10458,7 +10641,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>420</v>
       </c>
@@ -10490,7 +10673,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>658</v>
       </c>
@@ -10522,7 +10705,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>446</v>
       </c>
@@ -10554,7 +10737,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>663</v>
       </c>
@@ -10586,7 +10769,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>667</v>
       </c>
@@ -10618,7 +10801,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>671</v>
       </c>
@@ -10650,7 +10833,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
         <v>675</v>
       </c>
@@ -10682,7 +10865,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="225" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>679</v>
       </c>
@@ -10714,7 +10897,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>683</v>
       </c>
@@ -10746,7 +10929,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="165" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>687</v>
       </c>
@@ -10778,7 +10961,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
         <v>691</v>
       </c>
@@ -10810,7 +10993,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>694</v>
       </c>
@@ -10842,7 +11025,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
         <v>698</v>
       </c>
@@ -10874,7 +11057,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
         <v>702</v>
       </c>
@@ -10906,7 +11089,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
         <v>704</v>
       </c>
@@ -10938,7 +11121,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
         <v>708</v>
       </c>
@@ -10970,7 +11153,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
         <v>712</v>
       </c>
@@ -11002,7 +11185,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
         <v>715</v>
       </c>
@@ -11034,7 +11217,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="285" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="285" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
         <v>126</v>
       </c>
@@ -11066,7 +11249,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
         <v>427</v>
       </c>
@@ -11098,7 +11281,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
         <v>721</v>
       </c>
@@ -11130,7 +11313,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
         <v>725</v>
       </c>
@@ -11162,7 +11345,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
         <v>728</v>
       </c>
@@ -11194,7 +11377,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
         <v>82</v>
       </c>
@@ -11226,7 +11409,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
         <v>394</v>
       </c>
@@ -11258,7 +11441,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
         <v>41</v>
       </c>
@@ -11290,7 +11473,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
         <v>740</v>
       </c>
@@ -11322,7 +11505,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="120" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
         <v>744</v>
       </c>
@@ -11354,7 +11537,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
         <v>748</v>
       </c>
@@ -11386,7 +11569,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
         <v>752</v>
       </c>
@@ -11418,7 +11601,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
         <v>755</v>
       </c>
@@ -11450,7 +11633,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
         <v>759</v>
       </c>
@@ -11482,7 +11665,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
         <v>763</v>
       </c>
@@ -11514,7 +11697,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
         <v>388</v>
       </c>
@@ -11546,7 +11729,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
         <v>768</v>
       </c>
@@ -11578,7 +11761,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
         <v>771</v>
       </c>
@@ -11610,7 +11793,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
         <v>775</v>
       </c>
@@ -11642,7 +11825,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A99" s="1" t="s">
         <v>779</v>
       </c>
@@ -11674,7 +11857,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="135" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A100" s="1" t="s">
         <v>783</v>
       </c>
@@ -11706,7 +11889,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="1" t="s">
         <v>787</v>
       </c>
@@ -11738,7 +11921,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A102" s="1" t="s">
         <v>791</v>
       </c>
@@ -11770,7 +11953,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A103" s="1" t="s">
         <v>795</v>
       </c>
@@ -11802,7 +11985,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A104" s="1" t="s">
         <v>799</v>
       </c>
@@ -11834,7 +12017,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A105" s="1" t="s">
         <v>803</v>
       </c>
@@ -11866,7 +12049,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" ht="195" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A106" s="1" t="s">
         <v>807</v>
       </c>
@@ -11898,7 +12081,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A107" s="1" t="s">
         <v>811</v>
       </c>
@@ -11930,7 +12113,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A108" s="1" t="s">
         <v>815</v>
       </c>
@@ -11962,7 +12145,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A109" s="1" t="s">
         <v>819</v>
       </c>
@@ -11994,7 +12177,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A110" s="1" t="s">
         <v>823</v>
       </c>
@@ -12026,7 +12209,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A111" s="1" t="s">
         <v>827</v>
       </c>
@@ -12058,7 +12241,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A112" s="1" t="s">
         <v>416</v>
       </c>
@@ -12092,13 +12275,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:J1048576">
-    <cfRule type="expression" dxfId="38" priority="1">
+    <cfRule type="expression" dxfId="26" priority="1">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="2">
+    <cfRule type="expression" dxfId="25" priority="2">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="3">
+    <cfRule type="expression" dxfId="24" priority="3">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12118,24 +12301,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A114CABE-4723-471F-81B1-1F98BAE7D3E1}">
   <dimension ref="A1:N127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" customWidth="1"/>
-    <col min="2" max="2" width="49.7109375" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37.86328125" customWidth="1"/>
+    <col min="2" max="2" width="49.73046875" customWidth="1"/>
+    <col min="3" max="3" width="63.3984375" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="35.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" style="3" customWidth="1"/>
-    <col min="9" max="10" width="15.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="15.59765625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.59765625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="35.59765625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="20.59765625" style="3" customWidth="1"/>
+    <col min="9" max="10" width="15.59765625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="21" x14ac:dyDescent="0.65">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -12148,7 +12331,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="8" t="str">
         <f>CONCATENATE("Complete: ",COUNTIF(Table3[Implement],"=TRUE"),"/",ROWS(Table3[Implement]))</f>
-        <v>Complete: 0/40</v>
+        <v>Complete: 0/61</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -12156,7 +12339,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="4"/>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>459</v>
       </c>
@@ -12188,7 +12371,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>162</v>
       </c>
@@ -12221,7 +12404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>844</v>
       </c>
@@ -12254,7 +12437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>847</v>
       </c>
@@ -12287,7 +12470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>850</v>
       </c>
@@ -12320,7 +12503,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>853</v>
       </c>
@@ -12353,7 +12536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>856</v>
       </c>
@@ -12386,7 +12569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>859</v>
       </c>
@@ -12419,7 +12602,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>865</v>
       </c>
@@ -12452,7 +12635,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>864</v>
       </c>
@@ -12485,7 +12668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>867</v>
       </c>
@@ -12518,7 +12701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="10" t="s">
         <v>870</v>
       </c>
@@ -12551,7 +12734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>873</v>
       </c>
@@ -12584,7 +12767,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="26.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="13" t="s">
         <v>875</v>
       </c>
@@ -12617,7 +12800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="12" t="s">
         <v>878</v>
       </c>
@@ -12650,7 +12833,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="12" t="s">
         <v>881</v>
       </c>
@@ -12683,7 +12866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A18" s="12" t="s">
         <v>884</v>
       </c>
@@ -12716,7 +12899,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A19" s="12" t="s">
         <v>887</v>
       </c>
@@ -12749,7 +12932,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A20" s="13" t="s">
         <v>890</v>
       </c>
@@ -12782,7 +12965,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="13" t="s">
         <v>893</v>
       </c>
@@ -12815,7 +12998,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="18" t="s">
         <v>895</v>
       </c>
@@ -12848,7 +13031,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A23" s="11" t="s">
         <v>898</v>
       </c>
@@ -12881,7 +13064,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A24" s="18" t="s">
         <v>900</v>
       </c>
@@ -12914,7 +13097,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>904</v>
       </c>
@@ -12947,7 +13130,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="26.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A26" s="12" t="s">
         <v>907</v>
       </c>
@@ -12974,7 +13157,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A27" s="12" t="s">
         <v>909</v>
       </c>
@@ -13001,7 +13184,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A28" s="12" t="s">
         <v>911</v>
       </c>
@@ -13028,7 +13211,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A29" s="12" t="s">
         <v>913</v>
       </c>
@@ -13054,7 +13237,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A30" s="12" t="s">
         <v>915</v>
       </c>
@@ -13081,7 +13264,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A31" s="12" t="s">
         <v>917</v>
       </c>
@@ -13108,7 +13291,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="12" t="s">
         <v>919</v>
       </c>
@@ -13134,7 +13317,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A33" s="12" t="s">
         <v>922</v>
       </c>
@@ -13160,7 +13343,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A34" s="12"/>
       <c r="B34" s="11" t="s">
         <v>924</v>
@@ -13181,7 +13364,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A35" s="12" t="s">
         <v>926</v>
       </c>
@@ -13208,7 +13391,7 @@
       <c r="I35" s="2"/>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A36" s="12" t="s">
         <v>928</v>
       </c>
@@ -13235,7 +13418,7 @@
       <c r="I36" s="2"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A37" s="12" t="s">
         <v>930</v>
       </c>
@@ -13259,7 +13442,7 @@
       <c r="I37" s="2"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A38" s="12" t="s">
         <v>932</v>
       </c>
@@ -13286,7 +13469,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A39" s="12" t="s">
         <v>934</v>
       </c>
@@ -13312,7 +13495,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="3"/>
     </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A40" s="12" t="s">
         <v>937</v>
       </c>
@@ -13339,7 +13522,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A41" s="12" t="s">
         <v>938</v>
       </c>
@@ -13363,7 +13546,7 @@
       <c r="I41" s="2"/>
       <c r="J41" s="3"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="13" t="s">
         <v>940</v>
       </c>
@@ -13380,477 +13563,939 @@
       <c r="E42" s="2" t="s">
         <v>941</v>
       </c>
-      <c r="F42" s="21">
+      <c r="F42" s="2">
         <v>8</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>957</v>
       </c>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="22"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="3"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>965</v>
+      </c>
+      <c r="C43" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Eat a beetroot</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>1010</v>
+      </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="J43" s="3"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A44" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>971</v>
+      </c>
+      <c r="C44" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Wear a Turtle Shell</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F44" s="2">
+        <v>2</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>962</v>
+      </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C45" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Suffocate in sand</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F45" s="2">
+        <v>3</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>1019</v>
+      </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A46" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>964</v>
+      </c>
+      <c r="C46" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Visit a cherry grove during Sakura Season (day 74 to 105, annually)</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F46" s="2">
+        <v>4</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>963</v>
+      </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A47" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="C47" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Wear a leather helmet</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F47" s="2">
+        <v>5</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>1009</v>
+      </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>966</v>
+      </c>
+      <c r="C48" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Look at an Enderman</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F48" s="2">
+        <v>6</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>968</v>
+      </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A49" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>970</v>
+      </c>
+      <c r="C49" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Wear a Jack o'Lantern on your head</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F49" s="2">
+        <v>7</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>1008</v>
+      </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="3"/>
     </row>
-    <row r="50" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A50" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>973</v>
+      </c>
+      <c r="C50" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Eat glow berries</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F50" s="2">
+        <v>8</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>977</v>
+      </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="3"/>
     </row>
-    <row r="51" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A51" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>978</v>
+      </c>
+      <c r="C51" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Drink a Potion of Healing</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F51" s="2">
+        <v>9</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>1007</v>
+      </c>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="3"/>
     </row>
-    <row r="52" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A52" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>982</v>
+      </c>
+      <c r="C52" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Get killed by a Dolphin</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F52" s="2">
+        <v>10</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>1006</v>
+      </c>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="3"/>
     </row>
-    <row r="53" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A53" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>981</v>
+      </c>
+      <c r="C53" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Get killed by a Silverfish</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F53" s="2">
+        <v>11</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>1005</v>
+      </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="3"/>
     </row>
-    <row r="54" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A54" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>984</v>
+      </c>
+      <c r="C54" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Kill a baby sheep</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F54" s="2">
+        <v>12</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>985</v>
+      </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="3"/>
     </row>
-    <row r="55" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A55" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>987</v>
+      </c>
+      <c r="C55" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Teleport to the Nether with another entity</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F55" s="2">
+        <v>13</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>1004</v>
+      </c>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="3"/>
     </row>
-    <row r="56" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A56" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>988</v>
+      </c>
+      <c r="C56" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Get killed by a Drowned</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F56" s="2">
+        <v>14</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>989</v>
+      </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="3"/>
     </row>
-    <row r="57" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A57" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>991</v>
+      </c>
+      <c r="C57" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Kill a skeleton</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F57" s="2">
+        <v>15</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>992</v>
+      </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
       <c r="J57" s="3"/>
     </row>
-    <row r="58" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A58" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>993</v>
+      </c>
+      <c r="C58" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Kill a Stray</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F58" s="2">
+        <v>16</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>1002</v>
+      </c>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
       <c r="J58" s="3"/>
     </row>
-    <row r="59" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A59" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>998</v>
+      </c>
+      <c r="C59" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Breed mobs between 00:00 and 01:00 (day tick 18,000 to 19,000)</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F59" s="2">
+        <v>17</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>1003</v>
+      </c>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
       <c r="J59" s="3"/>
     </row>
-    <row r="60" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A60" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C60" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Get killed by a Creeper</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F60" s="2">
+        <v>18</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>1001</v>
+      </c>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="3"/>
     </row>
-    <row r="61" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A61" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C61" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Place a crimson door</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F61" s="2">
+        <v>19</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>1013</v>
+      </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A62" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C62" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Get hit by a Ravager</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F62" s="2">
+        <v>20</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>1016</v>
+      </c>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A63" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C63" s="1" t="str">
+        <f>Table3[[#This Row],[In-game description]]</f>
+        <v>Get killed by a Phantom</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="F63" s="2">
+        <v>21</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>1021</v>
+      </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="3"/>
     </row>
-    <row r="64" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
       <c r="J64" s="3"/>
     </row>
-    <row r="65" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
       <c r="J65" s="3"/>
     </row>
-    <row r="66" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
       <c r="J66" s="3"/>
     </row>
-    <row r="67" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
       <c r="J67" s="3"/>
     </row>
-    <row r="68" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
       <c r="J68" s="3"/>
     </row>
-    <row r="69" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="3"/>
     </row>
-    <row r="70" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
       <c r="J70" s="3"/>
     </row>
-    <row r="71" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
       <c r="J71" s="3"/>
     </row>
-    <row r="72" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
       <c r="J72" s="3"/>
     </row>
-    <row r="73" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
       <c r="J73" s="3"/>
     </row>
-    <row r="74" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
       <c r="J74" s="3"/>
     </row>
-    <row r="75" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
       <c r="J75" s="3"/>
     </row>
-    <row r="76" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
       <c r="J76" s="3"/>
     </row>
-    <row r="77" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="3"/>
     </row>
-    <row r="78" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="3"/>
     </row>
-    <row r="79" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
       <c r="J79" s="3"/>
     </row>
-    <row r="80" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
       <c r="J80" s="3"/>
     </row>
-    <row r="81" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
       <c r="J81" s="3"/>
     </row>
-    <row r="82" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
       <c r="J82" s="3"/>
     </row>
-    <row r="83" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
       <c r="J83" s="3"/>
     </row>
-    <row r="84" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
       <c r="J84" s="3"/>
     </row>
-    <row r="85" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
       <c r="J85" s="3"/>
     </row>
-    <row r="86" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
       <c r="J86" s="3"/>
     </row>
-    <row r="87" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
       <c r="J87" s="3"/>
     </row>
-    <row r="88" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
       <c r="J88" s="3"/>
     </row>
-    <row r="89" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
       <c r="J89" s="3"/>
     </row>
-    <row r="90" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
       <c r="J90" s="3"/>
     </row>
-    <row r="91" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
       <c r="J91" s="3"/>
     </row>
-    <row r="92" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
       <c r="J92" s="3"/>
     </row>
-    <row r="93" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
       <c r="J93" s="3"/>
     </row>
-    <row r="94" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
       <c r="J94" s="3"/>
     </row>
-    <row r="95" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
       <c r="J95" s="3"/>
     </row>
-    <row r="96" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
       <c r="J96" s="3"/>
     </row>
-    <row r="97" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
       <c r="J97" s="3"/>
     </row>
-    <row r="98" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
       <c r="J98" s="3"/>
     </row>
-    <row r="99" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
       <c r="J99" s="3"/>
     </row>
-    <row r="100" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
       <c r="J100" s="3"/>
     </row>
-    <row r="101" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
       <c r="J101" s="3"/>
     </row>
-    <row r="102" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
       <c r="J102" s="3"/>
     </row>
-    <row r="103" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
       <c r="J103" s="3"/>
     </row>
-    <row r="104" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
       <c r="J104" s="3"/>
     </row>
-    <row r="105" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
       <c r="J105" s="3"/>
     </row>
-    <row r="106" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
       <c r="J106" s="3"/>
     </row>
-    <row r="107" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
       <c r="J107" s="3"/>
     </row>
-    <row r="108" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
       <c r="J108" s="3"/>
     </row>
-    <row r="109" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109" s="3"/>
     </row>
-    <row r="110" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
       <c r="J110" s="3"/>
     </row>
-    <row r="111" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
       <c r="J111" s="3"/>
     </row>
-    <row r="112" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
       <c r="J112" s="3"/>
     </row>
-    <row r="113" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
       <c r="J113" s="3"/>
     </row>
-    <row r="114" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
       <c r="J114" s="3"/>
     </row>
-    <row r="115" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
       <c r="J115" s="3"/>
     </row>
-    <row r="116" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
       <c r="J116" s="3"/>
     </row>
-    <row r="117" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
       <c r="J117" s="3"/>
     </row>
-    <row r="118" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
       <c r="J118" s="3"/>
     </row>
-    <row r="119" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
       <c r="J119" s="3"/>
     </row>
-    <row r="120" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
       <c r="J120" s="3"/>
     </row>
-    <row r="121" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
       <c r="J121" s="3"/>
     </row>
-    <row r="122" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
       <c r="J122" s="3"/>
     </row>
-    <row r="123" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
       <c r="J123" s="3"/>
     </row>
-    <row r="124" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
       <c r="J124" s="3"/>
     </row>
-    <row r="125" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
       <c r="J125" s="3"/>
     </row>
-    <row r="126" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
       <c r="J126" s="3"/>
     </row>
-    <row r="127" spans="8:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="8:10" x14ac:dyDescent="0.45">
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
       <c r="J127" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="E1:J15 E16:G16 H16:J20 E21:J21 E43:J1048576 E17:F20 F40:J42 G26:J39">
-    <cfRule type="expression" dxfId="23" priority="10">
+  <conditionalFormatting sqref="E22:F22 H22:J22">
+    <cfRule type="expression" dxfId="23" priority="4">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="11">
+    <cfRule type="expression" dxfId="22" priority="5">
+      <formula>AND($A22&lt;&gt;"",MOD(ROW(),2)=1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="6">
+      <formula>AND($A22&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24:F24 H24:J24 E25:J25 E26:E42">
+    <cfRule type="expression" dxfId="20" priority="7">
+      <formula>ROW()=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="8">
+      <formula>AND($A24&lt;&gt;"",MOD(ROW(),2)=1)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="9">
+      <formula>AND($A24&lt;&gt;"",MOD(ROW(),2)=0)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:J15 E16:G16 H16:J20 E17:F20 E21:J21 G26:J39 F40:J42 E43:J1048576">
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>ROW()=2</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="11">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="12">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24:J24 E25:J25 E24:F24 F27:F28 F30:F31 F33:F34 F36:F37 F39 E26:E42">
-    <cfRule type="expression" dxfId="2" priority="7">
-      <formula>ROW()=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="8">
-      <formula>AND($A24&lt;&gt;"",MOD(ROW(),2)=1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9">
-      <formula>AND($A24&lt;&gt;"",MOD(ROW(),2)=0)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22:J22 E22:F22">
-    <cfRule type="expression" dxfId="20" priority="4">
-      <formula>ROW()=2</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="5">
-      <formula>AND($A22&lt;&gt;"",MOD(ROW(),2)=1)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="6">
-      <formula>AND($A22&lt;&gt;"",MOD(ROW(),2)=0)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23:J23 F26 F29 F32 F35 F38">
+  <conditionalFormatting sqref="E23:J23 F26:F39">
     <cfRule type="expression" dxfId="17" priority="1">
       <formula>ROW()=2</formula>
     </cfRule>
@@ -13862,7 +14507,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I42" xr:uid="{889EB968-2309-4054-9531-83439D0DAB8B}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I63" xr:uid="{889EB968-2309-4054-9531-83439D0DAB8B}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13882,14 +14527,14 @@
       <selection activeCell="G2" sqref="G2:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>834</v>
       </c>
@@ -13906,7 +14551,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>833</v>
       </c>
@@ -13931,7 +14576,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>838</v>
       </c>
@@ -13956,7 +14601,7 @@
         <v>0.59090909090909094</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>840</v>
       </c>

</xml_diff>

<commit_message>
Completed a few challenges
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEDA09B-DE01-4CDA-A791-F5F776F2FFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F89726-1E84-409D-9012-51D0BE8D573C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="1035">
   <si>
     <t>Display Only Text</t>
   </si>
@@ -2545,9 +2545,6 @@
     <t>PercentCompleted</t>
   </si>
   <si>
-    <t>Both</t>
-  </si>
-  <si>
     <t>Kill a mob with a pork chop</t>
   </si>
   <si>
@@ -3122,6 +3119,15 @@
   </si>
   <si>
     <t>OutOfFoodAreWe</t>
+  </si>
+  <si>
+    <t>NoMoreTraders</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Challenges</t>
   </si>
 </sst>
 </file>
@@ -3354,40 +3360,25 @@
   </cellStyles>
   <dxfs count="56">
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3472,6 +3463,73 @@
           <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3583,27 +3641,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -3725,37 +3762,6 @@
       </fill>
       <alignment horizontal="left" vertical="bottom" wrapText="1"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3770,23 +3776,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:K127" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:K127" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <autoFilter ref="A2:K127" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J127">
     <sortCondition ref="J2:J127"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Achievment" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="In-game description" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Actual requirements (if different)" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Category" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Property Name" dataDxfId="45"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Index" dataDxfId="44"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Achievement (English Title)" dataDxfId="43"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Implement" dataDxfId="42"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Player.json" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sort Order" dataDxfId="40"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column1" dataDxfId="39">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Achievment" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="In-game description" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Actual requirements (if different)" dataDxfId="51"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Category" dataDxfId="50"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Property Name" dataDxfId="49"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Index" dataDxfId="48"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Achievement (English Title)" dataDxfId="47"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Implement" dataDxfId="46"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Player.json" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sort Order" dataDxfId="44"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column1" dataDxfId="43">
       <calculatedColumnFormula>CONCATENATE(Table1[[#This Row],[Property Name]],Table1[[#This Row],[Index]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3795,43 +3801,43 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:J112" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A2:J112" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A2:J112" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J112">
     <sortCondition ref="J2:J112"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Advancement" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="In-game description" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Actual requirements (if different)" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Category" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Property Name" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Index" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Advancement (English Title)" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Implement" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Player.json" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Sort Order" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Advancement" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="In-game description" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Actual requirements (if different)" dataDxfId="38"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Category" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Property Name" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Index" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Advancement (English Title)" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Implement" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Player.json" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Sort Order" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE12FC0E-4709-4C73-B5B1-A169ACDBA6CE}" name="Table3" displayName="Table3" ref="A2:J66" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE12FC0E-4709-4C73-B5B1-A169ACDBA6CE}" name="Table3" displayName="Table3" ref="A2:J66" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A2:J66" xr:uid="{DE12FC0E-4709-4C73-B5B1-A169ACDBA6CE}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{8A34E490-4B28-46A5-A4B0-AA9721A0B999}" name="Advancement" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{240DE560-2643-41B9-93AE-AD1D0B88670F}" name="In-game description" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{C9EBD348-EFEF-45E4-B948-8938B27250F0}" name="Actual requirements (if different)" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{8A34E490-4B28-46A5-A4B0-AA9721A0B999}" name="Advancement" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{240DE560-2643-41B9-93AE-AD1D0B88670F}" name="In-game description" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{C9EBD348-EFEF-45E4-B948-8938B27250F0}" name="Actual requirements (if different)" dataDxfId="26">
       <calculatedColumnFormula>Table3[[#This Row],[In-game description]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9DFAE2BC-F7A2-4E66-90D3-F7DEEBB0B980}" name="Category" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{C0BC5EC9-9291-4522-9534-16D631CD7152}" name="Property Name" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{7DDCB0E6-93DB-429A-AB2F-32609D87D9F6}" name="Index" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{771A1498-3C80-4E7A-8546-D022BD7155E4}" name="Advancement (English Title)" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{FAE293DB-7B8C-4B07-A5E0-F90A7FFAEF84}" name="Implement" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{F2787C17-E8A3-485F-9265-F0C2BFC9FAB1}" name="Player.json" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{785A3721-274D-4362-BD30-E3B0A3260CA8}" name="Sort Order" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{9DFAE2BC-F7A2-4E66-90D3-F7DEEBB0B980}" name="Category" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{C0BC5EC9-9291-4522-9534-16D631CD7152}" name="Property Name" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{7DDCB0E6-93DB-429A-AB2F-32609D87D9F6}" name="Index" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{771A1498-3C80-4E7A-8546-D022BD7155E4}" name="Advancement (English Title)" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{FAE293DB-7B8C-4B07-A5E0-F90A7FFAEF84}" name="Implement" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{F2787C17-E8A3-485F-9265-F0C2BFC9FAB1}" name="Player.json" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{785A3721-274D-4362-BD30-E3B0A3260CA8}" name="Sort Order" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8681,18 +8687,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:K1048576">
-    <cfRule type="expression" dxfId="55" priority="3">
+    <cfRule type="expression" dxfId="18" priority="3">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="5">
+    <cfRule type="expression" dxfId="16" priority="5">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="duplicateValues" dxfId="52" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I127" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -12305,13 +12311,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:J1048576">
-    <cfRule type="expression" dxfId="38" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12331,8 +12337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A114CABE-4723-471F-81B1-1F98BAE7D3E1}">
   <dimension ref="A1:N126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12361,7 +12367,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="8" t="str">
         <f>CONCATENATE("Complete: ",COUNTIF(Table3[Implement],"=TRUE"),"/",ROWS(Table3[Implement]))</f>
-        <v>Complete: 0/64</v>
+        <v>Complete: 8/64</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -12406,17 +12412,17 @@
         <v>162</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C3" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Kill a mob with a pork chop</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -12425,7 +12431,7 @@
         <v>164</v>
       </c>
       <c r="H3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" s="2" t="b">
         <v>0</v>
@@ -12436,29 +12442,29 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>844</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>845</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Kill a mob with a cooked beef</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="H4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="2" t="b">
         <v>0</v>
@@ -12469,26 +12475,26 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>847</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>848</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Die in the end in the viod</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F5" s="2">
         <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="H5" s="2" t="b">
         <v>0</v>
@@ -12502,29 +12508,29 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>850</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>851</v>
       </c>
       <c r="C6" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Kill a Tamed Horse</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F6" s="2">
         <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="H6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2" t="b">
         <v>0</v>
@@ -12535,29 +12541,29 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>853</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>854</v>
       </c>
       <c r="C7" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Kill A named Horse</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F7" s="2">
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="H7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" s="2" t="b">
         <v>0</v>
@@ -12568,29 +12574,29 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>856</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>857</v>
       </c>
       <c r="C8" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Be Killed By a Dolphin.</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F8" s="2">
         <v>6</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="H8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="2" t="b">
         <v>0</v>
@@ -12601,26 +12607,26 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>859</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>860</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Get all 16 Dyes</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F9" s="2">
         <v>7</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="H9" s="2" t="b">
         <v>0</v>
@@ -12634,26 +12640,26 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C10" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Obtain a Wither Rose</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F10" s="2">
         <v>8</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="H10" s="2" t="b">
         <v>0</v>
@@ -12667,26 +12673,26 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C11" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Place Slime at Build Height</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F11" s="2">
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>864</v>
+        <v>1032</v>
       </c>
       <c r="H11" s="2" t="b">
         <v>0</v>
@@ -12700,26 +12706,26 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>867</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>868</v>
       </c>
       <c r="C12" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Have 20 vindicators within 16 blocks of the player</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F12" s="2">
         <v>10</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="H12" s="2" t="b">
         <v>0</v>
@@ -12733,26 +12739,26 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
+        <v>869</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>870</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>871</v>
       </c>
       <c r="C13" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Place 42,000 magma blocks</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F13" s="2">
         <v>11</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="H13" s="2" t="b">
         <v>0</v>
@@ -12766,26 +12772,26 @@
     </row>
     <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>873</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>874</v>
       </c>
       <c r="C14" s="4" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Break 1,000,000 Blocks</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F14" s="2">
         <v>12</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="H14" s="2" t="b">
         <v>0</v>
@@ -12799,26 +12805,26 @@
     </row>
     <row r="15" spans="1:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
+        <v>874</v>
+      </c>
+      <c r="B15" s="18" t="s">
         <v>875</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>876</v>
       </c>
       <c r="C15" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>swim in lava for 5 minutes Without dying (fire protection on everything)</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F15" s="2">
         <v>13</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="H15" s="2" t="b">
         <v>0</v>
@@ -12832,26 +12838,26 @@
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
+        <v>877</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>878</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>879</v>
       </c>
       <c r="C16" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Dye a sheep red</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F16" s="2">
         <v>14</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="H16" s="2" t="b">
         <v>0</v>
@@ -12865,26 +12871,26 @@
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
+        <v>880</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>881</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>882</v>
       </c>
       <c r="C17" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Did you loose a bet tman?</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F17" s="2">
         <v>15</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="H17" s="2" t="b">
         <v>0</v>
@@ -12898,29 +12904,29 @@
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
+        <v>883</v>
+      </c>
+      <c r="B18" s="11" t="s">
         <v>884</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>885</v>
       </c>
       <c r="C18" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Summon a Wither</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F18" s="2">
         <v>16</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="H18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18" s="2" t="b">
         <v>0</v>
@@ -12931,26 +12937,26 @@
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
+        <v>886</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>887</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>888</v>
       </c>
       <c r="C19" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Place 1,000,000 gravel</v>
       </c>
       <c r="D19" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F19" s="2">
         <v>17</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="H19" s="2" t="b">
         <v>0</v>
@@ -12964,29 +12970,29 @@
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
+        <v>889</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>890</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>891</v>
       </c>
       <c r="C20" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Kill a guardian with no diamond gear</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F20" s="2">
         <v>18</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="H20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="2" t="b">
         <v>0</v>
@@ -12997,26 +13003,26 @@
     </row>
     <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
+        <v>892</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>893</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>894</v>
       </c>
       <c r="C21" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Name tag an armorstand</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F21" s="2">
         <v>19</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H21" s="2" t="b">
         <v>0</v>
@@ -13030,29 +13036,29 @@
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
+        <v>894</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>895</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>896</v>
       </c>
       <c r="C22" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Kill a wither with no beacon effects and no diamond gear</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F22" s="2">
         <v>20</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="H22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22" s="2" t="b">
         <v>0</v>
@@ -13063,26 +13069,26 @@
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
+        <v>897</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>898</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>899</v>
       </c>
       <c r="C23" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Be killed by friendly fire while you have the wither effect</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F23" s="2">
         <v>21</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="H23" s="2" t="b">
         <v>0</v>
@@ -13096,26 +13102,26 @@
     </row>
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
+        <v>899</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>900</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>901</v>
       </c>
       <c r="C24" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Kill a player when that player has the wither effect</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F24" s="2">
         <v>22</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="H24" s="2" t="b">
         <v>0</v>
@@ -13129,26 +13135,26 @@
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>904</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>905</v>
       </c>
       <c r="C25" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Killed by a player when you have no gear on</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F25" s="2">
         <v>23</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="H25" s="2" t="b">
         <v>0</v>
@@ -13162,26 +13168,26 @@
     </row>
     <row r="26" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
+        <v>906</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>907</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>908</v>
       </c>
       <c r="C26" s="12" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>have dark oak log, dark oak saplings and a furnace in your inventory</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F26" s="2">
         <v>24</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="H26" s="2" t="b">
         <v>0</v>
@@ -13195,26 +13201,26 @@
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
+        <v>908</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>909</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>910</v>
       </c>
       <c r="C27" s="12" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>destroy a shulker with fire</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F27" s="2">
         <v>25</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="H27" s="2" t="b">
         <v>0</v>
@@ -13228,26 +13234,26 @@
     </row>
     <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
+        <v>910</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>911</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>912</v>
       </c>
       <c r="C28" s="12" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>have a shulker that is dyed black</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F28" s="2">
         <v>26</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="H28" s="2" t="b">
         <v>0</v>
@@ -13261,25 +13267,25 @@
     </row>
     <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
+        <v>912</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>913</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>914</v>
-      </c>
       <c r="C29" s="12" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F29" s="2">
         <v>27</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="H29" s="2" t="b">
         <v>0</v>
@@ -13293,26 +13299,26 @@
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
+        <v>914</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>915</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>916</v>
       </c>
       <c r="C30" s="12" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Obtain 164 gold blocks</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F30" s="2">
         <v>28</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="H30" s="2" t="b">
         <v>0</v>
@@ -13326,26 +13332,26 @@
     </row>
     <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
+        <v>916</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>917</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>918</v>
       </c>
       <c r="C31" s="12" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Send a dolphin to the nether</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F31" s="2">
         <v>29</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="H31" s="2" t="b">
         <v>0</v>
@@ -13359,25 +13365,25 @@
     </row>
     <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
+        <v>918</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>919</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="C32" s="12" t="s">
         <v>920</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>921</v>
-      </c>
       <c r="D32" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F32" s="2">
         <v>30</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="H32" s="2" t="b">
         <v>0</v>
@@ -13391,25 +13397,25 @@
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
+        <v>921</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>922</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>923</v>
-      </c>
       <c r="C33" s="20" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D33" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F33" s="2">
         <v>31</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="H33" s="2" t="b">
         <v>0</v>
@@ -13423,25 +13429,25 @@
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>843</v>
       </c>
       <c r="F34" s="2">
         <v>32</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="H34" s="2" t="b">
         <v>0</v>
@@ -13455,26 +13461,26 @@
     </row>
     <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
+        <v>924</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>925</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>926</v>
       </c>
       <c r="C35" s="12" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Craft 64 crafting tables</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F35" s="2">
         <v>1</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="H35" s="2" t="b">
         <v>0</v>
@@ -13488,26 +13494,26 @@
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
+        <v>926</v>
+      </c>
+      <c r="B36" s="11" t="s">
         <v>927</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>928</v>
       </c>
       <c r="C36" s="12" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Burn 64 dark oak logs</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F36" s="2">
         <v>2</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H36" s="2" t="b">
         <v>0</v>
@@ -13521,23 +13527,23 @@
     </row>
     <row r="37" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="12" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F37" s="2">
         <v>3</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="H37" s="2" t="b">
         <v>0</v>
@@ -13551,26 +13557,26 @@
     </row>
     <row r="38" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
+        <v>930</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>931</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>932</v>
       </c>
       <c r="C38" s="12" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Have 164 netherite blocks and a beacon in your inventory</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F38" s="2">
         <v>4</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="H38" s="2" t="b">
         <v>0</v>
@@ -13584,25 +13590,25 @@
     </row>
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
+        <v>932</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>933</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="C39" s="12" t="s">
         <v>934</v>
       </c>
-      <c r="C39" s="12" t="s">
-        <v>935</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F39" s="2">
         <v>5</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="H39" s="2" t="b">
         <v>0</v>
@@ -13616,26 +13622,26 @@
     </row>
     <row r="40" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="C40" s="12" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Name a cow super cow.</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F40" s="2">
         <v>6</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="H40" s="2" t="b">
         <v>0</v>
@@ -13649,23 +13655,23 @@
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="12" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F41" s="2">
         <v>7</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="H41" s="2" t="b">
         <v>0</v>
@@ -13679,26 +13685,26 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="C42" s="13" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Punch a zombie piglin or a piglin with an empty hand.</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F42" s="2">
         <v>8</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="H42" s="2" t="b">
         <v>0</v>
@@ -13712,26 +13718,26 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C43" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Eat a beetroot</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>973</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>974</v>
-      </c>
       <c r="F43" s="2">
         <v>1</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="H43" s="2" t="b">
         <v>0</v>
@@ -13745,26 +13751,26 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C44" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Wear a Turtle Shell</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F44" s="2">
         <v>2</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="H44" s="2" t="b">
         <v>0</v>
@@ -13778,26 +13784,26 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>1013</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>1014</v>
       </c>
       <c r="C45" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Suffocate in sand</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F45" s="2">
         <v>3</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="H45" s="2" t="b">
         <v>0</v>
@@ -13811,26 +13817,26 @@
     </row>
     <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>962</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>963</v>
       </c>
       <c r="C46" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Visit a cherry grove during Sakura Season (day 74 to 105, annually)</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F46" s="2">
         <v>4</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="H46" s="2" t="b">
         <v>0</v>
@@ -13844,26 +13850,26 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C47" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Wear a leather helmet</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F47" s="2">
         <v>5</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="H47" s="2" t="b">
         <v>0</v>
@@ -13877,26 +13883,26 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="C48" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Look at an Enderman</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F48" s="2">
         <v>6</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="H48" s="2" t="b">
         <v>0</v>
@@ -13910,26 +13916,26 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>968</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>969</v>
       </c>
       <c r="C49" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Wear a Jack o'Lantern on your head</v>
       </c>
       <c r="D49" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F49" s="2">
         <v>7</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="H49" s="2" t="b">
         <v>0</v>
@@ -13943,26 +13949,26 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C50" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Eat glow berries</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F50" s="2">
         <v>8</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="H50" s="2" t="b">
         <v>0</v>
@@ -13976,26 +13982,26 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C51" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Drink a Potion of Healing</v>
       </c>
       <c r="D51" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F51" s="2">
         <v>9</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="H51" s="2" t="b">
         <v>0</v>
@@ -14009,26 +14015,26 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="C52" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Get killed by an Elder Guardian</v>
       </c>
       <c r="D52" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F52" s="2">
         <v>10</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="H52" s="2" t="b">
         <v>0</v>
@@ -14042,26 +14048,26 @@
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>979</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>980</v>
       </c>
       <c r="C53" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Get killed by a Silverfish</v>
       </c>
       <c r="D53" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F53" s="2">
         <v>11</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="H53" s="2" t="b">
         <v>0</v>
@@ -14075,26 +14081,26 @@
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>981</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>982</v>
       </c>
       <c r="C54" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Kill a baby sheep</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F54" s="2">
         <v>12</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="H54" s="2" t="b">
         <v>0</v>
@@ -14108,26 +14114,26 @@
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B55" s="4" t="s">
         <v>984</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>985</v>
       </c>
       <c r="C55" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Teleport to the Nether with another entity</v>
       </c>
       <c r="D55" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F55" s="2">
         <v>13</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="H55" s="2" t="b">
         <v>0</v>
@@ -14141,26 +14147,26 @@
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C56" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Get killed by a Drowned</v>
       </c>
       <c r="D56" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F56" s="2">
         <v>14</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="H56" s="2" t="b">
         <v>0</v>
@@ -14174,26 +14180,26 @@
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>988</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>989</v>
       </c>
       <c r="C57" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Kill a skeleton</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F57" s="2">
         <v>15</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="H57" s="2" t="b">
         <v>0</v>
@@ -14207,26 +14213,26 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C58" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Kill a Stray</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F58" s="2">
         <v>16</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="H58" s="2" t="b">
         <v>0</v>
@@ -14240,26 +14246,26 @@
     </row>
     <row r="59" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C59" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Breed mobs between 00:00 and 01:00 (day tick 18,000 to 19,000)</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F59" s="2">
         <v>17</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="H59" s="2" t="b">
         <v>0</v>
@@ -14273,26 +14279,26 @@
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>996</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>997</v>
       </c>
       <c r="C60" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Get killed by a Creeper</v>
       </c>
       <c r="D60" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F60" s="2">
         <v>18</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="H60" s="2" t="b">
         <v>0</v>
@@ -14306,26 +14312,26 @@
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C61" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Place a crimson door</v>
       </c>
       <c r="D61" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F61" s="2">
         <v>19</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="H61" s="2" t="b">
         <v>0</v>
@@ -14339,26 +14345,26 @@
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C62" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Get hit by a Ravager</v>
       </c>
       <c r="D62" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F62" s="2">
         <v>20</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="H62" s="2" t="b">
         <v>0</v>
@@ -14372,26 +14378,26 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>1017</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>1018</v>
       </c>
       <c r="C63" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Get killed by a Phantom</v>
       </c>
       <c r="D63" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F63" s="2">
         <v>21</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="H63" s="2" t="b">
         <v>0</v>
@@ -14405,26 +14411,26 @@
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="C64" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Kill another player while your health is full</v>
       </c>
       <c r="D64" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F64" s="2">
         <v>22</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="H64" s="2" t="b">
         <v>0</v>
@@ -14438,26 +14444,26 @@
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="C65" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Place an Ender Chest</v>
       </c>
       <c r="D65" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F65" s="2">
         <v>23</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="H65" s="2" t="b">
         <v>0</v>
@@ -14471,26 +14477,26 @@
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>1028</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>1029</v>
       </c>
       <c r="C66" s="1" t="str">
         <f>Table3[[#This Row],[In-game description]]</f>
         <v>Look at a Zombie through a spyglass</v>
       </c>
       <c r="D66" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>973</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>974</v>
       </c>
       <c r="F66" s="2">
         <v>24</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="H66" s="2" t="b">
         <v>0</v>
@@ -14805,46 +14811,46 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="E22:F22 H22:J22 E67:J1048576 E43:G66">
-    <cfRule type="expression" dxfId="23" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>AND($A22&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="6">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>AND($A22&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24:F24 H24:J24 E25:J25 E26:E42 H26:I66 J66 J27:J28 J30:J31 J33:J34 J36:J37 J39:J40 J42:J43 J45:J46 J48:J49 J51:J52 J54:J55 J57:J58 J60:J61 J63:J64">
-    <cfRule type="expression" dxfId="20" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>AND($A24&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="9">
+    <cfRule type="expression" dxfId="6" priority="9">
       <formula>AND($A24&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:J15 E16:G16 H16:J20 E17:F20 E21:J21 G26:G39 F40:G42">
-    <cfRule type="expression" dxfId="17" priority="10">
+    <cfRule type="expression" dxfId="5" priority="10">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="11">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="12">
+    <cfRule type="expression" dxfId="3" priority="12">
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:J23 F26:F39 J26 J29 J32 J35 J38 J41 J44 J47 J50 J53 J56 J59 J62 J65">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>ROW()=2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND($A23&lt;&gt;"",MOD(ROW(),2)=1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>AND($A23&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14863,10 +14869,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03723C66-8E0B-48F3-9CF4-1B0F8B736B8C}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14939,33 +14945,58 @@
         <v>110</v>
       </c>
       <c r="F3" s="9">
-        <f t="shared" ref="F3:F4" si="0">B3/E3</f>
+        <f t="shared" ref="F3:F5" si="0">B3/E3</f>
         <v>0.61818181818181817</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>840</v>
+        <v>1034</v>
       </c>
       <c r="B4">
-        <f>B3+B2</f>
-        <v>133</v>
+        <f>COUNTIF(Table3[Implement],"=TRUE")</f>
+        <v>8</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:E4" si="1">C3+C2</f>
+        <f>COUNTIF(Table3[Player.json],"=TRUE")</f>
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
-        <v>102</v>
+        <f>COUNTIF(Table3[Implement],"=FALSE")</f>
+        <v>56</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
-        <v>235</v>
+        <f>ROWS(Table3[Implement])</f>
+        <v>64</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" si="0"/>
-        <v>0.56595744680851068</v>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B5">
+        <f>B3+B2+B4</f>
+        <v>141</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:D5" si="1">C3+C2+C4</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>158</v>
+      </c>
+      <c r="E5">
+        <f>E3+E2+E4</f>
+        <v>299</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" si="0"/>
+        <v>0.47157190635451507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added advancement "The power of books"
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBFC6B8-87FE-4693-B6F6-C1AD53E99FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415F7453-40B4-454F-97BE-A9AA1B5671CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="1" r:id="rId1"/>
@@ -8716,7 +8716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N112"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -8749,7 +8749,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="8" t="str">
         <f>CONCATENATE("Complete: ",COUNTIF(Table2[Implement],"=TRUE"),"/",ROWS(Table2[Implement]))</f>
-        <v>Complete: 68/110</v>
+        <v>Complete: 69/110</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -10508,7 +10508,7 @@
         <v>639</v>
       </c>
       <c r="H56" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" s="2" t="b">
         <v>0</v>
@@ -12337,8 +12337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A114CABE-4723-471F-81B1-1F98BAE7D3E1}">
   <dimension ref="A1:N126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14930,7 +14930,7 @@
       </c>
       <c r="B3">
         <f>COUNTIF(Table2[Implement],"=TRUE")</f>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C3">
         <f>COUNTIF(Table2[Player.json],"=TRUE")</f>
@@ -14938,7 +14938,7 @@
       </c>
       <c r="D3">
         <f>COUNTIF(Table2[Implement],"=FALSE")</f>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3">
         <f>ROWS(Table2[Implement])</f>
@@ -14946,7 +14946,7 @@
       </c>
       <c r="F3" s="9">
         <f t="shared" ref="F3:F5" si="0">B3/E3</f>
-        <v>0.61818181818181817</v>
+        <v>0.62727272727272732</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -14980,7 +14980,7 @@
       </c>
       <c r="B5">
         <f>B3+B2+B4</f>
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:D5" si="1">C3+C2+C4</f>
@@ -14988,7 +14988,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E5">
         <f>E3+E2+E4</f>
@@ -14996,7 +14996,7 @@
       </c>
       <c r="F5" s="9">
         <f t="shared" si="0"/>
-        <v>0.55852842809364545</v>
+        <v>0.56187290969899661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added "We're being attacked" achievement
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F6C25AC-8A25-45B2-80E6-C55262940593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0A31DD-4998-4AEA-AB46-D391E3DF1628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4137,7 +4137,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="8" t="str">
         <f>CONCATENATE("Complete: ",COUNTIF(Table1[Implement],"=TRUE"),"/",ROWS(Table1[Implement]))</f>
-        <v>Complete: 67/125</v>
+        <v>Complete: 68/125</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -4178,7 +4178,7 @@
       </c>
       <c r="M2" s="1">
         <f>COUNTIF(Table1[Implement],"=TRUE")</f>
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
@@ -4218,7 +4218,7 @@
       </c>
       <c r="M3" s="1">
         <f>COUNTIF(Table1[Implement],"=FALSE")</f>
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
@@ -7772,7 +7772,7 @@
         <v>371</v>
       </c>
       <c r="H102" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I102" s="2" t="b">
         <v>0</v>
@@ -14905,7 +14905,7 @@
       </c>
       <c r="B2">
         <f>COUNTIF(Table1[Implement],"=TRUE")</f>
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C2">
         <f>COUNTIF(Table1[Player.json],"=TRUE")</f>
@@ -14913,7 +14913,7 @@
       </c>
       <c r="D2">
         <f>COUNTIF(Table1[Implement],"=FALSE")</f>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2">
         <f>ROWS(Table1[Implement])</f>
@@ -14921,7 +14921,7 @@
       </c>
       <c r="F2" s="9">
         <f>B2/E2</f>
-        <v>0.53600000000000003</v>
+        <v>0.54400000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -14980,7 +14980,7 @@
       </c>
       <c r="B5">
         <f>B3+B2+B4</f>
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:D5" si="1">C3+C2+C4</f>
@@ -14988,7 +14988,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E5">
         <f>E3+E2+E4</f>
@@ -14996,7 +14996,7 @@
       </c>
       <c r="F5" s="9">
         <f t="shared" si="0"/>
-        <v>0.56856187290969895</v>
+        <v>0.57190635451505012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added sea pickle achievement
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0A31DD-4998-4AEA-AB46-D391E3DF1628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98034291-3039-4630-BF37-17BBAB06F06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4137,7 +4137,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="8" t="str">
         <f>CONCATENATE("Complete: ",COUNTIF(Table1[Implement],"=TRUE"),"/",ROWS(Table1[Implement]))</f>
-        <v>Complete: 68/125</v>
+        <v>Complete: 69/125</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -4178,7 +4178,7 @@
       </c>
       <c r="M2" s="1">
         <f>COUNTIF(Table1[Implement],"=TRUE")</f>
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
@@ -4218,7 +4218,7 @@
       </c>
       <c r="M3" s="1">
         <f>COUNTIF(Table1[Implement],"=FALSE")</f>
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
@@ -7376,7 +7376,7 @@
         <v>333</v>
       </c>
       <c r="H91" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I91" s="2" t="b">
         <v>0</v>
@@ -14905,7 +14905,7 @@
       </c>
       <c r="B2">
         <f>COUNTIF(Table1[Implement],"=TRUE")</f>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <f>COUNTIF(Table1[Player.json],"=TRUE")</f>
@@ -14913,7 +14913,7 @@
       </c>
       <c r="D2">
         <f>COUNTIF(Table1[Implement],"=FALSE")</f>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2">
         <f>ROWS(Table1[Implement])</f>
@@ -14921,7 +14921,7 @@
       </c>
       <c r="F2" s="9">
         <f>B2/E2</f>
-        <v>0.54400000000000004</v>
+        <v>0.55200000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -14980,7 +14980,7 @@
       </c>
       <c r="B5">
         <f>B3+B2+B4</f>
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:D5" si="1">C3+C2+C4</f>
@@ -14988,7 +14988,7 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E5">
         <f>E3+E2+E4</f>
@@ -14996,7 +14996,7 @@
       </c>
       <c r="F5" s="9">
         <f t="shared" si="0"/>
-        <v>0.57190635451505012</v>
+        <v>0.57525083612040129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated to remove non-functional achievements
</commit_message>
<xml_diff>
--- a/lookupData/en.xlsx
+++ b/lookupData/en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\GitHub\BedrockStatsTracker\lookupData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EAA2F3-6CA7-4E73-84FB-24EEA0796208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E12532-F44D-4EA3-9A4F-82518CA81EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Achievements" sheetId="1" r:id="rId1"/>
@@ -4005,9 +4005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M127"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4035,7 +4033,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="8" t="str">
         <f>CONCATENATE("Complete: ",COUNTIF(Table1[Implement],"=TRUE"),"/",ROWS(Table1[Implement]))</f>
-        <v>Complete: 70/125</v>
+        <v>Complete: 67/125</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -4076,7 +4074,7 @@
       </c>
       <c r="M2" s="1">
         <f>COUNTIF(Table1[Implement],"=TRUE")</f>
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -4116,7 +4114,7 @@
       </c>
       <c r="M3" s="1">
         <f>COUNTIF(Table1[Implement],"=FALSE")</f>
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -7274,7 +7272,7 @@
         <v>336</v>
       </c>
       <c r="H91" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I91" s="2" t="b">
         <v>0</v>
@@ -7382,7 +7380,7 @@
         <v>346</v>
       </c>
       <c r="H94" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I94" s="2" t="b">
         <v>0</v>
@@ -7670,7 +7668,7 @@
         <v>373</v>
       </c>
       <c r="H102" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I102" s="2" t="b">
         <v>0</v>
@@ -8598,7 +8596,7 @@
   <conditionalFormatting sqref="K1:K1048576">
     <cfRule type="duplicateValues" dxfId="52" priority="2"/>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I127" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
@@ -8614,8 +8612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="C81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="50.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8647,7 +8645,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="8" t="str">
         <f>CONCATENATE("Complete: ",COUNTIF(Table2[Implement],"=TRUE"),"/",ROWS(Table2[Implement]))</f>
-        <v>Complete: 67/110</v>
+        <v>Complete: 65/110</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -10406,7 +10404,7 @@
         <v>641</v>
       </c>
       <c r="H56" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" s="2" t="b">
         <v>0</v>
@@ -11270,7 +11268,7 @@
         <v>729</v>
       </c>
       <c r="H83" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83" s="2" t="b">
         <v>0</v>
@@ -12219,7 +12217,7 @@
       <formula>AND($A1&lt;&gt;"",MOD(ROW(),2)=0)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3:I112" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
@@ -12236,7 +12234,7 @@
   <dimension ref="A1:N126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14802,7 +14800,7 @@
       </c>
       <c r="B2">
         <f>COUNTIF(Table1[Implement],"=TRUE")</f>
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C2">
         <f>COUNTIF(Table1[Player.json],"=TRUE")</f>
@@ -14810,7 +14808,7 @@
       </c>
       <c r="D2">
         <f>COUNTIF(Table1[Implement],"=FALSE")</f>
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E2">
         <f>ROWS(Table1[Implement])</f>
@@ -14818,7 +14816,7 @@
       </c>
       <c r="F2" s="9">
         <f>B2/E2</f>
-        <v>0.56000000000000005</v>
+        <v>0.53600000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -14827,7 +14825,7 @@
       </c>
       <c r="B3">
         <f>COUNTIF(Table2[Implement],"=TRUE")</f>
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3">
         <f>COUNTIF(Table2[Player.json],"=TRUE")</f>
@@ -14835,7 +14833,7 @@
       </c>
       <c r="D3">
         <f>COUNTIF(Table2[Implement],"=FALSE")</f>
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E3">
         <f>ROWS(Table2[Implement])</f>
@@ -14843,7 +14841,7 @@
       </c>
       <c r="F3" s="9">
         <f>B3/E3</f>
-        <v>0.60909090909090913</v>
+        <v>0.59090909090909094</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -14877,7 +14875,7 @@
       </c>
       <c r="B5">
         <f>B3+B2+B4</f>
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C5">
         <f>C3+C2+C4</f>
@@ -14885,7 +14883,7 @@
       </c>
       <c r="D5">
         <f>D3+D2+D4</f>
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="E5">
         <f>E3+E2+E4</f>
@@ -14893,7 +14891,7 @@
       </c>
       <c r="F5" s="9">
         <f>B5/E5</f>
-        <v>0.59197324414715724</v>
+        <v>0.57525083612040129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>